<commit_message>
pass document name to lomake
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19220" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2752" uniqueCount="1939">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2754" uniqueCount="1940">
   <si>
     <t>fi</t>
   </si>
@@ -5838,6 +5838,9 @@
   </si>
   <si>
     <t>kutsu</t>
+  </si>
+  <si>
+    <t>userinfo.role</t>
   </si>
 </sst>
 </file>
@@ -5998,7 +6001,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -6016,6 +6019,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="75">
     <cellStyle name="Avattu hyperlinkki" xfId="2" builtinId="9" hidden="1"/>
@@ -6094,7 +6098,17 @@
     <cellStyle name="Hyperlinkki" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -6662,16 +6676,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C370"/>
+  <dimension ref="A1:C371"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A28" sqref="A11:A28"/>
+    <sheetView tabSelected="1" topLeftCell="A257" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C276" sqref="C276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="100.83203125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="50.83203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="50.83203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15">
@@ -6681,7 +6696,7 @@
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -6708,7 +6723,7 @@
       <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" t="s">
         <v>1918</v>
       </c>
     </row>
@@ -6727,7 +6742,7 @@
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" t="s">
         <v>1919</v>
       </c>
     </row>
@@ -7114,7 +7129,7 @@
       <c r="B54" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" t="s">
         <v>187</v>
       </c>
     </row>
@@ -7125,7 +7140,7 @@
       <c r="B55" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" t="s">
         <v>189</v>
       </c>
     </row>
@@ -7160,7 +7175,7 @@
       <c r="B59" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" t="s">
         <v>1920</v>
       </c>
     </row>
@@ -7187,7 +7202,7 @@
       <c r="B62" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" t="s">
         <v>1927</v>
       </c>
     </row>
@@ -7198,7 +7213,7 @@
       <c r="B63" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" t="s">
         <v>1928</v>
       </c>
     </row>
@@ -7241,7 +7256,7 @@
       <c r="B68" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" t="s">
         <v>1929</v>
       </c>
     </row>
@@ -7252,7 +7267,7 @@
       <c r="B69" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" t="s">
         <v>1930</v>
       </c>
     </row>
@@ -7263,7 +7278,7 @@
       <c r="B70" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" t="s">
         <v>1931</v>
       </c>
     </row>
@@ -7458,7 +7473,7 @@
       <c r="B94" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="C94" s="5" t="s">
+      <c r="C94" t="s">
         <v>267</v>
       </c>
     </row>
@@ -7469,7 +7484,7 @@
       <c r="B95" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="C95" t="s">
         <v>1921</v>
       </c>
     </row>
@@ -8080,7 +8095,7 @@
       <c r="B171" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="C171" s="5" t="s">
+      <c r="C171" t="s">
         <v>419</v>
       </c>
     </row>
@@ -8243,7 +8258,7 @@
       <c r="B191" s="5" t="s">
         <v>491</v>
       </c>
-      <c r="C191" s="5" t="s">
+      <c r="C191" t="s">
         <v>491</v>
       </c>
     </row>
@@ -8558,7 +8573,7 @@
       <c r="B230" s="5" t="s">
         <v>597</v>
       </c>
-      <c r="C230" s="5" t="s">
+      <c r="C230" t="s">
         <v>597</v>
       </c>
     </row>
@@ -8585,7 +8600,7 @@
       <c r="B233" s="5" t="s">
         <v>602</v>
       </c>
-      <c r="C233" s="5" t="s">
+      <c r="C233" t="s">
         <v>602</v>
       </c>
     </row>
@@ -8612,7 +8627,7 @@
       <c r="B236" s="5" t="s">
         <v>650</v>
       </c>
-      <c r="C236" s="5" t="s">
+      <c r="C236" t="s">
         <v>650</v>
       </c>
     </row>
@@ -8775,7 +8790,7 @@
       <c r="B256" s="5" t="s">
         <v>680</v>
       </c>
-      <c r="C256" s="5" t="s">
+      <c r="C256" t="s">
         <v>680</v>
       </c>
     </row>
@@ -8794,7 +8809,7 @@
       <c r="B258" s="5" t="s">
         <v>1130</v>
       </c>
-      <c r="C258" s="5" t="s">
+      <c r="C258" t="s">
         <v>1922</v>
       </c>
     </row>
@@ -8936,798 +8951,806 @@
     </row>
     <row r="276" spans="1:3">
       <c r="A276" s="1" t="s">
-        <v>1432</v>
+        <v>1939</v>
       </c>
       <c r="B276" s="5" t="s">
-        <v>658</v>
-      </c>
-      <c r="C276" s="5" t="s">
-        <v>1923</v>
+        <v>177</v>
       </c>
     </row>
     <row r="277" spans="1:3">
       <c r="A277" s="1" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="B277" s="5" t="s">
-        <v>1434</v>
+        <v>658</v>
+      </c>
+      <c r="C277" t="s">
+        <v>1923</v>
       </c>
     </row>
     <row r="278" spans="1:3">
       <c r="A278" s="1" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="B278" s="5" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="279" spans="1:3">
       <c r="A279" s="1" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="B279" s="5" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="280" spans="1:3">
       <c r="A280" s="1" t="s">
-        <v>1439</v>
-      </c>
-      <c r="B280" s="6" t="s">
-        <v>1917</v>
-      </c>
-      <c r="C280" s="6" t="s">
-        <v>1917</v>
+        <v>1437</v>
+      </c>
+      <c r="B280" s="5" t="s">
+        <v>1438</v>
       </c>
     </row>
     <row r="281" spans="1:3">
       <c r="A281" s="1" t="s">
-        <v>1440</v>
-      </c>
-      <c r="B281" s="5" t="s">
-        <v>1441</v>
+        <v>1439</v>
+      </c>
+      <c r="B281" s="6" t="s">
+        <v>1917</v>
+      </c>
+      <c r="C281" s="7" t="s">
+        <v>1917</v>
       </c>
     </row>
     <row r="282" spans="1:3">
       <c r="A282" s="1" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="B282" s="5" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" s="1" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="B283" s="5" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="284" spans="1:3">
       <c r="A284" s="1" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="285" spans="1:3">
       <c r="A285" s="1" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="286" spans="1:3">
       <c r="A286" s="1" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="B286" s="5" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="287" spans="1:3">
       <c r="A287" s="1" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="B287" s="5" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="288" spans="1:3">
       <c r="A288" s="1" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="B288" s="5" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="289" spans="1:3">
       <c r="A289" s="1" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="B289" s="5" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="290" spans="1:3">
       <c r="A290" s="1" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="B290" s="5" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="291" spans="1:3">
       <c r="A291" s="1" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="B291" s="5" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="292" spans="1:3">
       <c r="A292" s="1" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="B292" s="5" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="293" spans="1:3">
       <c r="A293" s="1" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="B293" s="5" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="294" spans="1:3">
       <c r="A294" s="1" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="B294" s="5" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="295" spans="1:3">
       <c r="A295" s="1" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="B295" s="5" t="s">
-        <v>1469</v>
-      </c>
-      <c r="C295" s="5" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="296" spans="1:3">
       <c r="A296" s="1" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="B296" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="C296" s="5" t="s">
-        <v>419</v>
+        <v>1469</v>
+      </c>
+      <c r="C296" t="s">
+        <v>1469</v>
       </c>
     </row>
     <row r="297" spans="1:3">
       <c r="A297" s="1" t="s">
-        <v>1505</v>
+        <v>1470</v>
       </c>
       <c r="B297" s="5" t="s">
-        <v>1506</v>
+        <v>419</v>
+      </c>
+      <c r="C297" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="298" spans="1:3">
       <c r="A298" s="1" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
       <c r="B298" s="5" t="s">
-        <v>1436</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="299" spans="1:3">
       <c r="A299" s="1" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="B299" s="5" t="s">
-        <v>1509</v>
-      </c>
-      <c r="C299" s="5" t="s">
-        <v>1924</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="300" spans="1:3">
       <c r="A300" s="1" t="s">
-        <v>1781</v>
+        <v>1508</v>
       </c>
       <c r="B300" s="5" t="s">
-        <v>37</v>
+        <v>1509</v>
+      </c>
+      <c r="C300" t="s">
+        <v>1924</v>
       </c>
     </row>
     <row r="301" spans="1:3">
       <c r="A301" s="1" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="B301" s="5" t="s">
-        <v>1783</v>
+        <v>37</v>
       </c>
     </row>
     <row r="302" spans="1:3">
       <c r="A302" s="1" t="s">
-        <v>1784</v>
+        <v>1782</v>
       </c>
       <c r="B302" s="5" t="s">
-        <v>1785</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="303" spans="1:3">
       <c r="A303" s="1" t="s">
-        <v>1786</v>
+        <v>1784</v>
       </c>
       <c r="B303" s="5" t="s">
-        <v>1787</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="304" spans="1:3">
       <c r="A304" s="1" t="s">
-        <v>1788</v>
+        <v>1786</v>
       </c>
       <c r="B304" s="5" t="s">
-        <v>1789</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="305" spans="1:2">
       <c r="A305" s="1" t="s">
-        <v>1790</v>
+        <v>1788</v>
       </c>
       <c r="B305" s="5" t="s">
-        <v>1791</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="306" spans="1:2">
       <c r="A306" s="1" t="s">
-        <v>1792</v>
+        <v>1790</v>
       </c>
       <c r="B306" s="5" t="s">
-        <v>1793</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="307" spans="1:2">
       <c r="A307" s="1" t="s">
-        <v>1794</v>
+        <v>1792</v>
       </c>
       <c r="B307" s="5" t="s">
-        <v>1795</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="308" spans="1:2">
       <c r="A308" s="1" t="s">
-        <v>1796</v>
+        <v>1794</v>
       </c>
       <c r="B308" s="5" t="s">
-        <v>1797</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="309" spans="1:2">
       <c r="A309" s="1" t="s">
-        <v>1798</v>
+        <v>1796</v>
       </c>
       <c r="B309" s="5" t="s">
-        <v>1799</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="310" spans="1:2">
       <c r="A310" s="1" t="s">
-        <v>1800</v>
+        <v>1798</v>
       </c>
       <c r="B310" s="5" t="s">
-        <v>1801</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="311" spans="1:2">
       <c r="A311" s="1" t="s">
-        <v>1802</v>
+        <v>1800</v>
       </c>
       <c r="B311" s="5" t="s">
-        <v>1803</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="312" spans="1:2">
       <c r="A312" s="1" t="s">
-        <v>1804</v>
+        <v>1802</v>
       </c>
       <c r="B312" s="5" t="s">
-        <v>1805</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="313" spans="1:2">
       <c r="A313" s="1" t="s">
-        <v>1806</v>
+        <v>1804</v>
       </c>
       <c r="B313" s="5" t="s">
-        <v>1807</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="314" spans="1:2">
       <c r="A314" s="1" t="s">
-        <v>1808</v>
+        <v>1806</v>
       </c>
       <c r="B314" s="5" t="s">
-        <v>1809</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="315" spans="1:2">
       <c r="A315" s="1" t="s">
-        <v>1810</v>
+        <v>1808</v>
       </c>
       <c r="B315" s="5" t="s">
-        <v>1811</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="316" spans="1:2">
       <c r="A316" s="1" t="s">
-        <v>1812</v>
+        <v>1810</v>
       </c>
       <c r="B316" s="5" t="s">
-        <v>562</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="317" spans="1:2">
       <c r="A317" s="1" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="B317" s="5" t="s">
-        <v>1814</v>
+        <v>562</v>
       </c>
     </row>
     <row r="318" spans="1:2">
       <c r="A318" s="1" t="s">
-        <v>1815</v>
+        <v>1813</v>
       </c>
       <c r="B318" s="5" t="s">
-        <v>1816</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="319" spans="1:2">
       <c r="A319" s="1" t="s">
-        <v>1817</v>
+        <v>1815</v>
       </c>
       <c r="B319" s="5" t="s">
-        <v>1818</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="320" spans="1:2">
       <c r="A320" s="1" t="s">
-        <v>1819</v>
+        <v>1817</v>
       </c>
       <c r="B320" s="5" t="s">
-        <v>1820</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="321" spans="1:2">
       <c r="A321" s="1" t="s">
-        <v>1821</v>
+        <v>1819</v>
       </c>
       <c r="B321" s="5" t="s">
-        <v>1822</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="322" spans="1:2">
       <c r="A322" s="1" t="s">
-        <v>1823</v>
+        <v>1821</v>
       </c>
       <c r="B322" s="5" t="s">
-        <v>1824</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="323" spans="1:2">
       <c r="A323" s="1" t="s">
-        <v>1825</v>
+        <v>1823</v>
       </c>
       <c r="B323" s="5" t="s">
-        <v>1826</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="324" spans="1:2">
       <c r="A324" s="1" t="s">
-        <v>1827</v>
+        <v>1825</v>
       </c>
       <c r="B324" s="5" t="s">
-        <v>1828</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="325" spans="1:2">
       <c r="A325" s="1" t="s">
-        <v>1829</v>
+        <v>1827</v>
       </c>
       <c r="B325" s="5" t="s">
-        <v>1830</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="326" spans="1:2">
       <c r="A326" s="1" t="s">
-        <v>1831</v>
+        <v>1829</v>
       </c>
       <c r="B326" s="5" t="s">
-        <v>1832</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="327" spans="1:2">
       <c r="A327" s="1" t="s">
-        <v>1833</v>
+        <v>1831</v>
       </c>
       <c r="B327" s="5" t="s">
-        <v>1834</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="328" spans="1:2">
       <c r="A328" s="1" t="s">
-        <v>1835</v>
+        <v>1833</v>
       </c>
       <c r="B328" s="5" t="s">
-        <v>1836</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="329" spans="1:2">
       <c r="A329" s="1" t="s">
-        <v>1837</v>
+        <v>1835</v>
       </c>
       <c r="B329" s="5" t="s">
-        <v>1838</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="330" spans="1:2">
       <c r="A330" s="1" t="s">
-        <v>1839</v>
+        <v>1837</v>
       </c>
       <c r="B330" s="5" t="s">
-        <v>1840</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="331" spans="1:2">
       <c r="A331" s="1" t="s">
-        <v>1841</v>
+        <v>1839</v>
       </c>
       <c r="B331" s="5" t="s">
-        <v>1842</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="332" spans="1:2">
       <c r="A332" s="1" t="s">
-        <v>1843</v>
+        <v>1841</v>
       </c>
       <c r="B332" s="5" t="s">
-        <v>1844</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="333" spans="1:2">
       <c r="A333" s="1" t="s">
-        <v>1845</v>
+        <v>1843</v>
       </c>
       <c r="B333" s="5" t="s">
-        <v>1846</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="334" spans="1:2">
       <c r="A334" s="1" t="s">
-        <v>1847</v>
+        <v>1845</v>
       </c>
       <c r="B334" s="5" t="s">
-        <v>1848</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="335" spans="1:2">
       <c r="A335" s="1" t="s">
-        <v>1849</v>
+        <v>1847</v>
       </c>
       <c r="B335" s="5" t="s">
-        <v>1850</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="336" spans="1:2">
       <c r="A336" s="1" t="s">
-        <v>1851</v>
+        <v>1849</v>
       </c>
       <c r="B336" s="5" t="s">
-        <v>1852</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="337" spans="1:2">
       <c r="A337" s="1" t="s">
-        <v>1853</v>
+        <v>1851</v>
       </c>
       <c r="B337" s="5" t="s">
-        <v>1854</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="338" spans="1:2">
       <c r="A338" s="1" t="s">
-        <v>1855</v>
+        <v>1853</v>
       </c>
       <c r="B338" s="5" t="s">
-        <v>1856</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="339" spans="1:2">
       <c r="A339" s="1" t="s">
-        <v>1857</v>
+        <v>1855</v>
       </c>
       <c r="B339" s="5" t="s">
-        <v>1858</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="340" spans="1:2">
       <c r="A340" s="1" t="s">
-        <v>1859</v>
+        <v>1857</v>
       </c>
       <c r="B340" s="5" t="s">
-        <v>1860</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="341" spans="1:2">
       <c r="A341" s="1" t="s">
-        <v>1861</v>
+        <v>1859</v>
       </c>
       <c r="B341" s="5" t="s">
-        <v>1862</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="342" spans="1:2">
       <c r="A342" s="1" t="s">
-        <v>1863</v>
+        <v>1861</v>
       </c>
       <c r="B342" s="5" t="s">
-        <v>1864</v>
+        <v>1862</v>
       </c>
     </row>
     <row r="343" spans="1:2">
       <c r="A343" s="1" t="s">
-        <v>1865</v>
+        <v>1863</v>
       </c>
       <c r="B343" s="5" t="s">
-        <v>1866</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="344" spans="1:2">
       <c r="A344" s="1" t="s">
-        <v>1867</v>
+        <v>1865</v>
       </c>
       <c r="B344" s="5" t="s">
-        <v>1868</v>
+        <v>1866</v>
       </c>
     </row>
     <row r="345" spans="1:2">
       <c r="A345" s="1" t="s">
-        <v>1869</v>
+        <v>1867</v>
       </c>
       <c r="B345" s="5" t="s">
-        <v>1870</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="346" spans="1:2">
       <c r="A346" s="1" t="s">
-        <v>1871</v>
+        <v>1869</v>
       </c>
       <c r="B346" s="5" t="s">
-        <v>1872</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="347" spans="1:2">
       <c r="A347" s="1" t="s">
-        <v>1873</v>
+        <v>1871</v>
       </c>
       <c r="B347" s="5" t="s">
-        <v>1874</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="348" spans="1:2">
       <c r="A348" s="1" t="s">
-        <v>1875</v>
+        <v>1873</v>
       </c>
       <c r="B348" s="5" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="349" spans="1:2">
       <c r="A349" s="1" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="B349" s="5" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="350" spans="1:2">
       <c r="A350" s="1" t="s">
-        <v>1879</v>
+        <v>1877</v>
       </c>
       <c r="B350" s="5" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="351" spans="1:2">
       <c r="A351" s="1" t="s">
-        <v>1881</v>
+        <v>1879</v>
       </c>
       <c r="B351" s="5" t="s">
-        <v>1882</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="352" spans="1:2">
       <c r="A352" s="1" t="s">
-        <v>1883</v>
+        <v>1881</v>
       </c>
       <c r="B352" s="5" t="s">
-        <v>1884</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="353" spans="1:3">
       <c r="A353" s="1" t="s">
-        <v>1885</v>
+        <v>1883</v>
       </c>
       <c r="B353" s="5" t="s">
-        <v>1886</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="354" spans="1:3">
       <c r="A354" s="1" t="s">
-        <v>1887</v>
+        <v>1885</v>
       </c>
       <c r="B354" s="5" t="s">
-        <v>1888</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="355" spans="1:3">
       <c r="A355" s="1" t="s">
-        <v>1889</v>
+        <v>1887</v>
       </c>
       <c r="B355" s="5" t="s">
-        <v>1890</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="356" spans="1:3">
       <c r="A356" s="1" t="s">
-        <v>1891</v>
+        <v>1889</v>
       </c>
       <c r="B356" s="5" t="s">
-        <v>1892</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="357" spans="1:3">
       <c r="A357" s="1" t="s">
-        <v>1893</v>
+        <v>1891</v>
       </c>
       <c r="B357" s="5" t="s">
-        <v>1894</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="358" spans="1:3">
       <c r="A358" s="1" t="s">
-        <v>1895</v>
+        <v>1893</v>
       </c>
       <c r="B358" s="5" t="s">
-        <v>1896</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="359" spans="1:3">
       <c r="A359" s="1" t="s">
-        <v>1897</v>
+        <v>1895</v>
       </c>
       <c r="B359" s="5" t="s">
-        <v>1898</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="360" spans="1:3">
       <c r="A360" s="1" t="s">
-        <v>1899</v>
+        <v>1897</v>
       </c>
       <c r="B360" s="5" t="s">
-        <v>1900</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="361" spans="1:3">
       <c r="A361" s="1" t="s">
-        <v>1901</v>
+        <v>1899</v>
       </c>
       <c r="B361" s="5" t="s">
-        <v>1902</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="362" spans="1:3">
       <c r="A362" s="1" t="s">
-        <v>1903</v>
+        <v>1901</v>
       </c>
       <c r="B362" s="5" t="s">
-        <v>1904</v>
-      </c>
-      <c r="C362" s="5" t="s">
-        <v>1904</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="363" spans="1:3">
       <c r="A363" s="1" t="s">
-        <v>1905</v>
+        <v>1903</v>
       </c>
       <c r="B363" s="5" t="s">
-        <v>45</v>
+        <v>1904</v>
+      </c>
+      <c r="C363" t="s">
+        <v>1904</v>
       </c>
     </row>
     <row r="364" spans="1:3">
       <c r="A364" s="1" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="B364" s="5" t="s">
-        <v>1702</v>
+        <v>45</v>
       </c>
     </row>
     <row r="365" spans="1:3">
       <c r="A365" s="1" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="B365" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C365" s="5" t="s">
-        <v>1928</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="366" spans="1:3">
       <c r="A366" s="1" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="B366" s="5" t="s">
-        <v>1909</v>
+        <v>205</v>
+      </c>
+      <c r="C366" t="s">
+        <v>1928</v>
       </c>
     </row>
     <row r="367" spans="1:3">
       <c r="A367" s="1" t="s">
-        <v>1910</v>
+        <v>1908</v>
       </c>
       <c r="B367" s="5" t="s">
-        <v>1911</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="368" spans="1:3">
       <c r="A368" s="1" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B368" s="5" t="s">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3">
+      <c r="A369" s="1" t="s">
         <v>1925</v>
       </c>
-      <c r="B368" s="5" t="s">
+      <c r="B369" s="5" t="s">
         <v>1926</v>
       </c>
-      <c r="C368" s="5" t="s">
+      <c r="C369" t="s">
         <v>1926</v>
       </c>
     </row>
-    <row r="369" spans="1:2">
-      <c r="A369" s="1" t="s">
+    <row r="370" spans="1:3">
+      <c r="A370" s="1" t="s">
         <v>1935</v>
       </c>
-      <c r="B369" s="5" t="s">
+      <c r="B370" s="5" t="s">
         <v>1932</v>
       </c>
     </row>
-    <row r="370" spans="1:2">
-      <c r="A370" s="1" t="s">
+    <row r="371" spans="1:3">
+      <c r="A371" s="1" t="s">
         <v>1933</v>
       </c>
-      <c r="B370" s="5" t="s">
+      <c r="B371" s="5" t="s">
         <v>1934</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <conditionalFormatting sqref="A1355:A1048576 A2:A368">
-    <cfRule type="expression" dxfId="23" priority="9">
+  <conditionalFormatting sqref="A2:A369 A1356:A1048576">
+    <cfRule type="expression" dxfId="24" priority="10">
       <formula>AND( $A2 = "", OR( $B2 &lt;&gt; "", $C2 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="expression" dxfId="22" priority="1">
-      <formula>AND($B1 &lt;&gt; "", $C1 = "")</formula>
+    <cfRule type="containsBlanks" dxfId="22" priority="1">
+      <formula>LEN(TRIM(C1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9744,7 +9767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A971" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B988" sqref="B988"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Localization for register views
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11544" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17688" windowHeight="6996" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" r:id="rId1"/>
@@ -9634,7 +9634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Email title and parameters
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4382" uniqueCount="2794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4388" uniqueCount="2799">
   <si>
     <t>fi</t>
   </si>
@@ -8428,6 +8428,21 @@
   </si>
   <si>
     <t>Inför</t>
+  </si>
+  <si>
+    <t>new-comment-email-title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Lupapiste] </t>
+  </si>
+  <si>
+    <t>Uusi kommentti</t>
+  </si>
+  <si>
+    <t>Ett nytt kommentt</t>
+  </si>
+  <si>
+    <t>email-title-prefix</t>
   </si>
 </sst>
 </file>
@@ -9464,10 +9479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C373"/>
+  <dimension ref="A1:C376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="A356" workbookViewId="0">
+      <selection activeCell="B374" sqref="B374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12498,7 +12513,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A369" s="1" t="s">
         <v>1932</v>
       </c>
@@ -12506,7 +12521,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A370" s="1" t="s">
         <v>1934</v>
       </c>
@@ -12514,7 +12529,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A371" s="1" t="s">
         <v>1935</v>
       </c>
@@ -12522,7 +12537,7 @@
         <v>1936</v>
       </c>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A372" s="1" t="s">
         <v>1937</v>
       </c>
@@ -12530,12 +12545,34 @@
         <v>521</v>
       </c>
     </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A373" s="1" t="s">
         <v>1938</v>
       </c>
       <c r="B373" s="5" t="s">
         <v>176</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A375" s="1" t="s">
+        <v>2794</v>
+      </c>
+      <c r="B375" s="5" t="s">
+        <v>2796</v>
+      </c>
+      <c r="C375" s="5" t="s">
+        <v>2797</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A376" s="1" t="s">
+        <v>2798</v>
+      </c>
+      <c r="B376" s="5" t="s">
+        <v>2795</v>
+      </c>
+      <c r="C376" s="5" t="s">
+        <v>2795</v>
       </c>
     </row>
   </sheetData>
@@ -20990,7 +21027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C766"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A883" workbookViewId="0">
       <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
email for application ongoing
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4394" uniqueCount="2804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4395" uniqueCount="2805">
   <si>
     <t>fi</t>
   </si>
@@ -8458,6 +8458,9 @@
   </si>
   <si>
     <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t>Pågår</t>
   </si>
 </sst>
 </file>
@@ -9496,8 +9499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A366" workbookViewId="0">
-      <selection activeCell="C381" sqref="C381"/>
+    <sheetView tabSelected="1" topLeftCell="A257" workbookViewId="0">
+      <selection activeCell="C276" sqref="C276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11761,6 +11764,9 @@
       </c>
       <c r="B275" s="5" t="s">
         <v>1429</v>
+      </c>
+      <c r="C275" s="5" t="s">
+        <v>2804</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
@@ -21064,8 +21070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C766"/>
   <sheetViews>
-    <sheetView topLeftCell="A883" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView topLeftCell="A322" workbookViewId="0">
+      <selection activeCell="B341" sqref="B341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
UI for request for commpletion
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4350" uniqueCount="2770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4352" uniqueCount="2772">
   <si>
     <t>fi</t>
   </si>
@@ -8356,6 +8356,12 @@
   </si>
   <si>
     <t xml:space="preserve">[Lupapiste] </t>
+  </si>
+  <si>
+    <t>Pyydä täydennyksiä</t>
+  </si>
+  <si>
+    <t>application.requestForComplement</t>
   </si>
 </sst>
 </file>
@@ -9422,10 +9428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C355"/>
+  <dimension ref="A1:C356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B338" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C351" sqref="C351"/>
+    <sheetView tabSelected="1" topLeftCell="A338" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A356" sqref="A356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12360,6 +12366,14 @@
       </c>
       <c r="C355" s="5" t="s">
         <v>2768</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A356" s="1" t="s">
+        <v>2771</v>
+      </c>
+      <c r="B356" s="5" t="s">
+        <v>2770</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last updates before kuntademo
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -8118,9 +8118,6 @@
     <t>varasto-tms._group_label</t>
   </si>
   <si>
-    <t>Uusi varasto tai muu sellainen</t>
-  </si>
-  <si>
     <t>laajentaminen._group_label</t>
   </si>
   <si>
@@ -8434,6 +8431,9 @@
   </si>
   <si>
     <t>Lupahakemus</t>
+  </si>
+  <si>
+    <t>Varasto, sauna, autotalli tai muu talousrakennus</t>
   </si>
 </sst>
 </file>
@@ -9502,8 +9502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="67" zoomScaleNormal="67" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B141" sqref="B141"/>
+    <sheetView tabSelected="1" topLeftCell="A334" zoomScale="67" zoomScaleNormal="67" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B349" sqref="B349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
@@ -9574,7 +9574,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>2750</v>
+        <v>2749</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -9582,7 +9582,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>2748</v>
+        <v>2747</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -9702,7 +9702,7 @@
         <v>42</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>2725</v>
+        <v>2724</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -9734,7 +9734,7 @@
         <v>48</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>2795</v>
+        <v>2794</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -10345,10 +10345,10 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
+        <v>2725</v>
+      </c>
+      <c r="B100" s="5" t="s">
         <v>2726</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>2727</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
@@ -10543,7 +10543,7 @@
         <v>355</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>2745</v>
+        <v>2744</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
@@ -10615,7 +10615,7 @@
         <v>2600</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>2741</v>
+        <v>2740</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
@@ -10631,7 +10631,7 @@
         <v>375</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
@@ -10679,7 +10679,7 @@
         <v>385</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>2751</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
@@ -11475,170 +11475,170 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239" s="1" t="s">
+        <v>2755</v>
+      </c>
+      <c r="B239" s="5" t="s">
         <v>2756</v>
-      </c>
-      <c r="B239" s="5" t="s">
-        <v>2757</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240" s="1" t="s">
+        <v>2757</v>
+      </c>
+      <c r="B240" s="5" t="s">
         <v>2758</v>
-      </c>
-      <c r="B240" s="5" t="s">
-        <v>2759</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" s="1" t="s">
+        <v>2753</v>
+      </c>
+      <c r="B241" s="5" t="s">
         <v>2754</v>
-      </c>
-      <c r="B241" s="5" t="s">
-        <v>2755</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="s">
+        <v>2763</v>
+      </c>
+      <c r="B242" s="5" t="s">
         <v>2764</v>
-      </c>
-      <c r="B242" s="5" t="s">
-        <v>2765</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="s">
+        <v>2759</v>
+      </c>
+      <c r="B243" s="5" t="s">
         <v>2760</v>
-      </c>
-      <c r="B243" s="5" t="s">
-        <v>2761</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" s="1" t="s">
+        <v>2769</v>
+      </c>
+      <c r="B244" s="5" t="s">
         <v>2770</v>
-      </c>
-      <c r="B244" s="5" t="s">
-        <v>2771</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" s="1" t="s">
-        <v>2769</v>
+        <v>2768</v>
       </c>
       <c r="B245" s="5" t="s">
-        <v>2768</v>
+        <v>2767</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" s="1" t="s">
+        <v>2761</v>
+      </c>
+      <c r="B246" s="5" t="s">
         <v>2762</v>
-      </c>
-      <c r="B246" s="5" t="s">
-        <v>2763</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" s="1" t="s">
+        <v>2765</v>
+      </c>
+      <c r="B247" s="5" t="s">
         <v>2766</v>
-      </c>
-      <c r="B247" s="5" t="s">
-        <v>2767</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" s="1" t="s">
+        <v>2773</v>
+      </c>
+      <c r="B248" s="5" t="s">
         <v>2774</v>
-      </c>
-      <c r="B248" s="5" t="s">
-        <v>2775</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" s="1" t="s">
+        <v>2771</v>
+      </c>
+      <c r="B249" s="5" t="s">
         <v>2772</v>
-      </c>
-      <c r="B249" s="5" t="s">
-        <v>2773</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" s="1" t="s">
+        <v>2775</v>
+      </c>
+      <c r="B250" s="5" t="s">
         <v>2776</v>
-      </c>
-      <c r="B250" s="5" t="s">
-        <v>2777</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" s="1" t="s">
+        <v>2779</v>
+      </c>
+      <c r="B251" s="5" t="s">
         <v>2780</v>
-      </c>
-      <c r="B251" s="5" t="s">
-        <v>2781</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" s="1" t="s">
+        <v>2777</v>
+      </c>
+      <c r="B252" s="5" t="s">
         <v>2778</v>
-      </c>
-      <c r="B252" s="5" t="s">
-        <v>2779</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" s="1" t="s">
+        <v>2783</v>
+      </c>
+      <c r="B253" s="5" t="s">
         <v>2784</v>
-      </c>
-      <c r="B253" s="5" t="s">
-        <v>2785</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" s="1" t="s">
+        <v>2781</v>
+      </c>
+      <c r="B254" s="5" t="s">
         <v>2782</v>
-      </c>
-      <c r="B254" s="5" t="s">
-        <v>2783</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" s="1" t="s">
-        <v>2789</v>
+        <v>2788</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>2787</v>
+        <v>2786</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" s="1" t="s">
-        <v>2788</v>
+        <v>2787</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>2787</v>
+        <v>2786</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A257" s="1" t="s">
+        <v>2785</v>
+      </c>
+      <c r="B257" s="5" t="s">
         <v>2786</v>
-      </c>
-      <c r="B257" s="5" t="s">
-        <v>2787</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A258" s="1" t="s">
+        <v>2791</v>
+      </c>
+      <c r="B258" s="5" t="s">
         <v>2792</v>
-      </c>
-      <c r="B258" s="5" t="s">
-        <v>2793</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A259" s="1" t="s">
+        <v>2789</v>
+      </c>
+      <c r="B259" s="5" t="s">
         <v>2790</v>
-      </c>
-      <c r="B259" s="5" t="s">
-        <v>2791</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.35">
@@ -12277,7 +12277,7 @@
         <v>1819</v>
       </c>
       <c r="B337" s="5" t="s">
-        <v>2752</v>
+        <v>2751</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.35">
@@ -12293,7 +12293,7 @@
         <v>1821</v>
       </c>
       <c r="B339" s="5" t="s">
-        <v>2753</v>
+        <v>2752</v>
       </c>
       <c r="C339" s="5" t="s">
         <v>540</v>
@@ -12304,7 +12304,7 @@
         <v>1823</v>
       </c>
       <c r="B340" s="5" t="s">
-        <v>2749</v>
+        <v>2748</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.35">
@@ -12376,92 +12376,92 @@
         <v>2689</v>
       </c>
       <c r="B349" s="5" t="s">
-        <v>2690</v>
+        <v>2795</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A350" s="9" t="s">
+        <v>2690</v>
+      </c>
+      <c r="B350" s="5" t="s">
         <v>2691</v>
-      </c>
-      <c r="B350" s="5" t="s">
-        <v>2692</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A351" s="9" t="s">
-        <v>2693</v>
+        <v>2692</v>
       </c>
       <c r="B351" s="5" t="s">
-        <v>2714</v>
+        <v>2713</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A352" s="9" t="s">
-        <v>2694</v>
+        <v>2693</v>
       </c>
       <c r="B352" s="5" t="s">
-        <v>2715</v>
+        <v>2714</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A353" s="9" t="s">
-        <v>2695</v>
+        <v>2694</v>
       </c>
       <c r="B353" s="5" t="s">
-        <v>2716</v>
+        <v>2715</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A354" s="9" t="s">
-        <v>2696</v>
+        <v>2695</v>
       </c>
       <c r="B354" s="5" t="s">
-        <v>2728</v>
+        <v>2727</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A355" s="9" t="s">
-        <v>2697</v>
+        <v>2696</v>
       </c>
       <c r="B355" s="5" t="s">
-        <v>2717</v>
+        <v>2716</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A356" s="9" t="s">
-        <v>2698</v>
+        <v>2697</v>
       </c>
       <c r="B356" s="5" t="s">
-        <v>2747</v>
+        <v>2746</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A357" s="9" t="s">
-        <v>2700</v>
+        <v>2699</v>
       </c>
       <c r="B357" s="5" t="s">
-        <v>2699</v>
+        <v>2698</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A358" s="9" t="s">
-        <v>2701</v>
+        <v>2700</v>
       </c>
       <c r="B358" s="5" t="s">
-        <v>2718</v>
+        <v>2717</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A359" s="9" t="s">
-        <v>2706</v>
+        <v>2705</v>
       </c>
       <c r="B359" s="5" t="s">
-        <v>2719</v>
+        <v>2718</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A360" s="9" t="s">
-        <v>2702</v>
+        <v>2701</v>
       </c>
       <c r="B360" s="5" t="s">
         <v>310</v>
@@ -12469,15 +12469,15 @@
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A361" s="9" t="s">
-        <v>2703</v>
+        <v>2702</v>
       </c>
       <c r="B361" s="5" t="s">
-        <v>2720</v>
+        <v>2719</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A362" s="9" t="s">
-        <v>2704</v>
+        <v>2703</v>
       </c>
       <c r="B362" s="5" t="s">
         <v>313</v>
@@ -12485,15 +12485,15 @@
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A363" s="9" t="s">
-        <v>2705</v>
+        <v>2704</v>
       </c>
       <c r="B363" s="5" t="s">
-        <v>2721</v>
+        <v>2720</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A364" s="9" t="s">
-        <v>2707</v>
+        <v>2706</v>
       </c>
       <c r="B364" s="5" t="s">
         <v>311</v>
@@ -12501,47 +12501,47 @@
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A365" s="9" t="s">
-        <v>2708</v>
+        <v>2707</v>
       </c>
       <c r="B365" s="5" t="s">
-        <v>2746</v>
+        <v>2745</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A366" s="9" t="s">
-        <v>2709</v>
+        <v>2708</v>
       </c>
       <c r="B366" s="5" t="s">
-        <v>2723</v>
+        <v>2722</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A367" s="9" t="s">
-        <v>2710</v>
+        <v>2709</v>
       </c>
       <c r="B367" s="5" t="s">
-        <v>2722</v>
+        <v>2721</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A368" s="9" t="s">
-        <v>2711</v>
+        <v>2710</v>
       </c>
       <c r="B368" s="5" t="s">
-        <v>2722</v>
+        <v>2721</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A369" s="9" t="s">
-        <v>2712</v>
+        <v>2711</v>
       </c>
       <c r="B369" s="5" t="s">
-        <v>2724</v>
+        <v>2723</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A370" s="9" t="s">
-        <v>2713</v>
+        <v>2712</v>
       </c>
       <c r="B370" s="5" t="s">
         <v>314</v>
@@ -12906,7 +12906,7 @@
         <v>460</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>2735</v>
+        <v>2734</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -12914,7 +12914,7 @@
         <v>461</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>2734</v>
+        <v>2733</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -12922,7 +12922,7 @@
         <v>462</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>2742</v>
+        <v>2741</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -12930,7 +12930,7 @@
         <v>463</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>2730</v>
+        <v>2729</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -13258,7 +13258,7 @@
         <v>522</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>2740</v>
+        <v>2739</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -13434,7 +13434,7 @@
         <v>589</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>2731</v>
+        <v>2730</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
@@ -13458,7 +13458,7 @@
         <v>594</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>2732</v>
+        <v>2731</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
@@ -13586,7 +13586,7 @@
         <v>624</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>2733</v>
+        <v>2732</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
@@ -14866,7 +14866,7 @@
         <v>894</v>
       </c>
       <c r="B283" s="5" t="s">
-        <v>2736</v>
+        <v>2735</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.35">
@@ -15274,7 +15274,7 @@
         <v>967</v>
       </c>
       <c r="B334" s="5" t="s">
-        <v>2731</v>
+        <v>2730</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.35">
@@ -15604,7 +15604,7 @@
         <v>1029</v>
       </c>
       <c r="B374" s="5" t="s">
-        <v>2731</v>
+        <v>2730</v>
       </c>
       <c r="C374" s="5"/>
     </row>
@@ -17224,7 +17224,7 @@
         <v>1210</v>
       </c>
       <c r="B554" s="5" t="s">
-        <v>2736</v>
+        <v>2735</v>
       </c>
       <c r="C554" s="5"/>
     </row>
@@ -17683,7 +17683,7 @@
         <v>1262</v>
       </c>
       <c r="B605" s="5" t="s">
-        <v>2731</v>
+        <v>2730</v>
       </c>
       <c r="C605" s="5"/>
     </row>
@@ -18330,7 +18330,7 @@
         <v>1406</v>
       </c>
       <c r="B678" s="5" t="s">
-        <v>2731</v>
+        <v>2730</v>
       </c>
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.35">
@@ -18354,7 +18354,7 @@
         <v>1409</v>
       </c>
       <c r="B681" s="5" t="s">
-        <v>2732</v>
+        <v>2731</v>
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.35">
@@ -18434,7 +18434,7 @@
         <v>1419</v>
       </c>
       <c r="B691" s="5" t="s">
-        <v>2739</v>
+        <v>2738</v>
       </c>
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.35">
@@ -19762,7 +19762,7 @@
         <v>1585</v>
       </c>
       <c r="B857" s="5" t="s">
-        <v>2736</v>
+        <v>2735</v>
       </c>
     </row>
     <row r="858" spans="1:2" x14ac:dyDescent="0.35">
@@ -20170,7 +20170,7 @@
         <v>1637</v>
       </c>
       <c r="B908" s="5" t="s">
-        <v>2731</v>
+        <v>2730</v>
       </c>
     </row>
     <row r="909" spans="1:2" x14ac:dyDescent="0.35">
@@ -20234,7 +20234,7 @@
         <v>1645</v>
       </c>
       <c r="B916" s="5" t="s">
-        <v>2737</v>
+        <v>2736</v>
       </c>
     </row>
     <row r="917" spans="1:2" x14ac:dyDescent="0.35">
@@ -20410,7 +20410,7 @@
         <v>92</v>
       </c>
       <c r="B938" s="5" t="s">
-        <v>2729</v>
+        <v>2728</v>
       </c>
       <c r="C938" s="5"/>
     </row>
@@ -20671,7 +20671,7 @@
         <v>138</v>
       </c>
       <c r="B967" s="5" t="s">
-        <v>2740</v>
+        <v>2739</v>
       </c>
       <c r="C967" s="5"/>
     </row>
@@ -20850,7 +20850,7 @@
         <v>171</v>
       </c>
       <c r="B986" s="5" t="s">
-        <v>2738</v>
+        <v>2737</v>
       </c>
       <c r="C986" s="5"/>
     </row>
@@ -27273,7 +27273,7 @@
         <v>2612</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>2743</v>
+        <v>2742</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -27289,7 +27289,7 @@
         <v>2616</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>2744</v>
+        <v>2743</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Moving localizations from txt to xlsx
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="156" yWindow="0" windowWidth="38400" windowHeight="14616" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="156" yWindow="0" windowWidth="38400" windowHeight="14616" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6392" uniqueCount="3573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6491" uniqueCount="3671">
   <si>
     <t>fi</t>
   </si>
@@ -10773,6 +10773,300 @@
   </si>
   <si>
     <t>hengelle</t>
+  </si>
+  <si>
+    <t>operations.asuinrakennus.desc: Hankkeesi vaatii luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.perus-tai-kant-rak-muutos.desc: Hankkeesi vaatii luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.varasto-tms.desc: Hankkeesi vaatii luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.vapaa-ajan-asuinrakennus.desc: Hankkeesi vaatii luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.julkinen-rakennus.desc: Hankkeesi vaatii luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.muu-uusi-rakentaminen.desc: Hankkeesi vaatii luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.laajentaminen.desc: Hankkeesi vaatii luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.kayttotark-muutos.desc: Hankkeesi vaatii luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.julkisivu-muutos.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.jakaminen-tai-yhdistaminen.desc: Hankkeesi vaatii luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.markatilan-laajentaminen.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.takka-tai-hormi.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.parveke-tai-terassi.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.muu-laajentaminen.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.auto-katos.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.masto-tms.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.mainoslaite.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.maalampo.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.aita.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.purkaminen.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.kaivuu.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.puun-kaataminen.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.muu-maisema-toimenpide.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.tontin-ajoliittyman-muutos.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.paikoutysjarjestus-muutos.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.kortteli-yht-alue-muutos.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.muu-tontti-tai-kort-muutos.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.jatevesi.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.muu-rakentaminen.desc: Hankkeesi vaatii todennäköisesti luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
+  </si>
+  <si>
+    <t>operations.tree.Rakentaminen ja purkaminen: Rakentaminen ja purkaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Elinympariston muuttaminen: Elinympäristön muuttaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Rakennuksen korjaaminen tai muuttaminen: Rakennuksen korjaaminen tai muuttaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Rakennelman rakentaminen: Rakennelman rakentaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Rakennuksen purkaminen: Rakennuksen purkaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Uuden rakennuksen rakentaminen: Uuden rakennuksen rakentaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Asuinrakennus: Asuinrakennuksen rakentaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Vapaa-ajan asuinrakennus: Vapaa-ajan asuinrakennuksen rakentaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Varasto, sauna, autotalli tai muu talousrakennus: Varaston, saunan, autotallin tai muun talousrakennuksen rakentaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Julkinen rakennus: Julkisen rakennuksen rakentaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Muun rakennuksen rakentaminen: Muun rakennuksen rakentaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Rakennuksen laajentaminen tai korjaaminen: Rakennuksen laajentaminen tai korjaaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Perustusten tai kantavien rakenteiden muuttaminen tai korjaaminen: Perustusten tai kantavien rakenteiden muuttaminen tai korjaaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Kayttotarkoituksen muutos: Rakennuksen tai sen osan käyttötarkoituksen muuttaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Rakennuksen julkisivun tai katon muuttaminen: Rakennuksen julkisivun tai katon muuttaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Asuinhuoneiston jakaminen tai yhdistaminen: Asuinhuoneiston jakaminen tai yhdistäminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Markatilan laajentaminen: Märkätilan muuttaminen tai laajentaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Takan ja savuhormin rakentaminen: Takan ja savuhormin rakentaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Parvekkeen tai terassin lasittaminen: Parvekkeen tai terassin rakentaminen tai lasittaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Muu rakennuksen muutostyo: Muu rakennuksen muutostyö</t>
+  </si>
+  <si>
+    <t>operations.tree.Auto- tai grillikatos, vaja, kioski tai vastaava:Auto- tai grillikatoksen, vajan, kioskin tai vastaavan rakentaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Masto, piippu, sailio, laituri tai vastaava: Maston, piipun, säiliön, laiturin tai vastaavan rakentaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Mainoslaite: Mainos- tai muun laitteen asentaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Aita: Aidan rakentaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Maalampokaivon poraaminen tai lammonkeruuputkiston asentaminen: Maalämpökaivon poraaminen tai lämmönkeruuputkiston asentaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Rakennuksen jatevesijarjestelman uusiminen: Rakennuksen jätevesijärjestelmän uusiminen tai rakentaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Muun rakennelman rakentaminen: Muun rakennelman rakentaminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Maisemaa muutava toimenpide: Maisemaa muuttava toimenpide</t>
+  </si>
+  <si>
+    <t>operations.tree.Tontti tai korttelialueen jarjestelymuutos: Tontti- tai korttelialueen järjestelymuutos</t>
+  </si>
+  <si>
+    <t>operations.tree.Kaivaminen, louhiminen tai maan tayttaminen:Kaivaminen, louhiminen tai maan täyttäminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Puun kaataminen: Puun kaataminen</t>
+  </si>
+  <si>
+    <t>operations.tree.Muu maisemaa muuttava toimenpide: Muu maisemaa muuttava toimenpide</t>
+  </si>
+  <si>
+    <t>operations.tree.Tontin ajoliittyman muutos: Tontin ajoliittymän muutos</t>
+  </si>
+  <si>
+    <t>operations.tree.Paikoitusjarjestelyihin liittyvat muutokset: Paikoitusjärjestelyihin liittyvät muutokset</t>
+  </si>
+  <si>
+    <t>operations.tree.Korttelin yhteisiin alueisiin liittyva muutos: Korttelin yhteisiin alueisiin liittyvä muutos</t>
+  </si>
+  <si>
+    <t>operations.tree.Muu-tontti-tai-korttelialueen-jarjestelymuutos: Muu tontti- tai korttelialueen järjestelymuutos</t>
+  </si>
+  <si>
+    <t>operations.selected</t>
+  </si>
+  <si>
+    <t>Valittu toimenpide:</t>
+  </si>
+  <si>
+    <t>create.choose-op</t>
+  </si>
+  <si>
+    <t>Valitse toimenpide:</t>
+  </si>
+  <si>
+    <t>operations.add</t>
+  </si>
+  <si>
+    <t>integration.getAddressNotWorking</t>
+  </si>
+  <si>
+    <t>Kolmannenosapuolen osoitehakupalvelu ei ole käytettävissä, ole hyvä ja syötä osoite ja kunta:</t>
+  </si>
+  <si>
+    <t>municipalityNotSupported</t>
+  </si>
+  <si>
+    <t>Kunta ei mukana lupapiste.fi palvelussa.</t>
+  </si>
+  <si>
+    <t>municipality.564</t>
+  </si>
+  <si>
+    <t>Oulu</t>
+  </si>
+  <si>
+    <t>municipality.links</t>
+  </si>
+  <si>
+    <t>Kunnan rakennusvalvonnan suosittelemat linkit:</t>
+  </si>
+  <si>
+    <t>person-selector</t>
+  </si>
+  <si>
+    <t>Valitse henkilö</t>
+  </si>
+  <si>
+    <t>register.accept-terms.label</t>
+  </si>
+  <si>
+    <t>Hyväksyn palvelun</t>
+  </si>
+  <si>
+    <t>register.accept-terms.link</t>
+  </si>
+  <si>
+    <t>käyttöehdot</t>
+  </si>
+  <si>
+    <t>attachment.upload.instructions</t>
+  </si>
+  <si>
+    <t>Suurin sallittu tiedostokoko on 100 Mt. Sallitut tiedostomuodot ovat:</t>
+  </si>
+  <si>
+    <t>invite.error.missing-parameters</t>
+  </si>
+  <si>
+    <t>Täytä kaikki kentät.</t>
+  </si>
+  <si>
+    <t>invite.already-has-auth</t>
+  </si>
+  <si>
+    <t>email.title.new-comment</t>
+  </si>
+  <si>
+    <t>uusi kommentti</t>
+  </si>
+  <si>
+    <t>Kyseinen henkilö on jo kutsuttu.</t>
+  </si>
+  <si>
+    <t>email.title.state-change</t>
+  </si>
+  <si>
+    <t>hakemuksen tila muuttunut</t>
+  </si>
+  <si>
+    <t>email.title.verdict</t>
+  </si>
+  <si>
+    <t>päätös</t>
+  </si>
+  <si>
+    <t>email.title.invite</t>
+  </si>
+  <si>
+    <t>kutsu</t>
   </si>
 </sst>
 </file>
@@ -11953,10 +12247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C429"/>
+  <dimension ref="A1:C446"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A413" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B446" sqref="B446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
@@ -15476,6 +15770,142 @@
       </c>
       <c r="B429" s="5" t="s">
         <v>3206</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A430" s="1" t="s">
+        <v>3638</v>
+      </c>
+      <c r="B430" s="5" t="s">
+        <v>3639</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A431" s="1" t="s">
+        <v>3642</v>
+      </c>
+      <c r="B431" s="5" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A432" s="1" t="s">
+        <v>3640</v>
+      </c>
+      <c r="B432" s="5" t="s">
+        <v>3641</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A433" s="1" t="s">
+        <v>3643</v>
+      </c>
+      <c r="B433" s="5" t="s">
+        <v>3644</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A434" s="1" t="s">
+        <v>3645</v>
+      </c>
+      <c r="B434" s="5" t="s">
+        <v>3646</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A435" s="1" t="s">
+        <v>3647</v>
+      </c>
+      <c r="B435" s="5" t="s">
+        <v>3648</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A436" s="1" t="s">
+        <v>3649</v>
+      </c>
+      <c r="B436" s="5" t="s">
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A437" s="1" t="s">
+        <v>3651</v>
+      </c>
+      <c r="B437" s="5" t="s">
+        <v>3652</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A438" s="1" t="s">
+        <v>3653</v>
+      </c>
+      <c r="B438" s="5" t="s">
+        <v>3654</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A439" s="1" t="s">
+        <v>3655</v>
+      </c>
+      <c r="B439" s="5" t="s">
+        <v>3656</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A440" s="1" t="s">
+        <v>3657</v>
+      </c>
+      <c r="B440" s="5" t="s">
+        <v>3658</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A441" s="1" t="s">
+        <v>3659</v>
+      </c>
+      <c r="B441" s="5" t="s">
+        <v>3660</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A442" s="1" t="s">
+        <v>3661</v>
+      </c>
+      <c r="B442" s="5" t="s">
+        <v>3664</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A443" s="1" t="s">
+        <v>3662</v>
+      </c>
+      <c r="B443" s="5" t="s">
+        <v>3663</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A444" s="1" t="s">
+        <v>3665</v>
+      </c>
+      <c r="B444" s="5" t="s">
+        <v>3666</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A445" s="1" t="s">
+        <v>3667</v>
+      </c>
+      <c r="B445" s="5" t="s">
+        <v>3668</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A446" s="1" t="s">
+        <v>3669</v>
+      </c>
+      <c r="B446" s="5" t="s">
+        <v>3670</v>
       </c>
     </row>
   </sheetData>
@@ -15526,10 +15956,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1556"/>
+  <dimension ref="A1:C1621"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1514" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="B1566" sqref="B1566"/>
+    <sheetView topLeftCell="A1580" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="A1586" sqref="A1586:A1621"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
@@ -28619,6 +29049,331 @@
       </c>
       <c r="B1556" s="2" t="s">
         <v>3572</v>
+      </c>
+    </row>
+    <row r="1557" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1557" s="1" t="s">
+        <v>3573</v>
+      </c>
+    </row>
+    <row r="1558" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1558" s="1" t="s">
+        <v>3574</v>
+      </c>
+    </row>
+    <row r="1559" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1559" s="1" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1560" s="1" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1561" s="1" t="s">
+        <v>3577</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1562" s="1" t="s">
+        <v>3578</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1563" s="1" t="s">
+        <v>3579</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1564" s="1" t="s">
+        <v>3580</v>
+      </c>
+    </row>
+    <row r="1565" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1565" s="1" t="s">
+        <v>3581</v>
+      </c>
+    </row>
+    <row r="1566" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1566" s="1" t="s">
+        <v>3582</v>
+      </c>
+    </row>
+    <row r="1567" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1567" s="1" t="s">
+        <v>3583</v>
+      </c>
+    </row>
+    <row r="1568" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1568" s="1" t="s">
+        <v>3584</v>
+      </c>
+    </row>
+    <row r="1569" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1569" s="1" t="s">
+        <v>3585</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1570" s="1" t="s">
+        <v>3586</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1571" s="1" t="s">
+        <v>3587</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1572" s="1" t="s">
+        <v>3588</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1573" s="1" t="s">
+        <v>3589</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1574" s="1" t="s">
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1575" s="1" t="s">
+        <v>3591</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1576" s="1" t="s">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1577" s="1" t="s">
+        <v>3593</v>
+      </c>
+    </row>
+    <row r="1578" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1578" s="1" t="s">
+        <v>3594</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1579" s="1" t="s">
+        <v>3595</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1580" s="1" t="s">
+        <v>3596</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1581" s="1" t="s">
+        <v>3597</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1582" s="1" t="s">
+        <v>3598</v>
+      </c>
+    </row>
+    <row r="1583" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1583" s="1" t="s">
+        <v>3599</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1584" s="1" t="s">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1585" s="1" t="s">
+        <v>3601</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1586" s="1" t="s">
+        <v>3602</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1587" s="1" t="s">
+        <v>3603</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1588" s="1" t="s">
+        <v>3604</v>
+      </c>
+    </row>
+    <row r="1589" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1589" s="1" t="s">
+        <v>3605</v>
+      </c>
+    </row>
+    <row r="1590" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1590" s="1" t="s">
+        <v>3606</v>
+      </c>
+    </row>
+    <row r="1591" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1591" s="1" t="s">
+        <v>3607</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1592" s="1" t="s">
+        <v>3608</v>
+      </c>
+    </row>
+    <row r="1593" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1593" s="1" t="s">
+        <v>3609</v>
+      </c>
+    </row>
+    <row r="1594" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1594" s="1" t="s">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="1595" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1595" s="1" t="s">
+        <v>3611</v>
+      </c>
+    </row>
+    <row r="1596" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1596" s="1" t="s">
+        <v>3612</v>
+      </c>
+    </row>
+    <row r="1597" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1597" s="1" t="s">
+        <v>3613</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1598" s="1" t="s">
+        <v>3614</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1599" s="1" t="s">
+        <v>3615</v>
+      </c>
+    </row>
+    <row r="1600" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1600" s="1" t="s">
+        <v>3616</v>
+      </c>
+    </row>
+    <row r="1601" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1601" s="1" t="s">
+        <v>3617</v>
+      </c>
+    </row>
+    <row r="1602" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1602" s="1" t="s">
+        <v>3618</v>
+      </c>
+    </row>
+    <row r="1603" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1603" s="1" t="s">
+        <v>3619</v>
+      </c>
+    </row>
+    <row r="1604" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1604" s="1" t="s">
+        <v>3620</v>
+      </c>
+    </row>
+    <row r="1605" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1605" s="1" t="s">
+        <v>3621</v>
+      </c>
+    </row>
+    <row r="1606" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1606" s="1" t="s">
+        <v>3622</v>
+      </c>
+    </row>
+    <row r="1607" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1607" s="1" t="s">
+        <v>3623</v>
+      </c>
+    </row>
+    <row r="1608" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1608" s="1" t="s">
+        <v>3624</v>
+      </c>
+    </row>
+    <row r="1609" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1609" s="1" t="s">
+        <v>3625</v>
+      </c>
+    </row>
+    <row r="1610" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1610" s="1" t="s">
+        <v>3626</v>
+      </c>
+    </row>
+    <row r="1611" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1611" s="1" t="s">
+        <v>3627</v>
+      </c>
+    </row>
+    <row r="1612" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1612" s="1" t="s">
+        <v>3628</v>
+      </c>
+    </row>
+    <row r="1613" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1613" s="1" t="s">
+        <v>3629</v>
+      </c>
+    </row>
+    <row r="1614" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1614" s="1" t="s">
+        <v>3630</v>
+      </c>
+    </row>
+    <row r="1615" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1615" s="1" t="s">
+        <v>3631</v>
+      </c>
+    </row>
+    <row r="1616" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1616" s="1" t="s">
+        <v>3632</v>
+      </c>
+    </row>
+    <row r="1617" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1617" s="1" t="s">
+        <v>3633</v>
+      </c>
+    </row>
+    <row r="1618" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1618" s="1" t="s">
+        <v>3634</v>
+      </c>
+    </row>
+    <row r="1619" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1619" s="1" t="s">
+        <v>3635</v>
+      </c>
+    </row>
+    <row r="1620" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1620" s="1" t="s">
+        <v>3636</v>
+      </c>
+    </row>
+    <row r="1621" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1621" s="1" t="s">
+        <v>3637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got missing localization error from inforequest_submitted
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7469" uniqueCount="4548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7471" uniqueCount="4549">
   <si>
     <t>fi</t>
   </si>
@@ -13699,6 +13699,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tänne voit lisätä hakemukseen kuuluvia liitteitä. Viranomainen voi myös pyytää sinulta tarpeellisia liitteitä. Nämä pyynnöt merkitään taulukossa punaisella lipulla. Viranomainen voi myös merkitä liitteen alustavasti hyväksytyksi tai korjattavaksi. Tämä ei ole vielä virallinen hyväksyntä, sillä sitä varten hakemus pitää käsitellä kunnan päätöksentekoprosessin mukaisesti. </t>
+  </si>
+  <si>
+    <t>inforequest_submitted</t>
   </si>
 </sst>
 </file>
@@ -14074,7 +14077,47 @@
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="53">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -14909,10 +14952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C421"/>
+  <dimension ref="A1:C422"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A247" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B282" sqref="B282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -17205,1168 +17248,1176 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" s="1" t="s">
-        <v>8</v>
+        <v>4548</v>
       </c>
       <c r="B281" s="5" t="s">
-        <v>9</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" s="1" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="B282" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" s="1" t="s">
-        <v>214</v>
+        <v>91</v>
       </c>
       <c r="B283" s="5" t="s">
-        <v>215</v>
+        <v>13</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" s="1" t="s">
-        <v>486</v>
+        <v>214</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>5</v>
+        <v>215</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" s="1" t="s">
-        <v>3570</v>
+        <v>486</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>3571</v>
+        <v>5</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" s="1" t="s">
-        <v>3587</v>
+        <v>3570</v>
       </c>
       <c r="B286" s="5" t="s">
-        <v>3590</v>
+        <v>3571</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" s="1" t="s">
+        <v>3587</v>
+      </c>
+      <c r="B287" s="5" t="s">
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A288" s="1" t="s">
         <v>3585</v>
       </c>
-      <c r="B287" s="5" t="s">
+      <c r="B288" s="5" t="s">
         <v>3586</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="9" t="s">
-        <v>2665</v>
-      </c>
-      <c r="B288" s="5" t="s">
-        <v>2663</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="9" t="s">
-        <v>2676</v>
+        <v>2665</v>
       </c>
       <c r="B289" s="5" t="s">
-        <v>2697</v>
+        <v>2663</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="9" t="s">
-        <v>2685</v>
+        <v>2676</v>
       </c>
       <c r="B290" s="5" t="s">
-        <v>310</v>
+        <v>2697</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="9" t="s">
-        <v>2693</v>
+        <v>2685</v>
       </c>
       <c r="B291" s="5" t="s">
-        <v>2704</v>
+        <v>310</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="9" t="s">
-        <v>2675</v>
+        <v>2693</v>
       </c>
       <c r="B292" s="5" t="s">
-        <v>2696</v>
+        <v>2704</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="9" t="s">
-        <v>2690</v>
+        <v>2675</v>
       </c>
       <c r="B293" s="5" t="s">
-        <v>2703</v>
+        <v>2696</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="9" t="s">
-        <v>2692</v>
+        <v>2690</v>
       </c>
       <c r="B294" s="5" t="s">
-        <v>2788</v>
+        <v>2703</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="9" t="s">
-        <v>2674</v>
+        <v>2692</v>
       </c>
       <c r="B295" s="5" t="s">
-        <v>2695</v>
+        <v>2788</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" s="9" t="s">
+        <v>2674</v>
+      </c>
+      <c r="B296" s="5" t="s">
+        <v>2695</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" s="9" t="s">
         <v>2672</v>
       </c>
-      <c r="B296" s="5" t="s">
+      <c r="B297" s="5" t="s">
         <v>2673</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A297" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B297" s="5" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B298" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B299" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A300" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B299" s="5" t="s">
+      <c r="B300" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="C299" s="5" t="s">
+      <c r="C300" s="5" t="s">
         <v>1791</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A300" s="9" t="s">
-        <v>2683</v>
-      </c>
-      <c r="B300" s="5" t="s">
-        <v>2779</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="9" t="s">
-        <v>2691</v>
+        <v>2683</v>
       </c>
       <c r="B301" s="5" t="s">
-        <v>2788</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="9" t="s">
-        <v>2677</v>
+        <v>2691</v>
       </c>
       <c r="B302" s="5" t="s">
-        <v>2707</v>
+        <v>2788</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="9" t="s">
+        <v>2677</v>
+      </c>
+      <c r="B303" s="5" t="s">
+        <v>2707</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A304" s="9" t="s">
         <v>2682</v>
       </c>
-      <c r="B303" s="5" t="s">
+      <c r="B304" s="5" t="s">
         <v>2699</v>
-      </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A304" s="1" t="s">
-        <v>1337</v>
-      </c>
-      <c r="B304" s="5" t="s">
-        <v>1338</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A305" s="1" t="s">
-        <v>3575</v>
+        <v>1337</v>
       </c>
       <c r="B305" s="5" t="s">
-        <v>3576</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A306" s="1" t="s">
-        <v>1339</v>
+        <v>3575</v>
       </c>
       <c r="B306" s="5" t="s">
-        <v>1340</v>
+        <v>3576</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A307" s="1" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="B307" s="5" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B308" s="5" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A309" s="1" t="s">
         <v>3572</v>
       </c>
-      <c r="B308" s="5" t="s">
+      <c r="B309" s="5" t="s">
         <v>3573</v>
-      </c>
-    </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A309" s="9" t="s">
-        <v>2684</v>
-      </c>
-      <c r="B309" s="5" t="s">
-        <v>2701</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" s="9" t="s">
-        <v>2689</v>
+        <v>2684</v>
       </c>
       <c r="B310" s="5" t="s">
-        <v>2722</v>
+        <v>2701</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" s="9" t="s">
+        <v>2689</v>
+      </c>
+      <c r="B311" s="5" t="s">
+        <v>2722</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A312" s="9" t="s">
         <v>2686</v>
       </c>
-      <c r="B311" s="5" t="s">
+      <c r="B312" s="5" t="s">
         <v>2702</v>
-      </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A312" s="1" t="s">
-        <v>1317</v>
-      </c>
-      <c r="B312" s="5" t="s">
-        <v>1318</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A313" s="1" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B313" s="6" t="s">
-        <v>1787</v>
-      </c>
-      <c r="C313" s="6" t="s">
-        <v>1787</v>
+        <v>1317</v>
+      </c>
+      <c r="B313" s="5" t="s">
+        <v>1318</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A314" s="1" t="s">
         <v>1314</v>
       </c>
-      <c r="B314" s="5" t="s">
-        <v>2826</v>
+      <c r="B314" s="6" t="s">
+        <v>1787</v>
+      </c>
+      <c r="C314" s="6" t="s">
+        <v>1787</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A315" s="1" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="B315" s="5" t="s">
-        <v>1316</v>
+        <v>2826</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A316" s="1" t="s">
-        <v>1319</v>
+        <v>1315</v>
       </c>
       <c r="B316" s="5" t="s">
-        <v>1320</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A317" s="1" t="s">
-        <v>1325</v>
+        <v>1319</v>
       </c>
       <c r="B317" s="5" t="s">
-        <v>1326</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A318" s="1" t="s">
-        <v>1329</v>
+        <v>1325</v>
       </c>
       <c r="B318" s="5" t="s">
-        <v>1330</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A319" s="1" t="s">
-        <v>1327</v>
+        <v>1329</v>
       </c>
       <c r="B319" s="5" t="s">
-        <v>1328</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A320" s="1" t="s">
-        <v>1323</v>
+        <v>1327</v>
       </c>
       <c r="B320" s="5" t="s">
-        <v>1324</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A321" s="1" t="s">
-        <v>1321</v>
+        <v>1323</v>
       </c>
       <c r="B321" s="5" t="s">
-        <v>1322</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322" s="1" t="s">
-        <v>1312</v>
+        <v>1321</v>
       </c>
       <c r="B322" s="5" t="s">
-        <v>1313</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A323" s="1" t="s">
-        <v>3180</v>
+        <v>1312</v>
       </c>
       <c r="B323" s="5" t="s">
-        <v>3181</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A324" s="1" t="s">
-        <v>560</v>
+        <v>3180</v>
       </c>
       <c r="B324" s="5" t="s">
-        <v>561</v>
+        <v>3181</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A325" s="1" t="s">
-        <v>364</v>
+        <v>560</v>
       </c>
       <c r="B325" s="5" t="s">
-        <v>365</v>
+        <v>561</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A326" s="1" t="s">
-        <v>2583</v>
+        <v>364</v>
       </c>
       <c r="B326" s="5" t="s">
-        <v>2718</v>
+        <v>365</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A327" s="1" t="s">
-        <v>372</v>
+        <v>2583</v>
       </c>
       <c r="B327" s="5" t="s">
-        <v>2766</v>
+        <v>2718</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A328" s="1" t="s">
-        <v>356</v>
+        <v>372</v>
       </c>
       <c r="B328" s="5" t="s">
-        <v>357</v>
+        <v>2766</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A329" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B329" s="5" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A330" s="1" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="B330" s="5" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A331" s="1" t="s">
-        <v>352</v>
+        <v>366</v>
       </c>
       <c r="B331" s="5" t="s">
-        <v>2721</v>
+        <v>367</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A332" s="1" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="B332" s="5" t="s">
-        <v>363</v>
+        <v>2721</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A333" s="1" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="B333" s="5" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A334" s="1" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="B334" s="5" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A335" s="1" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="B335" s="5" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A336" s="1" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="B336" s="5" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A337" s="1" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="B337" s="5" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A338" s="1" t="s">
-        <v>2823</v>
+        <v>368</v>
       </c>
       <c r="B338" s="5" t="s">
-        <v>2662</v>
+        <v>369</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A339" s="1" t="s">
-        <v>2769</v>
-      </c>
-      <c r="B339" s="4" t="s">
-        <v>2770</v>
-      </c>
-      <c r="C339" s="5" t="s">
-        <v>2772</v>
+        <v>2823</v>
+      </c>
+      <c r="B339" s="5" t="s">
+        <v>2662</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A340" s="1" t="s">
-        <v>14</v>
+        <v>2769</v>
       </c>
       <c r="B340" s="4" t="s">
-        <v>15</v>
+        <v>2770</v>
       </c>
       <c r="C340" s="5" t="s">
-        <v>1789</v>
+        <v>2772</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A341" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="B341" s="5" t="s">
-        <v>563</v>
+        <v>14</v>
+      </c>
+      <c r="B341" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C341" s="5" t="s">
+        <v>1789</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A342" s="1" t="s">
-        <v>264</v>
+        <v>562</v>
       </c>
       <c r="B342" s="5" t="s">
-        <v>265</v>
+        <v>563</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A343" s="1" t="s">
-        <v>3569</v>
+        <v>264</v>
       </c>
       <c r="B343" s="5" t="s">
-        <v>395</v>
+        <v>265</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A344" s="1" t="s">
-        <v>3565</v>
+        <v>3569</v>
       </c>
       <c r="B344" s="5" t="s">
-        <v>3566</v>
+        <v>395</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A345" s="1" t="s">
+        <v>3565</v>
+      </c>
+      <c r="B345" s="5" t="s">
+        <v>3566</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A346" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="B345" s="5" t="s">
+      <c r="B346" s="5" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A346" s="9" t="s">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A347" s="9" t="s">
         <v>2679</v>
       </c>
-      <c r="B346" s="5" t="s">
+      <c r="B347" s="5" t="s">
         <v>2723</v>
-      </c>
-    </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A347" s="1" t="s">
-        <v>1002</v>
-      </c>
-      <c r="B347" s="5" t="s">
-        <v>1003</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A348" s="1" t="s">
-        <v>564</v>
+        <v>1002</v>
       </c>
       <c r="B348" s="5" t="s">
-        <v>387</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A349" s="1" t="s">
-        <v>1776</v>
+        <v>564</v>
       </c>
       <c r="B349" s="5" t="s">
-        <v>43</v>
+        <v>387</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A350" s="1" t="s">
-        <v>3577</v>
+        <v>1776</v>
       </c>
       <c r="B350" s="5" t="s">
-        <v>3578</v>
+        <v>43</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A351" s="1" t="s">
-        <v>1811</v>
+        <v>3577</v>
       </c>
       <c r="B351" s="5" t="s">
-        <v>416</v>
+        <v>3578</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A352" s="1" t="s">
+        <v>1811</v>
+      </c>
+      <c r="B352" s="5" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A353" s="1" t="s">
         <v>2776</v>
       </c>
-      <c r="B352" s="4" t="s">
+      <c r="B353" s="4" t="s">
         <v>2771</v>
       </c>
-      <c r="C352" s="5" t="s">
+      <c r="C353" s="5" t="s">
         <v>2773</v>
       </c>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A353" s="9" t="s">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A354" s="9" t="s">
         <v>2694</v>
       </c>
-      <c r="B353" s="5" t="s">
+      <c r="B354" s="5" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A354" s="9" t="s">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A355" s="9" t="s">
         <v>2688</v>
       </c>
-      <c r="B354" s="5" t="s">
+      <c r="B355" s="5" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A355" s="9" t="s">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A356" s="9" t="s">
         <v>2666</v>
       </c>
-      <c r="B355" s="5" t="s">
+      <c r="B356" s="5" t="s">
         <v>2664</v>
       </c>
     </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A356" s="1" t="s">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A357" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B356" s="5" t="s">
+      <c r="B357" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A357" s="1" t="s">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A358" s="1" t="s">
         <v>3579</v>
       </c>
-      <c r="B357" s="5" t="s">
+      <c r="B358" s="5" t="s">
         <v>3580</v>
       </c>
     </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A358" s="1" t="s">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A359" s="1" t="s">
         <v>3581</v>
       </c>
-      <c r="B358" s="5" t="s">
+      <c r="B359" s="5" t="s">
         <v>3582</v>
       </c>
     </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A359" s="1" t="s">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A360" s="1" t="s">
         <v>2797</v>
       </c>
-      <c r="B359" s="5" t="s">
+      <c r="B360" s="5" t="s">
         <v>2798</v>
       </c>
     </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A360" s="1" t="s">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A361" s="1" t="s">
         <v>2812</v>
       </c>
-      <c r="B360" s="5" t="s">
+      <c r="B361" s="5" t="s">
         <v>2811</v>
       </c>
     </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A361" s="1" t="s">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A362" s="1" t="s">
         <v>2813</v>
       </c>
-      <c r="B361" s="5" t="s">
+      <c r="B362" s="5" t="s">
         <v>2814</v>
       </c>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A362" s="1" t="s">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A363" s="1" t="s">
         <v>2804</v>
       </c>
-      <c r="B362" s="5" t="s">
+      <c r="B363" s="5" t="s">
         <v>2801</v>
       </c>
     </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A363" s="1" t="s">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A364" s="1" t="s">
         <v>2805</v>
       </c>
-      <c r="B363" s="5" t="s">
+      <c r="B364" s="5" t="s">
         <v>2802</v>
       </c>
     </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A364" s="1" t="s">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A365" s="1" t="s">
         <v>2806</v>
       </c>
-      <c r="B364" s="5" t="s">
+      <c r="B365" s="5" t="s">
         <v>2803</v>
       </c>
     </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A365" s="1" t="s">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A366" s="1" t="s">
         <v>2793</v>
       </c>
-      <c r="B365" s="5" t="s">
+      <c r="B366" s="5" t="s">
         <v>2794</v>
       </c>
     </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A366" s="1" t="s">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A367" s="1" t="s">
         <v>2795</v>
       </c>
-      <c r="B366" s="5" t="s">
+      <c r="B367" s="5" t="s">
         <v>2796</v>
       </c>
     </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A367" s="1" t="s">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A368" s="1" t="s">
         <v>2789</v>
       </c>
-      <c r="B367" s="5" t="s">
+      <c r="B368" s="5" t="s">
         <v>2790</v>
-      </c>
-    </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A368" s="1" t="s">
-        <v>2792</v>
-      </c>
-      <c r="B368" s="5" t="s">
-        <v>2791</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A369" s="1" t="s">
-        <v>2808</v>
+        <v>2792</v>
       </c>
       <c r="B369" s="5" t="s">
-        <v>2807</v>
+        <v>2791</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A370" s="1" t="s">
-        <v>2810</v>
+        <v>2808</v>
       </c>
       <c r="B370" s="5" t="s">
-        <v>2809</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A371" s="1" t="s">
-        <v>176</v>
+        <v>2810</v>
       </c>
       <c r="B371" s="5" t="s">
-        <v>177</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A372" s="1" t="s">
-        <v>543</v>
+        <v>176</v>
       </c>
       <c r="B372" s="5" t="s">
-        <v>544</v>
+        <v>177</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A373" s="1" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="B373" s="5" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A374" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B374" s="5" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A375" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B375" s="5" t="s">
-        <v>177</v>
+        <v>538</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A376" s="1" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="B376" s="5" t="s">
-        <v>538</v>
+        <v>177</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A377" s="1" t="s">
-        <v>377</v>
+        <v>537</v>
       </c>
       <c r="B377" s="5" t="s">
-        <v>2662</v>
+        <v>538</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A378" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B378" s="5" t="s">
-        <v>379</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A379" s="1" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B379" s="5" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A380" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B380" s="5" t="s">
-        <v>3</v>
+        <v>376</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A381" s="1" t="s">
-        <v>188</v>
+        <v>374</v>
       </c>
       <c r="B381" s="5" t="s">
-        <v>189</v>
+        <v>3</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A382" s="1" t="s">
-        <v>1381</v>
+        <v>188</v>
       </c>
       <c r="B382" s="5" t="s">
-        <v>1382</v>
-      </c>
-      <c r="C382" s="5" t="s">
-        <v>1794</v>
+        <v>189</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A383" s="1" t="s">
-        <v>206</v>
+        <v>1381</v>
       </c>
       <c r="B383" s="5" t="s">
-        <v>207</v>
+        <v>1382</v>
+      </c>
+      <c r="C383" s="5" t="s">
+        <v>1794</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A384" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B384" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="C384" s="5" t="s">
-        <v>1801</v>
+        <v>207</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A385" s="1" t="s">
-        <v>3171</v>
+        <v>212</v>
       </c>
       <c r="B385" s="5" t="s">
-        <v>7</v>
+        <v>213</v>
+      </c>
+      <c r="C385" s="5" t="s">
+        <v>1801</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A386" s="1" t="s">
-        <v>3175</v>
+        <v>3171</v>
       </c>
       <c r="B386" s="5" t="s">
-        <v>544</v>
+        <v>7</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A387" s="1" t="s">
-        <v>3167</v>
+        <v>3175</v>
       </c>
       <c r="B387" s="5" t="s">
-        <v>3168</v>
+        <v>544</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A388" s="1" t="s">
-        <v>3173</v>
+        <v>3167</v>
       </c>
       <c r="B388" s="5" t="s">
-        <v>3174</v>
+        <v>3168</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A389" s="1" t="s">
-        <v>3172</v>
+        <v>3173</v>
       </c>
       <c r="B389" s="5" t="s">
-        <v>177</v>
+        <v>3174</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A390" s="1" t="s">
-        <v>3169</v>
+        <v>3172</v>
       </c>
       <c r="B390" s="5" t="s">
-        <v>3170</v>
+        <v>177</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A391" s="1" t="s">
-        <v>304</v>
+        <v>3169</v>
       </c>
       <c r="B391" s="5" t="s">
-        <v>305</v>
+        <v>3170</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A392" s="1" t="s">
-        <v>1281</v>
+        <v>304</v>
       </c>
       <c r="B392" s="5" t="s">
-        <v>1282</v>
+        <v>305</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A393" s="1" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B393" s="5" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A394" s="1" t="s">
         <v>1308</v>
       </c>
-      <c r="B393" s="5" t="s">
+      <c r="B394" s="5" t="s">
         <v>1309</v>
       </c>
     </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A394" s="9" t="s">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A395" s="9" t="s">
         <v>2678</v>
       </c>
-      <c r="B394" s="5" t="s">
+      <c r="B395" s="5" t="s">
         <v>2698</v>
       </c>
     </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A395" s="7" t="s">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A396" s="7" t="s">
         <v>1816</v>
       </c>
-      <c r="B395" s="5" t="s">
+      <c r="B396" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="C395" s="5" t="s">
+      <c r="C396" s="5" t="s">
         <v>314</v>
-      </c>
-    </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A396" s="1" t="s">
-        <v>1778</v>
-      </c>
-      <c r="B396" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C396" s="5" t="s">
-        <v>1798</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A397" s="1" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B397" s="5" t="s">
-        <v>1780</v>
+        <v>199</v>
+      </c>
+      <c r="C397" s="5" t="s">
+        <v>1798</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A398" s="1" t="s">
-        <v>3203</v>
+        <v>1779</v>
       </c>
       <c r="B398" s="5" t="s">
-        <v>3204</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A399" s="1" t="s">
-        <v>182</v>
+        <v>3203</v>
       </c>
       <c r="B399" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C399" s="5" t="s">
-        <v>183</v>
+        <v>3204</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A400" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B400" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C400" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A401" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B400" s="5" t="s">
+      <c r="B401" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C400" s="5" t="s">
+      <c r="C401" s="5" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A401" s="1" t="s">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A402" s="1" t="s">
         <v>1293</v>
       </c>
-      <c r="B401" s="5" t="s">
+      <c r="B402" s="5" t="s">
         <v>1294</v>
       </c>
     </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A402" s="1" t="s">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A403" s="1" t="s">
         <v>1292</v>
       </c>
-      <c r="B402" s="5" t="s">
+      <c r="B403" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A403" s="1" t="s">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A404" s="1" t="s">
         <v>1305</v>
       </c>
-      <c r="B403" s="5" t="s">
+      <c r="B404" s="5" t="s">
         <v>1306</v>
       </c>
     </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A404" s="1" t="s">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A405" s="1" t="s">
         <v>1302</v>
       </c>
-      <c r="B404" s="5" t="s">
+      <c r="B405" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A405" s="1" t="s">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A406" s="1" t="s">
         <v>1287</v>
       </c>
-      <c r="B405" s="5" t="s">
+      <c r="B406" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A406" s="1" t="s">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A407" s="1" t="s">
         <v>1300</v>
       </c>
-      <c r="B406" s="5" t="s">
+      <c r="B407" s="5" t="s">
         <v>1301</v>
       </c>
     </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A407" s="1" t="s">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A408" s="1" t="s">
         <v>1298</v>
       </c>
-      <c r="B407" s="5" t="s">
+      <c r="B408" s="5" t="s">
         <v>1299</v>
       </c>
     </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A408" s="1" t="s">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A409" s="1" t="s">
         <v>1289</v>
       </c>
-      <c r="B408" s="5" t="s">
+      <c r="B409" s="5" t="s">
         <v>1290</v>
       </c>
     </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A409" s="1" t="s">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A410" s="1" t="s">
         <v>1303</v>
       </c>
-      <c r="B409" s="5" t="s">
+      <c r="B410" s="5" t="s">
         <v>1304</v>
       </c>
     </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A410" s="1" t="s">
+    <row r="411" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A411" s="1" t="s">
         <v>1295</v>
       </c>
-      <c r="B410" s="5" t="s">
+      <c r="B411" s="5" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A411" s="1" t="s">
+    <row r="412" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A412" s="1" t="s">
         <v>1812</v>
       </c>
-      <c r="B411" s="5" t="s">
+      <c r="B412" s="5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A412" s="1" t="s">
+    <row r="413" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A413" s="1" t="s">
         <v>1291</v>
       </c>
-      <c r="B412" s="5" t="s">
+      <c r="B413" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A413" s="1" t="s">
+    <row r="414" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A414" s="1" t="s">
         <v>1296</v>
       </c>
-      <c r="B413" s="5" t="s">
+      <c r="B414" s="5" t="s">
         <v>1297</v>
       </c>
     </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A414" s="1" t="s">
+    <row r="415" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A415" s="1" t="s">
         <v>1288</v>
       </c>
-      <c r="B414" s="5" t="s">
+      <c r="B415" s="5" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A415" s="1" t="s">
+    <row r="416" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A416" s="1" t="s">
         <v>1777</v>
       </c>
-      <c r="B415" s="5" t="s">
+      <c r="B416" s="5" t="s">
         <v>1575</v>
-      </c>
-    </row>
-    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A416" s="9" t="s">
-        <v>2670</v>
-      </c>
-      <c r="B416" s="5" t="s">
-        <v>2669</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" s="9" t="s">
+        <v>2670</v>
+      </c>
+      <c r="B417" s="5" t="s">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A418" s="9" t="s">
         <v>2671</v>
       </c>
-      <c r="B417" s="5" t="s">
+      <c r="B418" s="5" t="s">
         <v>2768</v>
-      </c>
-    </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A418" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B418" s="5" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A419" s="1" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="B419" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C419" s="5" t="s">
-        <v>1790</v>
+        <v>179</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A420" s="1" t="s">
-        <v>531</v>
+        <v>190</v>
       </c>
       <c r="B420" s="5" t="s">
-        <v>532</v>
+        <v>191</v>
+      </c>
+      <c r="C420" s="5" t="s">
+        <v>1790</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A421" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B421" s="5" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A422" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B421" s="5" t="s">
+      <c r="B422" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C421" s="5" t="s">
+      <c r="C422" s="5" t="s">
         <v>1799</v>
       </c>
     </row>
@@ -18374,39 +18425,49 @@
   <sortState ref="A2:C446">
     <sortCondition ref="A2:A446"/>
   </sortState>
-  <conditionalFormatting sqref="A61:A135 A2:A59 A137:A318 A1303:A1048576">
-    <cfRule type="expression" dxfId="48" priority="12">
+  <conditionalFormatting sqref="A61:A135 A2:A59 A137:A279 A1304:A1048576 A281:A319">
+    <cfRule type="expression" dxfId="52" priority="14">
       <formula>AND( $A2 = "", OR( $B2 &lt;&gt; "", $C2 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C7 C61:C135 C9:C59 C137:C340 C345:C1048576">
-    <cfRule type="expression" dxfId="47" priority="4">
+  <conditionalFormatting sqref="C1:C7 C61:C135 C9:C59 C137:C279 C346:C1048576 C281:C341">
+    <cfRule type="expression" dxfId="51" priority="6">
       <formula>AND($B1 &lt;&gt; "", $C1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136">
-    <cfRule type="expression" dxfId="46" priority="3">
+    <cfRule type="expression" dxfId="50" priority="5">
       <formula>AND( $A136 = "", OR( $B136 &lt;&gt; "", $C136 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C136">
-    <cfRule type="expression" dxfId="45" priority="2">
+    <cfRule type="expression" dxfId="49" priority="4">
       <formula>AND($B136 &lt;&gt; "", $C136 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C341:C343">
-    <cfRule type="expression" dxfId="44" priority="29">
-      <formula>AND($B342 &lt;&gt; "", $C341 = "")</formula>
+  <conditionalFormatting sqref="C342:C344">
+    <cfRule type="expression" dxfId="48" priority="31">
+      <formula>AND($B343 &lt;&gt; "", $C342 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C344">
-    <cfRule type="expression" dxfId="43" priority="30">
-      <formula>AND(#REF! &lt;&gt; "", $C344 = "")</formula>
+  <conditionalFormatting sqref="C345">
+    <cfRule type="expression" dxfId="47" priority="32">
+      <formula>AND(#REF! &lt;&gt; "", $C345 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="42" priority="1">
+    <cfRule type="expression" dxfId="46" priority="3">
       <formula>AND($B8 &lt;&gt; "", $C8 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A280">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>AND( $A280 = "", OR( $B280 &lt;&gt; "", $C280 &lt;&gt; "" ) )</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C280">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>AND($B280 &lt;&gt; "", $C280 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -21967,17 +22028,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="41" priority="3">
+    <cfRule type="expression" dxfId="45" priority="3">
       <formula>AND($B2 = "", $C2 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="expression" dxfId="40" priority="2">
+    <cfRule type="expression" dxfId="44" priority="2">
       <formula>AND( $C2 = "", $B2 &lt;&gt; "" )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="expression" dxfId="39" priority="1">
+    <cfRule type="expression" dxfId="43" priority="1">
       <formula>AND( $A2 = "", OR( $B2 &lt;&gt; "", $C2 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35608,147 +35669,147 @@
     <sortCondition ref="A2:A1621"/>
   </sortState>
   <conditionalFormatting sqref="B35:B52 B987:B1216 B1535:B1553 B1555:B1048576">
-    <cfRule type="expression" dxfId="38" priority="35">
+    <cfRule type="expression" dxfId="42" priority="35">
       <formula>AND($B35 = "", $C35 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A987 A35:A52 A990:A1216 A1535:A1553 A1555:A1048576">
-    <cfRule type="expression" dxfId="37" priority="33">
+    <cfRule type="expression" dxfId="41" priority="33">
       <formula>AND( $A35 = "", OR( $B35 &lt;&gt; "", $C35 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B34">
-    <cfRule type="expression" dxfId="36" priority="32">
+    <cfRule type="expression" dxfId="40" priority="32">
       <formula>AND($B2 = "", $C2 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A34">
-    <cfRule type="expression" dxfId="35" priority="31">
+    <cfRule type="expression" dxfId="39" priority="31">
       <formula>AND( $A2 = "", OR( $B2 &lt;&gt; "", $C2 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53:B92">
-    <cfRule type="expression" dxfId="34" priority="28">
+    <cfRule type="expression" dxfId="38" priority="28">
       <formula>AND($B53 = "", $C53 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:A92">
-    <cfRule type="expression" dxfId="33" priority="27">
+    <cfRule type="expression" dxfId="37" priority="27">
       <formula>AND( $A53 = "", OR( $B53 &lt;&gt; "", $C53 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93:B362">
-    <cfRule type="expression" dxfId="32" priority="26">
+    <cfRule type="expression" dxfId="36" priority="26">
       <formula>AND($B93 = "", $C93 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93:A362">
-    <cfRule type="expression" dxfId="31" priority="25">
+    <cfRule type="expression" dxfId="35" priority="25">
       <formula>AND( $A93 = "", OR( $B93 &lt;&gt; "", $C93 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B363:B633">
-    <cfRule type="expression" dxfId="30" priority="24">
+    <cfRule type="expression" dxfId="34" priority="24">
       <formula>AND($B363 = "", $C363 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A363:A633">
-    <cfRule type="expression" dxfId="29" priority="22">
+    <cfRule type="expression" dxfId="33" priority="22">
       <formula>AND( $A363 = "", OR( $B363 &lt;&gt; "", $C363 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B634:B666">
-    <cfRule type="expression" dxfId="28" priority="21">
+    <cfRule type="expression" dxfId="32" priority="21">
       <formula>AND($B634 = "", $C634 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A634:A666">
-    <cfRule type="expression" dxfId="27" priority="19">
+    <cfRule type="expression" dxfId="31" priority="19">
       <formula>AND( $A634 = "", OR( $B634 &lt;&gt; "", $C634 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B667:B936">
-    <cfRule type="expression" dxfId="26" priority="18">
+    <cfRule type="expression" dxfId="30" priority="18">
       <formula>AND($B667 = "", $C667 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A667:A936">
-    <cfRule type="expression" dxfId="25" priority="17">
+    <cfRule type="expression" dxfId="29" priority="17">
       <formula>AND( $A667 = "", OR( $B667 &lt;&gt; "", $C667 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B937:B986">
-    <cfRule type="expression" dxfId="24" priority="16">
+    <cfRule type="expression" dxfId="28" priority="16">
       <formula>AND($B937 = "", $C937 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A937:A986">
-    <cfRule type="expression" dxfId="23" priority="14">
+    <cfRule type="expression" dxfId="27" priority="14">
       <formula>AND( $A937 = "", OR( $B937 &lt;&gt; "", $C937 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1216 C1535:C1553 C1555:C1048576">
-    <cfRule type="expression" dxfId="22" priority="13">
+    <cfRule type="expression" dxfId="26" priority="13">
       <formula>AND($B1 &lt;&gt; "", $C1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A989">
-    <cfRule type="expression" dxfId="21" priority="12">
+    <cfRule type="expression" dxfId="25" priority="12">
       <formula>AND( $A989 = "", OR( $B989 &lt;&gt; "", $C989 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A988">
-    <cfRule type="expression" dxfId="20" priority="11">
+    <cfRule type="expression" dxfId="24" priority="11">
       <formula>AND( $A988 = "", OR( $B988 &lt;&gt; "", $C988 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1217:B1340">
-    <cfRule type="expression" dxfId="19" priority="10">
+    <cfRule type="expression" dxfId="23" priority="10">
       <formula>AND($B1217 = "", $C1217 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1217:A1340">
-    <cfRule type="expression" dxfId="18" priority="9">
+    <cfRule type="expression" dxfId="22" priority="9">
       <formula>AND( $A1217 = "", OR( $B1217 &lt;&gt; "", $C1217 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1341:B1373">
-    <cfRule type="expression" dxfId="17" priority="8">
+    <cfRule type="expression" dxfId="21" priority="8">
       <formula>AND($B1341 = "", $C1341 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1341:A1373">
-    <cfRule type="expression" dxfId="16" priority="7">
+    <cfRule type="expression" dxfId="20" priority="7">
       <formula>AND( $A1341 = "", OR( $B1341 &lt;&gt; "", $C1341 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1374:B1534">
-    <cfRule type="expression" dxfId="15" priority="6">
+    <cfRule type="expression" dxfId="19" priority="6">
       <formula>AND($B1374 = "", $C1374 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1374:A1534">
-    <cfRule type="expression" dxfId="14" priority="5">
+    <cfRule type="expression" dxfId="18" priority="5">
       <formula>AND( $A1374 = "", OR( $B1374 &lt;&gt; "", $C1374 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1217:C1534">
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>AND($B1217 &lt;&gt; "", $C1217 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1554">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="16" priority="3">
       <formula>AND($B1554 = "", $C1554 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1554">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>AND( $A1554 = "", OR( $B1554 &lt;&gt; "", $C1554 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1554">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>AND($B1554 &lt;&gt; "", $C1554 = "")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -44205,7 +44266,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>AND($B1 &lt;&gt; "", $C1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -44589,32 +44650,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2 B7:B18 B20:B1048576">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="12" priority="9">
       <formula>AND($B2 = "", $C2 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2 C7:C1048576">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="11" priority="8">
       <formula>AND( $C2 = "", $B2 &lt;&gt; "" )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2 A7:A1048576">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>AND( $A2 = "", OR( $B2 &lt;&gt; "", $C2 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>AND($B3 = "", $C3 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C6">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>AND( $C3 = "", $B3 &lt;&gt; "" )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A6">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>AND( $A3 = "", OR( $B3 &lt;&gt; "", $C3 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
@@ -44664,17 +44725,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>AND($B2 = "", $C2 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>AND( $C2 = "", $B2 &lt;&gt; "" )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>AND( $A2 = "", OR( $B2 &lt;&gt; "", $C2 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Moved messages to excel
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7473" uniqueCount="4551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7483" uniqueCount="4561">
   <si>
     <t>fi</t>
   </si>
@@ -13708,6 +13708,36 @@
   </si>
   <si>
     <t>Tarkista tietosi ja täytä puuttuvat kentät. Voit myöhemmin muuttaa yhteystietojasi "omat tiedot" valikosta.</t>
+  </si>
+  <si>
+    <t>create.placeholder</t>
+  </si>
+  <si>
+    <t>Kasarmikatu 25, Helsinki</t>
+  </si>
+  <si>
+    <t>error.duplicate-person-id</t>
+  </si>
+  <si>
+    <t>error.duplicate-email</t>
+  </si>
+  <si>
+    <t>Sähköpostiosoitteella on jo rekisteröity. Voit tarvittaessa tilata uuden salasanan etusivun "Oletko unohtanut salasanasi"-linkistä</t>
+  </si>
+  <si>
+    <t>Henkilötunnuksella on jo rekisteröity. Voit tarvittaessa tilata uuden salasanan etusivun "Oletko unohtanut salasanasi"-linkistä</t>
+  </si>
+  <si>
+    <t>Käyttäjätunnuksen luominen epäonnistui. Ole hyvä ja yritä tunnistautumista uudelleen.</t>
+  </si>
+  <si>
+    <t>error.create-user</t>
+  </si>
+  <si>
+    <t>register.confirm-cancel</t>
+  </si>
+  <si>
+    <t>Haluatko varmasti keskeyttää rekisteröitymisen?</t>
   </si>
 </sst>
 </file>
@@ -14938,10 +14968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C423"/>
+  <dimension ref="A1:C428"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B358" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B370" sqref="B370"/>
+    <sheetView tabSelected="1" topLeftCell="A360" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B376" sqref="B376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -16729,1689 +16759,1729 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
-        <v>3565</v>
+        <v>4551</v>
       </c>
       <c r="B219" s="5" t="s">
-        <v>3566</v>
+        <v>4552</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
-        <v>3176</v>
+        <v>3565</v>
       </c>
       <c r="B220" s="5" t="s">
-        <v>3177</v>
+        <v>3566</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
-        <v>3174</v>
+        <v>3176</v>
       </c>
       <c r="B221" s="5" t="s">
-        <v>3175</v>
+        <v>3177</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
-        <v>559</v>
+        <v>3174</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>353</v>
+        <v>3175</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
-        <v>546</v>
+        <v>559</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>376</v>
+        <v>353</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>552</v>
+        <v>365</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>357</v>
+        <v>552</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>558</v>
+        <v>373</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
-        <v>549</v>
+        <v>557</v>
       </c>
       <c r="B229" s="5" t="s">
-        <v>371</v>
+        <v>558</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B230" s="5" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="B231" s="5" t="s">
-        <v>554</v>
+        <v>359</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
-        <v>315</v>
+        <v>555</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>316</v>
+        <v>556</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
-        <v>210</v>
+        <v>315</v>
       </c>
       <c r="B234" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C234" s="5" t="s">
-        <v>1800</v>
+        <v>316</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
-        <v>1378</v>
+        <v>210</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>1379</v>
+        <v>211</v>
+      </c>
+      <c r="C235" s="5" t="s">
+        <v>1800</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B236" s="4" t="s">
-        <v>13</v>
+        <v>1378</v>
+      </c>
+      <c r="B236" s="5" t="s">
+        <v>1379</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B237" s="5" t="s">
-        <v>263</v>
+        <v>12</v>
+      </c>
+      <c r="B237" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
-        <v>3593</v>
+        <v>262</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>3594</v>
+        <v>263</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
-        <v>3586</v>
+        <v>3593</v>
       </c>
       <c r="B239" s="5" t="s">
-        <v>3587</v>
+        <v>3594</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
-        <v>3589</v>
+        <v>3586</v>
       </c>
       <c r="B240" s="5" t="s">
-        <v>3590</v>
+        <v>3587</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
-        <v>3591</v>
+        <v>3589</v>
       </c>
       <c r="B241" s="5" t="s">
-        <v>3592</v>
+        <v>3590</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
-        <v>230</v>
+        <v>3591</v>
       </c>
       <c r="B242" s="5" t="s">
-        <v>231</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B243" s="5" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
       <c r="B244" s="5" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B245" s="5" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="B247" s="5" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="B248" s="5" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="B249" s="5" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B251" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="B252" s="5" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="B253" s="5" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B256" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A257" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B256" s="5" t="s">
+      <c r="B257" s="5" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A257" s="1" t="s">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A258" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B257" s="5" t="s">
+      <c r="B258" s="5" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A258" s="1" t="s">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A259" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B258" s="5" t="s">
+      <c r="B259" s="5" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A259" s="1" t="s">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A260" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B259" s="5" t="s">
+      <c r="B260" s="5" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A260" s="1" t="s">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A261" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B260" s="5" t="s">
+      <c r="B261" s="5" t="s">
         <v>4544</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A261" s="1" t="s">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A262" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B261" s="5" t="s">
+      <c r="B262" s="5" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A262" s="1" t="s">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A263" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B262" s="5" t="s">
+      <c r="B263" s="5" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A263" s="1" t="s">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A264" s="1" t="s">
+        <v>4558</v>
+      </c>
+      <c r="B264" s="5" t="s">
+        <v>4557</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A265" s="1" t="s">
+        <v>4553</v>
+      </c>
+      <c r="B265" s="5" t="s">
+        <v>4556</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A266" s="1" t="s">
+        <v>4554</v>
+      </c>
+      <c r="B266" s="5" t="s">
+        <v>4555</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A267" s="1" t="s">
         <v>2798</v>
       </c>
-      <c r="B263" s="5" t="s">
+      <c r="B267" s="5" t="s">
         <v>2799</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A264" s="1" t="s">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A268" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B264" s="5" t="s">
+      <c r="B268" s="5" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A265" s="1" t="s">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A269" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B265" s="5" t="s">
+      <c r="B269" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A266" s="1" t="s">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A270" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B266" s="5" t="s">
+      <c r="B270" s="5" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A267" s="1" t="s">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A271" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B267" s="5" t="s">
+      <c r="B271" s="5" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A268" s="1" t="s">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A272" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B268" s="5" t="s">
+      <c r="B272" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A269" s="1" t="s">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A273" s="1" t="s">
         <v>1795</v>
       </c>
-      <c r="B269" s="5" t="s">
+      <c r="B273" s="5" t="s">
         <v>1796</v>
       </c>
-      <c r="C269" s="5" t="s">
+      <c r="C273" s="5" t="s">
         <v>1796</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A270" s="1" t="s">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A274" s="1" t="s">
         <v>1774</v>
       </c>
-      <c r="B270" s="5" t="s">
+      <c r="B274" s="5" t="s">
         <v>1775</v>
       </c>
-      <c r="C270" s="5" t="s">
+      <c r="C274" s="5" t="s">
         <v>1775</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A271" s="1" t="s">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A275" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B271" s="4" t="s">
+      <c r="B275" s="4" t="s">
         <v>2725</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A272" s="1" t="s">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A276" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B272" s="5" t="s">
+      <c r="B276" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A273" s="1" t="s">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A277" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B273" s="5" t="s">
+      <c r="B277" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A274" s="1" t="s">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A278" s="1" t="s">
         <v>2580</v>
       </c>
-      <c r="B274" s="5" t="s">
+      <c r="B278" s="5" t="s">
         <v>2581</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A275" s="1" t="s">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A279" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B275" s="5" t="s">
+      <c r="B279" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A276" s="1" t="s">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A280" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B276" s="5" t="s">
+      <c r="B280" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A277" s="1" t="s">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A281" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B277" s="5" t="s">
+      <c r="B281" s="5" t="s">
         <v>2723</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A278" s="1" t="s">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A282" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B278" s="5" t="s">
+      <c r="B282" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A279" s="1" t="s">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A283" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B279" s="5" t="s">
+      <c r="B283" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A280" s="1" t="s">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A284" s="1" t="s">
         <v>1310</v>
       </c>
-      <c r="B280" s="5" t="s">
+      <c r="B284" s="5" t="s">
         <v>1311</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A281" s="1" t="s">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A285" s="1" t="s">
         <v>4546</v>
       </c>
-      <c r="B281" s="5" t="s">
+      <c r="B285" s="5" t="s">
         <v>1309</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A282" s="1" t="s">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A286" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B282" s="5" t="s">
+      <c r="B286" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A283" s="1" t="s">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A287" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B283" s="5" t="s">
+      <c r="B287" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A284" s="1" t="s">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A288" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B284" s="5" t="s">
+      <c r="B288" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A285" s="1" t="s">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A289" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="B285" s="5" t="s">
+      <c r="B289" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A286" s="1" t="s">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A290" s="1" t="s">
         <v>3568</v>
       </c>
-      <c r="B286" s="5" t="s">
+      <c r="B290" s="5" t="s">
         <v>3569</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A287" s="1" t="s">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A291" s="1" t="s">
         <v>3585</v>
       </c>
-      <c r="B287" s="5" t="s">
+      <c r="B291" s="5" t="s">
         <v>3588</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A288" s="1" t="s">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A292" s="1" t="s">
         <v>3583</v>
       </c>
-      <c r="B288" s="5" t="s">
+      <c r="B292" s="5" t="s">
         <v>3584</v>
-      </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A289" s="9" t="s">
-        <v>2665</v>
-      </c>
-      <c r="B289" s="5" t="s">
-        <v>2663</v>
-      </c>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A290" s="9" t="s">
-        <v>2676</v>
-      </c>
-      <c r="B290" s="5" t="s">
-        <v>2697</v>
-      </c>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A291" s="9" t="s">
-        <v>2685</v>
-      </c>
-      <c r="B291" s="5" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A292" s="9" t="s">
-        <v>2693</v>
-      </c>
-      <c r="B292" s="5" t="s">
-        <v>2704</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="9" t="s">
-        <v>2675</v>
+        <v>2665</v>
       </c>
       <c r="B293" s="5" t="s">
-        <v>2696</v>
+        <v>2663</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="9" t="s">
-        <v>2690</v>
+        <v>2676</v>
       </c>
       <c r="B294" s="5" t="s">
-        <v>2703</v>
+        <v>2697</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="9" t="s">
-        <v>2692</v>
+        <v>2685</v>
       </c>
       <c r="B295" s="5" t="s">
-        <v>2787</v>
+        <v>310</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" s="9" t="s">
-        <v>2674</v>
+        <v>2693</v>
       </c>
       <c r="B296" s="5" t="s">
-        <v>2695</v>
+        <v>2704</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" s="9" t="s">
-        <v>2672</v>
+        <v>2675</v>
       </c>
       <c r="B297" s="5" t="s">
-        <v>2673</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A298" s="1" t="s">
-        <v>184</v>
+        <v>2696</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298" s="9" t="s">
+        <v>2690</v>
       </c>
       <c r="B298" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A299" s="1" t="s">
-        <v>186</v>
+        <v>2703</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" s="9" t="s">
+        <v>2692</v>
       </c>
       <c r="B299" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A300" s="1" t="s">
-        <v>260</v>
+        <v>2787</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" s="9" t="s">
+        <v>2674</v>
       </c>
       <c r="B300" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="C300" s="5" t="s">
-        <v>1791</v>
+        <v>2695</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="9" t="s">
+        <v>2672</v>
+      </c>
+      <c r="B301" s="5" t="s">
+        <v>2673</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A302" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B302" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A303" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B303" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A304" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B304" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C304" s="5" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A305" s="9" t="s">
         <v>2683</v>
       </c>
-      <c r="B301" s="5" t="s">
+      <c r="B305" s="5" t="s">
         <v>2778</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A302" s="9" t="s">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A306" s="9" t="s">
         <v>2691</v>
       </c>
-      <c r="B302" s="5" t="s">
+      <c r="B306" s="5" t="s">
         <v>2787</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A303" s="9" t="s">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A307" s="9" t="s">
         <v>2677</v>
       </c>
-      <c r="B303" s="5" t="s">
+      <c r="B307" s="5" t="s">
         <v>2707</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A304" s="9" t="s">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A308" s="9" t="s">
         <v>2682</v>
       </c>
-      <c r="B304" s="5" t="s">
+      <c r="B308" s="5" t="s">
         <v>2699</v>
-      </c>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A305" s="1" t="s">
-        <v>1337</v>
-      </c>
-      <c r="B305" s="5" t="s">
-        <v>1338</v>
-      </c>
-    </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A306" s="1" t="s">
-        <v>3573</v>
-      </c>
-      <c r="B306" s="5" t="s">
-        <v>3574</v>
-      </c>
-    </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A307" s="1" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B307" s="5" t="s">
-        <v>1340</v>
-      </c>
-    </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A308" s="1" t="s">
-        <v>1341</v>
-      </c>
-      <c r="B308" s="5" t="s">
-        <v>1342</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309" s="1" t="s">
-        <v>3570</v>
+        <v>1337</v>
       </c>
       <c r="B309" s="5" t="s">
-        <v>3571</v>
-      </c>
-    </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A310" s="9" t="s">
-        <v>2684</v>
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A310" s="1" t="s">
+        <v>3573</v>
       </c>
       <c r="B310" s="5" t="s">
-        <v>2701</v>
-      </c>
-    </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A311" s="9" t="s">
-        <v>2689</v>
+        <v>3574</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A311" s="1" t="s">
+        <v>1339</v>
       </c>
       <c r="B311" s="5" t="s">
-        <v>2721</v>
-      </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A312" s="9" t="s">
-        <v>2686</v>
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A312" s="1" t="s">
+        <v>1341</v>
       </c>
       <c r="B312" s="5" t="s">
-        <v>2702</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A313" s="1" t="s">
-        <v>1317</v>
+        <v>3570</v>
       </c>
       <c r="B313" s="5" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A314" s="1" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B314" s="6" t="s">
-        <v>1787</v>
-      </c>
-      <c r="C314" s="6" t="s">
-        <v>1787</v>
-      </c>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A315" s="1" t="s">
-        <v>1314</v>
+        <v>3571</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A314" s="9" t="s">
+        <v>2684</v>
+      </c>
+      <c r="B314" s="5" t="s">
+        <v>2701</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A315" s="9" t="s">
+        <v>2689</v>
       </c>
       <c r="B315" s="5" t="s">
-        <v>2824</v>
-      </c>
-    </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A316" s="1" t="s">
-        <v>1315</v>
+        <v>2721</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A316" s="9" t="s">
+        <v>2686</v>
       </c>
       <c r="B316" s="5" t="s">
-        <v>1316</v>
+        <v>2702</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A317" s="1" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="B317" s="5" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A318" s="1" t="s">
-        <v>1325</v>
-      </c>
-      <c r="B318" s="5" t="s">
-        <v>1326</v>
+        <v>1314</v>
+      </c>
+      <c r="B318" s="6" t="s">
+        <v>1787</v>
+      </c>
+      <c r="C318" s="6" t="s">
+        <v>1787</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A319" s="1" t="s">
-        <v>1329</v>
+        <v>1314</v>
       </c>
       <c r="B319" s="5" t="s">
-        <v>1330</v>
+        <v>2824</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A320" s="1" t="s">
-        <v>1327</v>
+        <v>1315</v>
       </c>
       <c r="B320" s="5" t="s">
-        <v>1328</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A321" s="1" t="s">
-        <v>1323</v>
+        <v>1319</v>
       </c>
       <c r="B321" s="5" t="s">
-        <v>1324</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322" s="1" t="s">
-        <v>1321</v>
+        <v>1325</v>
       </c>
       <c r="B322" s="5" t="s">
-        <v>1322</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A323" s="1" t="s">
-        <v>1312</v>
+        <v>1329</v>
       </c>
       <c r="B323" s="5" t="s">
-        <v>1313</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A324" s="1" t="s">
-        <v>3178</v>
+        <v>1327</v>
       </c>
       <c r="B324" s="5" t="s">
-        <v>3179</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A325" s="1" t="s">
-        <v>560</v>
+        <v>1323</v>
       </c>
       <c r="B325" s="5" t="s">
-        <v>561</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A326" s="1" t="s">
-        <v>364</v>
+        <v>1321</v>
       </c>
       <c r="B326" s="5" t="s">
-        <v>365</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A327" s="1" t="s">
-        <v>2583</v>
+        <v>1312</v>
       </c>
       <c r="B327" s="5" t="s">
-        <v>2717</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A328" s="1" t="s">
-        <v>372</v>
+        <v>3178</v>
       </c>
       <c r="B328" s="5" t="s">
-        <v>2765</v>
+        <v>3179</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A329" s="1" t="s">
-        <v>356</v>
+        <v>560</v>
       </c>
       <c r="B329" s="5" t="s">
-        <v>357</v>
+        <v>561</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A330" s="1" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="B330" s="5" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A331" s="1" t="s">
-        <v>366</v>
+        <v>2583</v>
       </c>
       <c r="B331" s="5" t="s">
-        <v>367</v>
+        <v>2717</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A332" s="1" t="s">
-        <v>352</v>
+        <v>372</v>
       </c>
       <c r="B332" s="5" t="s">
-        <v>2720</v>
+        <v>2765</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A333" s="1" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B333" s="5" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A334" s="1" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="B334" s="5" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A335" s="1" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="B335" s="5" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A336" s="1" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B336" s="5" t="s">
-        <v>351</v>
+        <v>2720</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A337" s="1" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="B337" s="5" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A338" s="1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B338" s="5" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A339" s="1" t="s">
-        <v>2821</v>
+        <v>360</v>
       </c>
       <c r="B339" s="5" t="s">
-        <v>2662</v>
+        <v>361</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A340" s="1" t="s">
-        <v>2768</v>
-      </c>
-      <c r="B340" s="4" t="s">
-        <v>2769</v>
-      </c>
-      <c r="C340" s="5" t="s">
-        <v>2771</v>
+        <v>350</v>
+      </c>
+      <c r="B340" s="5" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A341" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B341" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C341" s="5" t="s">
-        <v>1789</v>
+        <v>358</v>
+      </c>
+      <c r="B341" s="5" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A342" s="1" t="s">
-        <v>562</v>
+        <v>368</v>
       </c>
       <c r="B342" s="5" t="s">
-        <v>563</v>
+        <v>369</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A343" s="1" t="s">
-        <v>264</v>
+        <v>2821</v>
       </c>
       <c r="B343" s="5" t="s">
-        <v>265</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A344" s="1" t="s">
-        <v>3567</v>
-      </c>
-      <c r="B344" s="5" t="s">
-        <v>395</v>
+        <v>2768</v>
+      </c>
+      <c r="B344" s="4" t="s">
+        <v>2769</v>
+      </c>
+      <c r="C344" s="5" t="s">
+        <v>2771</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A345" s="1" t="s">
-        <v>3563</v>
-      </c>
-      <c r="B345" s="5" t="s">
-        <v>3564</v>
+        <v>14</v>
+      </c>
+      <c r="B345" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C345" s="5" t="s">
+        <v>1789</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A346" s="1" t="s">
-        <v>533</v>
+        <v>562</v>
       </c>
       <c r="B346" s="5" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A347" s="9" t="s">
-        <v>2679</v>
+        <v>563</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A347" s="1" t="s">
+        <v>264</v>
       </c>
       <c r="B347" s="5" t="s">
-        <v>2722</v>
+        <v>265</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A348" s="1" t="s">
-        <v>1002</v>
+        <v>3567</v>
       </c>
       <c r="B348" s="5" t="s">
-        <v>1003</v>
+        <v>395</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A349" s="1" t="s">
-        <v>564</v>
+        <v>3563</v>
       </c>
       <c r="B349" s="5" t="s">
-        <v>387</v>
+        <v>3564</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A350" s="1" t="s">
-        <v>1776</v>
+        <v>533</v>
       </c>
       <c r="B350" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A351" s="1" t="s">
-        <v>3575</v>
+        <v>534</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A351" s="9" t="s">
+        <v>2679</v>
       </c>
       <c r="B351" s="5" t="s">
-        <v>3576</v>
+        <v>2722</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A352" s="1" t="s">
-        <v>1811</v>
+        <v>1002</v>
       </c>
       <c r="B352" s="5" t="s">
-        <v>416</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A353" s="1" t="s">
-        <v>2775</v>
-      </c>
-      <c r="B353" s="4" t="s">
-        <v>2770</v>
-      </c>
-      <c r="C353" s="5" t="s">
-        <v>2772</v>
-      </c>
-    </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A354" s="9" t="s">
-        <v>2694</v>
+        <v>564</v>
+      </c>
+      <c r="B353" s="5" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A354" s="1" t="s">
+        <v>1776</v>
       </c>
       <c r="B354" s="5" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A355" s="9" t="s">
-        <v>2688</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A355" s="1" t="s">
+        <v>3575</v>
       </c>
       <c r="B355" s="5" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A356" s="9" t="s">
-        <v>2666</v>
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A356" s="1" t="s">
+        <v>1811</v>
       </c>
       <c r="B356" s="5" t="s">
-        <v>2664</v>
+        <v>416</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A357" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B357" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A358" s="1" t="s">
-        <v>3577</v>
+        <v>2775</v>
+      </c>
+      <c r="B357" s="4" t="s">
+        <v>2770</v>
+      </c>
+      <c r="C357" s="5" t="s">
+        <v>2772</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A358" s="9" t="s">
+        <v>2694</v>
       </c>
       <c r="B358" s="5" t="s">
-        <v>3578</v>
-      </c>
-    </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A359" s="1" t="s">
-        <v>3579</v>
+        <v>311</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A359" s="9" t="s">
+        <v>2688</v>
       </c>
       <c r="B359" s="5" t="s">
-        <v>3580</v>
-      </c>
-    </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A360" s="1" t="s">
-        <v>2796</v>
+        <v>308</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A360" s="9" t="s">
+        <v>2666</v>
       </c>
       <c r="B360" s="5" t="s">
-        <v>2797</v>
+        <v>2664</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A361" s="1" t="s">
-        <v>2810</v>
+        <v>37</v>
       </c>
       <c r="B361" s="5" t="s">
-        <v>2809</v>
+        <v>38</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A362" s="1" t="s">
-        <v>2811</v>
+        <v>3577</v>
       </c>
       <c r="B362" s="5" t="s">
-        <v>2812</v>
+        <v>3578</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A363" s="1" t="s">
-        <v>2803</v>
+        <v>3579</v>
       </c>
       <c r="B363" s="5" t="s">
-        <v>2800</v>
+        <v>3580</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A364" s="1" t="s">
-        <v>2804</v>
+        <v>2796</v>
       </c>
       <c r="B364" s="5" t="s">
-        <v>2801</v>
+        <v>2797</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A365" s="1" t="s">
-        <v>2805</v>
+        <v>2810</v>
       </c>
       <c r="B365" s="5" t="s">
-        <v>2802</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A366" s="1" t="s">
-        <v>2792</v>
+        <v>2811</v>
       </c>
       <c r="B366" s="5" t="s">
-        <v>2793</v>
+        <v>2812</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A367" s="1" t="s">
-        <v>2794</v>
+        <v>2803</v>
       </c>
       <c r="B367" s="5" t="s">
-        <v>2795</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A368" s="1" t="s">
+        <v>2804</v>
+      </c>
+      <c r="B368" s="5" t="s">
+        <v>2801</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A369" s="1" t="s">
+        <v>2805</v>
+      </c>
+      <c r="B369" s="5" t="s">
+        <v>2802</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A370" s="1" t="s">
+        <v>2792</v>
+      </c>
+      <c r="B370" s="5" t="s">
+        <v>2793</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A371" s="1" t="s">
+        <v>2794</v>
+      </c>
+      <c r="B371" s="5" t="s">
+        <v>2795</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A372" s="1" t="s">
         <v>2788</v>
       </c>
-      <c r="B368" s="5" t="s">
+      <c r="B372" s="5" t="s">
         <v>2789</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A369" s="1" t="s">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A373" s="1" t="s">
         <v>2791</v>
       </c>
-      <c r="B369" s="5" t="s">
+      <c r="B373" s="5" t="s">
         <v>2790</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A370" s="1" t="s">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A374" s="1" t="s">
         <v>2806</v>
       </c>
-      <c r="B370" s="5" t="s">
+      <c r="B374" s="5" t="s">
         <v>4550</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A371" s="1" t="s">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A375" s="1" t="s">
         <v>2808</v>
       </c>
-      <c r="B371" s="5" t="s">
+      <c r="B375" s="5" t="s">
         <v>2807</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A372" s="1" t="s">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A376" s="1" t="s">
+        <v>4559</v>
+      </c>
+      <c r="B376" s="5" t="s">
+        <v>4560</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A377" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B372" s="5" t="s">
+      <c r="B377" s="5" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A373" s="1" t="s">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A378" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="B373" s="5" t="s">
+      <c r="B378" s="5" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A374" s="1" t="s">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A379" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="B374" s="5" t="s">
+      <c r="B379" s="5" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A375" s="1" t="s">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A380" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="B375" s="5" t="s">
+      <c r="B380" s="5" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A376" s="1" t="s">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A381" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="B376" s="5" t="s">
+      <c r="B381" s="5" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A377" s="1" t="s">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A382" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="B377" s="5" t="s">
+      <c r="B382" s="5" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A378" s="1" t="s">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A383" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="B378" s="5" t="s">
+      <c r="B383" s="5" t="s">
         <v>2662</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A379" s="1" t="s">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A384" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="B379" s="5" t="s">
+      <c r="B384" s="5" t="s">
         <v>379</v>
-      </c>
-    </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A380" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="B380" s="5" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A381" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="B381" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A382" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B382" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A383" s="1" t="s">
-        <v>1381</v>
-      </c>
-      <c r="B383" s="5" t="s">
-        <v>1382</v>
-      </c>
-      <c r="C383" s="5" t="s">
-        <v>1794</v>
-      </c>
-    </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A384" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B384" s="5" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A385" s="1" t="s">
-        <v>212</v>
+        <v>375</v>
       </c>
       <c r="B385" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="C385" s="5" t="s">
-        <v>1801</v>
+        <v>376</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A386" s="1" t="s">
-        <v>3169</v>
+        <v>374</v>
       </c>
       <c r="B386" s="5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A387" s="1" t="s">
-        <v>3173</v>
+        <v>188</v>
       </c>
       <c r="B387" s="5" t="s">
-        <v>544</v>
+        <v>189</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A388" s="1" t="s">
-        <v>3165</v>
+        <v>1381</v>
       </c>
       <c r="B388" s="5" t="s">
-        <v>3166</v>
+        <v>1382</v>
+      </c>
+      <c r="C388" s="5" t="s">
+        <v>1794</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A389" s="1" t="s">
-        <v>3171</v>
+        <v>206</v>
       </c>
       <c r="B389" s="5" t="s">
-        <v>3172</v>
+        <v>207</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A390" s="1" t="s">
-        <v>3170</v>
+        <v>212</v>
       </c>
       <c r="B390" s="5" t="s">
-        <v>177</v>
+        <v>213</v>
+      </c>
+      <c r="C390" s="5" t="s">
+        <v>1801</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A391" s="1" t="s">
-        <v>3167</v>
+        <v>3169</v>
       </c>
       <c r="B391" s="5" t="s">
-        <v>3168</v>
+        <v>7</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A392" s="1" t="s">
-        <v>304</v>
+        <v>3173</v>
       </c>
       <c r="B392" s="5" t="s">
-        <v>305</v>
+        <v>544</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A393" s="1" t="s">
-        <v>1281</v>
+        <v>3165</v>
       </c>
       <c r="B393" s="5" t="s">
-        <v>1282</v>
+        <v>3166</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A394" s="1" t="s">
-        <v>1308</v>
+        <v>3171</v>
       </c>
       <c r="B394" s="5" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A395" s="9" t="s">
-        <v>2678</v>
+        <v>3172</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A395" s="1" t="s">
+        <v>3170</v>
       </c>
       <c r="B395" s="5" t="s">
-        <v>2698</v>
+        <v>177</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A396" s="7" t="s">
-        <v>1816</v>
+      <c r="A396" s="1" t="s">
+        <v>3167</v>
       </c>
       <c r="B396" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="C396" s="5" t="s">
-        <v>314</v>
+        <v>3168</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A397" s="1" t="s">
-        <v>1778</v>
+        <v>304</v>
       </c>
       <c r="B397" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C397" s="5" t="s">
-        <v>1798</v>
+        <v>305</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A398" s="1" t="s">
-        <v>1779</v>
+        <v>1281</v>
       </c>
       <c r="B398" s="5" t="s">
-        <v>1780</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A399" s="1" t="s">
-        <v>3201</v>
+        <v>1308</v>
       </c>
       <c r="B399" s="5" t="s">
-        <v>3202</v>
-      </c>
-    </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A400" s="1" t="s">
-        <v>182</v>
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A400" s="9" t="s">
+        <v>2678</v>
       </c>
       <c r="B400" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C400" s="5" t="s">
-        <v>183</v>
+        <v>2698</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A401" s="1" t="s">
-        <v>180</v>
+      <c r="A401" s="7" t="s">
+        <v>1816</v>
       </c>
       <c r="B401" s="5" t="s">
-        <v>181</v>
+        <v>314</v>
       </c>
       <c r="C401" s="5" t="s">
-        <v>181</v>
+        <v>314</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A402" s="1" t="s">
-        <v>1293</v>
+        <v>1778</v>
       </c>
       <c r="B402" s="5" t="s">
-        <v>1294</v>
+        <v>199</v>
+      </c>
+      <c r="C402" s="5" t="s">
+        <v>1798</v>
       </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A403" s="1" t="s">
-        <v>1292</v>
+        <v>1779</v>
       </c>
       <c r="B403" s="5" t="s">
-        <v>118</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A404" s="1" t="s">
-        <v>1305</v>
+        <v>3201</v>
       </c>
       <c r="B404" s="5" t="s">
-        <v>4549</v>
+        <v>3202</v>
       </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A405" s="1" t="s">
-        <v>4547</v>
+        <v>182</v>
       </c>
       <c r="B405" s="5" t="s">
-        <v>103</v>
+        <v>183</v>
+      </c>
+      <c r="C405" s="5" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A406" s="1" t="s">
-        <v>1302</v>
+        <v>180</v>
       </c>
       <c r="B406" s="5" t="s">
-        <v>101</v>
+        <v>181</v>
+      </c>
+      <c r="C406" s="5" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A407" s="1" t="s">
-        <v>1287</v>
+        <v>1293</v>
       </c>
       <c r="B407" s="5" t="s">
-        <v>105</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A408" s="1" t="s">
-        <v>1300</v>
+        <v>1292</v>
       </c>
       <c r="B408" s="5" t="s">
-        <v>1301</v>
+        <v>118</v>
       </c>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A409" s="1" t="s">
-        <v>1298</v>
+        <v>1305</v>
       </c>
       <c r="B409" s="5" t="s">
-        <v>1299</v>
+        <v>4549</v>
       </c>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A410" s="1" t="s">
-        <v>1289</v>
+        <v>4547</v>
       </c>
       <c r="B410" s="5" t="s">
-        <v>1290</v>
+        <v>103</v>
       </c>
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A411" s="1" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="B411" s="5" t="s">
-        <v>1304</v>
+        <v>101</v>
       </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A412" s="1" t="s">
-        <v>1295</v>
+        <v>1287</v>
       </c>
       <c r="B412" s="5" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A413" s="1" t="s">
-        <v>1812</v>
+        <v>1300</v>
       </c>
       <c r="B413" s="5" t="s">
-        <v>171</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A414" s="1" t="s">
-        <v>1291</v>
+        <v>1298</v>
       </c>
       <c r="B414" s="5" t="s">
-        <v>114</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A415" s="1" t="s">
-        <v>1296</v>
+        <v>1289</v>
       </c>
       <c r="B415" s="5" t="s">
-        <v>1297</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A416" s="1" t="s">
-        <v>1288</v>
+        <v>1303</v>
       </c>
       <c r="B416" s="5" t="s">
-        <v>116</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A417" s="1" t="s">
-        <v>1777</v>
+        <v>1295</v>
       </c>
       <c r="B417" s="5" t="s">
-        <v>1575</v>
-      </c>
-    </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A418" s="9" t="s">
-        <v>2670</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A418" s="1" t="s">
+        <v>1812</v>
       </c>
       <c r="B418" s="5" t="s">
-        <v>2669</v>
-      </c>
-    </row>
-    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A419" s="9" t="s">
-        <v>2671</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A419" s="1" t="s">
+        <v>1291</v>
       </c>
       <c r="B419" s="5" t="s">
-        <v>2767</v>
+        <v>114</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A420" s="1" t="s">
-        <v>178</v>
+        <v>1296</v>
       </c>
       <c r="B420" s="5" t="s">
-        <v>179</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A421" s="1" t="s">
-        <v>190</v>
+        <v>1288</v>
       </c>
       <c r="B421" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C421" s="5" t="s">
-        <v>1790</v>
+        <v>116</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A422" s="1" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B422" s="5" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="423" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A423" s="9" t="s">
+        <v>2670</v>
+      </c>
+      <c r="B423" s="5" t="s">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="424" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A424" s="9" t="s">
+        <v>2671</v>
+      </c>
+      <c r="B424" s="5" t="s">
+        <v>2767</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A425" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B425" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A426" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B426" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C426" s="5" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A427" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="B422" s="5" t="s">
+      <c r="B427" s="5" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="423" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A423" s="1" t="s">
+    <row r="428" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A428" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B423" s="5" t="s">
+      <c r="B428" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C423" s="5" t="s">
+      <c r="C428" s="5" t="s">
         <v>1799</v>
       </c>
     </row>
@@ -18419,12 +18489,12 @@
   <sortState ref="A2:C446">
     <sortCondition ref="A2:A446"/>
   </sortState>
-  <conditionalFormatting sqref="A61:A135 A2:A59 A137:A279 A281:A319 A1305:A1048576">
+  <conditionalFormatting sqref="A61:A135 A2:A59 A137:A283 A285:A323 A1310:A1048576">
     <cfRule type="expression" dxfId="50" priority="14">
       <formula>AND( $A2 = "", OR( $B2 &lt;&gt; "", $C2 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C7 C61:C135 C9:C59 C137:C279 C281:C341 C346:C1048576">
+  <conditionalFormatting sqref="C1:C7 C61:C135 C9:C59 C137:C283 C285:C345 C350:C1048576">
     <cfRule type="expression" dxfId="49" priority="6">
       <formula>AND($B1 &lt;&gt; "", $C1 = "")</formula>
     </cfRule>
@@ -18439,14 +18509,14 @@
       <formula>AND($B136 &lt;&gt; "", $C136 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C342:C344">
+  <conditionalFormatting sqref="C346:C348">
     <cfRule type="expression" dxfId="46" priority="31">
-      <formula>AND($B343 &lt;&gt; "", $C342 = "")</formula>
+      <formula>AND($B347 &lt;&gt; "", $C346 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C345">
+  <conditionalFormatting sqref="C349">
     <cfRule type="expression" dxfId="45" priority="32">
-      <formula>AND(#REF! &lt;&gt; "", $C345 = "")</formula>
+      <formula>AND(#REF! &lt;&gt; "", $C349 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
@@ -18454,14 +18524,14 @@
       <formula>AND($B8 &lt;&gt; "", $C8 = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A280">
+  <conditionalFormatting sqref="A284">
     <cfRule type="expression" dxfId="43" priority="2">
-      <formula>AND( $A280 = "", OR( $B280 &lt;&gt; "", $C280 &lt;&gt; "" ) )</formula>
+      <formula>AND( $A284 = "", OR( $B284 &lt;&gt; "", $C284 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C280">
+  <conditionalFormatting sqref="C284">
     <cfRule type="expression" dxfId="42" priority="1">
-      <formula>AND($B280 &lt;&gt; "", $C280 = "")</formula>
+      <formula>AND($B284 &lt;&gt; "", $C284 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Saturday night's lost focus. added error nad saved indicators to form inputs
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7491" uniqueCount="4568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7497" uniqueCount="4574">
   <si>
     <t>fi</t>
   </si>
@@ -13759,6 +13759,24 @@
   </si>
   <si>
     <t xml:space="preserve">Ole hyvä, tarkista tietosi ja täytä puuttuvat kentät. </t>
+  </si>
+  <si>
+    <t>form.err</t>
+  </si>
+  <si>
+    <t>form.warn</t>
+  </si>
+  <si>
+    <t>form.saved</t>
+  </si>
+  <si>
+    <t>Tallennettu</t>
+  </si>
+  <si>
+    <t>Virhe tallennuksessa</t>
+  </si>
+  <si>
+    <t>Virheellinen arvo</t>
   </si>
 </sst>
 </file>
@@ -14989,10 +15007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C432"/>
+  <dimension ref="A1:C435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A342" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B374" sqref="B374"/>
+    <sheetView tabSelected="1" topLeftCell="A391" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B440" sqref="B440"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
@@ -18536,6 +18554,30 @@
       </c>
       <c r="B432" s="5" t="s">
         <v>4559</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A433" s="1" t="s">
+        <v>4568</v>
+      </c>
+      <c r="B433" s="5" t="s">
+        <v>4572</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A434" s="1" t="s">
+        <v>4569</v>
+      </c>
+      <c r="B434" s="5" t="s">
+        <v>4573</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A435" s="1" t="s">
+        <v>4570</v>
+      </c>
+      <c r="B435" s="5" t="s">
+        <v>4571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kuvaamasi toimenpide vaatii yleensä luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="156" yWindow="0" windowWidth="29664" windowHeight="14616" tabRatio="500"/>
+    <workbookView xWindow="156" yWindow="0" windowWidth="29664" windowHeight="14616" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7584" uniqueCount="4643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7584" uniqueCount="4644">
   <si>
     <t>fi</t>
   </si>
@@ -13985,6 +13985,9 @@
   <si>
     <t xml:space="preserve">Esimerkkejä hyvistä kuvauksista: Omakotitalo - Rakennetaan kaksikerroksinen, puuverhoiltu omakotitalo ja talousrakennus sekä maalämpökaivo; Rivitalo - Rakennetaan rivitaloa sekä väestönsuoja/varastorakennus. Asuntoja on 20 kpl; Kerrostalo - Rakennetaan neljäkerroksinen kerrostalo, josta osa on kellaritilaa ja tukimuuri. Asuntoja on 12 kpl. Anomus aloittaa rakennustyöt valitusaikana; Puunkaato - Kaadetaan n. 50 kuusta. Kiinteistöltä kaadetaan puita ja pintamaat poistetaan. Täyttöä on n. 10 000 m3.
 </t>
+  </si>
+  <si>
+    <t>Kuvaamasi toimenpide vaatii yleensä luvan. Voit hakea lupaa Lupapisteen kautta. Sinun kannattaa myös tutustua alla listattuihin sivustoihin, joilta löydät lisää tietoa rakennusvalvonnasta. Voit myös kysyä lisää aiheesta kunnan rakennusvalvonnasta Lupapisteen kautta tekemällä neuvontapyynnön.</t>
   </si>
 </sst>
 </file>
@@ -15241,8 +15244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C479"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A456" sqref="A456"/>
+    <sheetView topLeftCell="A463" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
@@ -22796,8 +22799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1621"/>
   <sheetViews>
-    <sheetView topLeftCell="A1583" zoomScale="54" zoomScaleNormal="54" zoomScalePageLayoutView="54" workbookViewId="0">
-      <selection activeCell="A1622" sqref="A1622"/>
+    <sheetView tabSelected="1" topLeftCell="B188" zoomScale="54" zoomScaleNormal="54" zoomScalePageLayoutView="54" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
@@ -23487,7 +23490,7 @@
         <v>3597</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
@@ -23543,7 +23546,7 @@
         <v>3593</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
@@ -23551,7 +23554,7 @@
         <v>3075</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
@@ -23591,7 +23594,7 @@
         <v>3606</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
@@ -23631,7 +23634,7 @@
         <v>3583</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
@@ -23655,7 +23658,7 @@
         <v>3599</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
@@ -23703,7 +23706,7 @@
         <v>3604</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
@@ -23735,7 +23738,7 @@
         <v>3596</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
@@ -23767,7 +23770,7 @@
         <v>3595</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
@@ -23799,7 +23802,7 @@
         <v>3589</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
@@ -23823,7 +23826,7 @@
         <v>3594</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
@@ -23855,7 +23858,7 @@
         <v>3592</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
@@ -23871,7 +23874,7 @@
         <v>3601</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
@@ -23919,7 +23922,7 @@
         <v>3605</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
@@ -23967,7 +23970,7 @@
         <v>3603</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
@@ -23983,7 +23986,7 @@
         <v>3591</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
@@ -24031,7 +24034,7 @@
         <v>3598</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
@@ -24055,7 +24058,7 @@
         <v>3600</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
@@ -24135,7 +24138,7 @@
         <v>3590</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
@@ -24159,7 +24162,7 @@
         <v>3602</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>3076</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Moved texts to excel (LUPA-480)
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="0" windowWidth="29040" windowHeight="14625" tabRatio="500"/>
+    <workbookView xWindow="165" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10804" uniqueCount="6463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10815" uniqueCount="6473">
   <si>
     <t>fi</t>
   </si>
@@ -19448,6 +19448,36 @@
   </si>
   <si>
     <t xml:space="preserve"> Alareunasta</t>
+  </si>
+  <si>
+    <t>session-dead.title</t>
+  </si>
+  <si>
+    <t>Istunto vanhentunut</t>
+  </si>
+  <si>
+    <t>session-dead.message</t>
+  </si>
+  <si>
+    <t>Istunto on vanhentunut ja sinun tulee kirjautua järjestelmään uudelleen.</t>
+  </si>
+  <si>
+    <t>session-dead.logout</t>
+  </si>
+  <si>
+    <t>Kirjaudu</t>
+  </si>
+  <si>
+    <t>connection.offline</t>
+  </si>
+  <si>
+    <t>Yhteys palvelimeen on katkennut.&lt;br/&gt;Yhteyttä yritetään muodostaa uudelleen...</t>
+  </si>
+  <si>
+    <t>application.filter.search</t>
+  </si>
+  <si>
+    <t>etsi:</t>
   </si>
 </sst>
 </file>
@@ -20366,10 +20396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C664"/>
+  <dimension ref="A1:C670"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A543" zoomScale="59" zoomScaleNormal="59" zoomScalePageLayoutView="59" workbookViewId="0">
-      <selection activeCell="B561" sqref="B561"/>
+    <sheetView tabSelected="1" topLeftCell="A644" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="59" workbookViewId="0">
+      <selection activeCell="B670" sqref="B670"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -27120,6 +27150,51 @@
       </c>
       <c r="C664" s="5" t="s">
         <v>1794</v>
+      </c>
+    </row>
+    <row r="665" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A665" s="1" t="s">
+        <v>6463</v>
+      </c>
+      <c r="B665" s="5" t="s">
+        <v>6464</v>
+      </c>
+    </row>
+    <row r="666" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A666" s="1" t="s">
+        <v>6465</v>
+      </c>
+      <c r="B666" s="5" t="s">
+        <v>6466</v>
+      </c>
+    </row>
+    <row r="667" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A667" s="1" t="s">
+        <v>6467</v>
+      </c>
+      <c r="B667" s="5" t="s">
+        <v>6468</v>
+      </c>
+    </row>
+    <row r="668" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A668" s="1" t="s">
+        <v>6469</v>
+      </c>
+      <c r="B668" s="5" t="s">
+        <v>6470</v>
+      </c>
+    </row>
+    <row r="669" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A669" s="1" t="s">
+        <v>4534</v>
+      </c>
+    </row>
+    <row r="670" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A670" s="1" t="s">
+        <v>6471</v>
+      </c>
+      <c r="B670" s="5" t="s">
+        <v>6472</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix percents to text
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11224" uniqueCount="6812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11226" uniqueCount="6814">
   <si>
     <t>fi</t>
   </si>
@@ -20503,15 +20503,18 @@
   </si>
   <si>
     <t>stamp.verdict</t>
+  </si>
+  <si>
+    <t>25%</t>
+  </si>
+  <si>
+    <t>75%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="##&quot;%&quot;"/>
-  </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -20638,8 +20641,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="159">
+  <cellStyleXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -20834,11 +20839,11 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="159">
+  <cellStyles count="161">
     <cellStyle name="Avattu hyperlinkki" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Avattu hyperlinkki" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Avattu hyperlinkki" xfId="6" builtinId="9" hidden="1"/>
@@ -20918,6 +20923,7 @@
     <cellStyle name="Avattu hyperlinkki" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Avattu hyperlinkki" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Avattu hyperlinkki" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Avattu hyperlinkki" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlinkki" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlinkki" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlinkki" xfId="5" builtinId="8" hidden="1"/>
@@ -20997,6 +21003,7 @@
     <cellStyle name="Hyperlinkki" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlinkki" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlinkki" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlinkki" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
@@ -21201,7 +21208,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mime-types_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mime-types" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21209,7 +21216,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mime-types" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mime-types_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21536,7 +21543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C847"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A781" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A825" workbookViewId="0">
       <selection activeCell="B833" sqref="B833"/>
     </sheetView>
   </sheetViews>
@@ -29453,8 +29460,8 @@
       <c r="A831" s="1" t="s">
         <v>6704</v>
       </c>
-      <c r="B831" s="15">
-        <v>25</v>
+      <c r="B831" s="15" t="s">
+        <v>6812</v>
       </c>
     </row>
     <row r="832" spans="1:2">
@@ -29469,8 +29476,8 @@
       <c r="A833" s="1" t="s">
         <v>6706</v>
       </c>
-      <c r="B833" s="15">
-        <v>75</v>
+      <c r="B833" s="15" t="s">
+        <v>6813</v>
       </c>
     </row>
     <row r="834" spans="1:3">

</xml_diff>

<commit_message>
Added missing localisation "maksaja.laskuviite".
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11848" uniqueCount="7250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11850" uniqueCount="7251">
   <si>
     <t>fi</t>
   </si>
@@ -20596,6 +20596,9 @@
   </si>
   <si>
     <t>Yrityksen nimi</t>
+  </si>
+  <si>
+    <t>yleiset-alueet-maksaja.laskuviite</t>
   </si>
   <si>
     <t>Laskuviite</t>
@@ -24295,7 +24298,7 @@
         <v>1804</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>7072</v>
+        <v>7073</v>
       </c>
       <c r="C134" s="5" t="s">
         <v>4914</v>
@@ -30950,7 +30953,7 @@
         <v>6815</v>
       </c>
       <c r="B845" s="2" t="s">
-        <v>7220</v>
+        <v>7221</v>
       </c>
       <c r="C845"/>
     </row>
@@ -30959,7 +30962,7 @@
         <v>6816</v>
       </c>
       <c r="B846" s="2" t="s">
-        <v>7221</v>
+        <v>7222</v>
       </c>
       <c r="C846"/>
     </row>
@@ -30968,7 +30971,7 @@
         <v>6817</v>
       </c>
       <c r="B847" s="2" t="s">
-        <v>7222</v>
+        <v>7223</v>
       </c>
       <c r="C847"/>
     </row>
@@ -30977,7 +30980,7 @@
         <v>6818</v>
       </c>
       <c r="B848" s="2" t="s">
-        <v>7223</v>
+        <v>7224</v>
       </c>
     </row>
     <row r="849" spans="1:2" x14ac:dyDescent="0.3">
@@ -37449,10 +37452,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2001"/>
+  <dimension ref="A1:D2002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1759" workbookViewId="0">
-      <selection activeCell="A1777" sqref="A1777"/>
+    <sheetView tabSelected="1" topLeftCell="A1732" workbookViewId="0">
+      <selection activeCell="A1753" sqref="A1753"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -38300,10 +38303,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>7224</v>
+        <v>7225</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>6843</v>
+        <v>6844</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
@@ -55857,7 +55860,7 @@
     </row>
     <row r="1685" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1685" s="1" t="s">
-        <v>7068</v>
+        <v>7069</v>
       </c>
       <c r="B1685" s="2" t="s">
         <v>184</v>
@@ -55869,7 +55872,7 @@
         <v>6834</v>
       </c>
       <c r="B1687" s="2" t="s">
-        <v>7069</v>
+        <v>7070</v>
       </c>
     </row>
     <row r="1688" spans="1:4" x14ac:dyDescent="0.3">
@@ -55877,111 +55880,111 @@
         <v>6836</v>
       </c>
       <c r="B1688" s="2" t="s">
-        <v>7070</v>
+        <v>7071</v>
       </c>
     </row>
     <row r="1690" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1690" s="1" t="s">
-        <v>7110</v>
+        <v>7111</v>
       </c>
       <c r="B1690" s="2" t="s">
-        <v>7111</v>
+        <v>7112</v>
       </c>
     </row>
     <row r="1691" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1691" s="1" t="s">
-        <v>7088</v>
+        <v>7089</v>
       </c>
       <c r="B1691" s="2" t="s">
-        <v>7089</v>
+        <v>7090</v>
       </c>
     </row>
     <row r="1692" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1692" s="1" t="s">
-        <v>7090</v>
+        <v>7091</v>
       </c>
       <c r="B1692" s="2" t="s">
-        <v>7091</v>
+        <v>7092</v>
       </c>
     </row>
     <row r="1693" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1693" s="1" t="s">
-        <v>7092</v>
+        <v>7093</v>
       </c>
       <c r="B1693" s="2" t="s">
-        <v>7093</v>
+        <v>7094</v>
       </c>
     </row>
     <row r="1694" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1694" s="1" t="s">
-        <v>7094</v>
+        <v>7095</v>
       </c>
       <c r="B1694" s="2" t="s">
-        <v>7095</v>
+        <v>7096</v>
       </c>
     </row>
     <row r="1695" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1695" s="1" t="s">
-        <v>7096</v>
+        <v>7097</v>
       </c>
       <c r="B1695" s="2" t="s">
-        <v>7097</v>
+        <v>7098</v>
       </c>
     </row>
     <row r="1696" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1696" s="1" t="s">
-        <v>7098</v>
+        <v>7099</v>
       </c>
       <c r="B1696" s="2" t="s">
-        <v>7099</v>
+        <v>7100</v>
       </c>
     </row>
     <row r="1697" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1697" s="1" t="s">
-        <v>7100</v>
+        <v>7101</v>
       </c>
       <c r="B1697" s="2" t="s">
-        <v>7101</v>
+        <v>7102</v>
       </c>
     </row>
     <row r="1698" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1698" s="1" t="s">
-        <v>7102</v>
+        <v>7103</v>
       </c>
       <c r="B1698" s="2" t="s">
-        <v>7103</v>
+        <v>7104</v>
       </c>
     </row>
     <row r="1700" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1700" s="1" t="s">
-        <v>7082</v>
+        <v>7083</v>
       </c>
       <c r="B1700" s="2" t="s">
-        <v>7083</v>
+        <v>7084</v>
       </c>
     </row>
     <row r="1701" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1701" s="1" t="s">
-        <v>7104</v>
+        <v>7105</v>
       </c>
       <c r="B1701" s="2" t="s">
-        <v>7105</v>
+        <v>7106</v>
       </c>
     </row>
     <row r="1702" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1702" s="1" t="s">
-        <v>7106</v>
+        <v>7107</v>
       </c>
       <c r="B1702" s="2" t="s">
-        <v>7107</v>
+        <v>7108</v>
       </c>
     </row>
     <row r="1703" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1703" s="1" t="s">
-        <v>7108</v>
+        <v>7109</v>
       </c>
       <c r="B1703" s="2" t="s">
-        <v>7109</v>
+        <v>7110</v>
       </c>
     </row>
     <row r="1705" spans="1:2" x14ac:dyDescent="0.3">
@@ -55997,31 +56000,31 @@
         <v>6840</v>
       </c>
       <c r="B1707" s="2" t="s">
-        <v>7086</v>
+        <v>7087</v>
       </c>
     </row>
     <row r="1708" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1708" s="1" t="s">
-        <v>7084</v>
+        <v>7085</v>
       </c>
       <c r="B1708" s="2" t="s">
-        <v>7085</v>
+        <v>7086</v>
       </c>
     </row>
     <row r="1709" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1709" s="1" t="s">
-        <v>7112</v>
+        <v>7113</v>
       </c>
       <c r="B1709" s="2" t="s">
-        <v>7113</v>
+        <v>7114</v>
       </c>
     </row>
     <row r="1710" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1710" s="1" t="s">
-        <v>7116</v>
+        <v>7117</v>
       </c>
       <c r="B1710" s="2" t="s">
-        <v>7091</v>
+        <v>7092</v>
       </c>
     </row>
     <row r="1712" spans="1:2" x14ac:dyDescent="0.3">
@@ -56034,7 +56037,7 @@
     </row>
     <row r="1713" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1713" s="1" t="s">
-        <v>7087</v>
+        <v>7088</v>
       </c>
       <c r="B1713" s="2" t="s">
         <v>3571</v>
@@ -56042,7 +56045,7 @@
     </row>
     <row r="1714" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1714" s="1" t="s">
-        <v>7114</v>
+        <v>7115</v>
       </c>
       <c r="B1714" s="2" t="s">
         <v>3571</v>
@@ -56050,7 +56053,7 @@
     </row>
     <row r="1715" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1715" s="1" t="s">
-        <v>7117</v>
+        <v>7118</v>
       </c>
       <c r="B1715" s="2" t="s">
         <v>3571</v>
@@ -56058,7 +56061,7 @@
     </row>
     <row r="1717" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1717" s="1" t="s">
-        <v>7190</v>
+        <v>7191</v>
       </c>
       <c r="B1717" s="2" t="s">
         <v>94</v>
@@ -56066,15 +56069,15 @@
     </row>
     <row r="1718" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1718" s="1" t="s">
-        <v>7191</v>
+        <v>7192</v>
       </c>
       <c r="B1718" s="2" t="s">
-        <v>7165</v>
+        <v>7166</v>
       </c>
     </row>
     <row r="1719" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1719" s="1" t="s">
-        <v>7218</v>
+        <v>7219</v>
       </c>
       <c r="B1719" s="17" t="s">
         <v>1779</v>
@@ -56082,7 +56085,7 @@
     </row>
     <row r="1720" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1720" s="1" t="s">
-        <v>7219</v>
+        <v>7220</v>
       </c>
       <c r="B1720" s="17" t="s">
         <v>35</v>
@@ -56093,7 +56096,7 @@
     </row>
     <row r="1722" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1722" s="1" t="s">
-        <v>7192</v>
+        <v>7193</v>
       </c>
       <c r="B1722" s="2" t="s">
         <v>94</v>
@@ -56101,7 +56104,7 @@
     </row>
     <row r="1723" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1723" s="1" t="s">
-        <v>7193</v>
+        <v>7194</v>
       </c>
       <c r="B1723" s="2" t="s">
         <v>98</v>
@@ -56109,7 +56112,7 @@
     </row>
     <row r="1724" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1724" s="1" t="s">
-        <v>7194</v>
+        <v>7195</v>
       </c>
       <c r="B1724" s="2" t="s">
         <v>100</v>
@@ -56117,7 +56120,7 @@
     </row>
     <row r="1725" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1725" s="1" t="s">
-        <v>7195</v>
+        <v>7196</v>
       </c>
       <c r="B1725" s="2" t="s">
         <v>104</v>
@@ -56125,7 +56128,7 @@
     </row>
     <row r="1726" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1726" s="1" t="s">
-        <v>7196</v>
+        <v>7197</v>
       </c>
       <c r="B1726" s="2" t="s">
         <v>102</v>
@@ -56133,7 +56136,7 @@
     </row>
     <row r="1727" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1727" s="1" t="s">
-        <v>7197</v>
+        <v>7198</v>
       </c>
       <c r="B1727" s="2" t="s">
         <v>111</v>
@@ -56141,7 +56144,7 @@
     </row>
     <row r="1728" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1728" s="1" t="s">
-        <v>7198</v>
+        <v>7199</v>
       </c>
       <c r="B1728" s="2" t="s">
         <v>113</v>
@@ -56149,7 +56152,7 @@
     </row>
     <row r="1729" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1729" s="1" t="s">
-        <v>7199</v>
+        <v>7200</v>
       </c>
       <c r="B1729" s="2" t="s">
         <v>115</v>
@@ -56157,7 +56160,7 @@
     </row>
     <row r="1730" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1730" s="1" t="s">
-        <v>7200</v>
+        <v>7201</v>
       </c>
       <c r="B1730" s="2" t="s">
         <v>117</v>
@@ -56165,7 +56168,7 @@
     </row>
     <row r="1731" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1731" s="1" t="s">
-        <v>7201</v>
+        <v>7202</v>
       </c>
       <c r="B1731" s="2" t="s">
         <v>121</v>
@@ -56173,7 +56176,7 @@
     </row>
     <row r="1732" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1732" s="1" t="s">
-        <v>7202</v>
+        <v>7203</v>
       </c>
       <c r="B1732" s="2" t="s">
         <v>126</v>
@@ -56181,7 +56184,7 @@
     </row>
     <row r="1733" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1733" s="1" t="s">
-        <v>7203</v>
+        <v>7204</v>
       </c>
       <c r="B1733" s="2" t="s">
         <v>124</v>
@@ -56189,15 +56192,15 @@
     </row>
     <row r="1735" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1735" s="1" t="s">
-        <v>7204</v>
+        <v>7205</v>
       </c>
       <c r="B1735" s="2" t="s">
-        <v>6847</v>
+        <v>6848</v>
       </c>
     </row>
     <row r="1736" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1736" s="1" t="s">
-        <v>7205</v>
+        <v>7206</v>
       </c>
       <c r="B1736" s="2" t="s">
         <v>6842</v>
@@ -56205,7 +56208,7 @@
     </row>
     <row r="1737" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1737" s="1" t="s">
-        <v>7206</v>
+        <v>7207</v>
       </c>
       <c r="B1737" s="2" t="s">
         <v>109</v>
@@ -56213,7 +56216,7 @@
     </row>
     <row r="1738" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1738" s="1" t="s">
-        <v>7207</v>
+        <v>7208</v>
       </c>
       <c r="B1738" s="2" t="s">
         <v>111</v>
@@ -56221,7 +56224,7 @@
     </row>
     <row r="1739" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1739" s="1" t="s">
-        <v>7208</v>
+        <v>7209</v>
       </c>
       <c r="B1739" s="2" t="s">
         <v>113</v>
@@ -56229,7 +56232,7 @@
     </row>
     <row r="1740" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1740" s="1" t="s">
-        <v>7209</v>
+        <v>7210</v>
       </c>
       <c r="B1740" s="2" t="s">
         <v>115</v>
@@ -56237,7 +56240,7 @@
     </row>
     <row r="1741" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1741" s="1" t="s">
-        <v>7210</v>
+        <v>7211</v>
       </c>
       <c r="B1741" s="2" t="s">
         <v>117</v>
@@ -56245,15 +56248,15 @@
     </row>
     <row r="1742" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1742" s="1" t="s">
-        <v>7211</v>
+        <v>7212</v>
       </c>
       <c r="B1742" s="2" t="s">
-        <v>7183</v>
+        <v>7184</v>
       </c>
     </row>
     <row r="1743" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1743" s="1" t="s">
-        <v>7212</v>
+        <v>7213</v>
       </c>
       <c r="B1743" s="2" t="s">
         <v>98</v>
@@ -56261,7 +56264,7 @@
     </row>
     <row r="1744" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1744" s="1" t="s">
-        <v>7213</v>
+        <v>7214</v>
       </c>
       <c r="B1744" s="2" t="s">
         <v>100</v>
@@ -56269,7 +56272,7 @@
     </row>
     <row r="1745" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1745" s="1" t="s">
-        <v>7214</v>
+        <v>7215</v>
       </c>
       <c r="B1745" s="2" t="s">
         <v>104</v>
@@ -56277,7 +56280,7 @@
     </row>
     <row r="1746" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1746" s="1" t="s">
-        <v>7215</v>
+        <v>7216</v>
       </c>
       <c r="B1746" s="2" t="s">
         <v>121</v>
@@ -56285,7 +56288,7 @@
     </row>
     <row r="1747" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1747" s="1" t="s">
-        <v>7216</v>
+        <v>7217</v>
       </c>
       <c r="B1747" s="2" t="s">
         <v>126</v>
@@ -56293,7 +56296,7 @@
     </row>
     <row r="1748" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1748" s="1" t="s">
-        <v>7217</v>
+        <v>7218</v>
       </c>
       <c r="B1748" s="2" t="s">
         <v>124</v>
@@ -56307,28 +56310,28 @@
         <v>1340</v>
       </c>
     </row>
+    <row r="1751" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1751" s="1" t="s">
+        <v>7226</v>
+      </c>
+      <c r="B1751" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
     <row r="1752" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1752" s="1" t="s">
-        <v>7225</v>
+        <v>7227</v>
       </c>
       <c r="B1752" s="2" t="s">
-        <v>94</v>
+        <v>7166</v>
       </c>
     </row>
     <row r="1753" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1753" s="1" t="s">
-        <v>7226</v>
+        <v>6843</v>
       </c>
       <c r="B1753" s="2" t="s">
-        <v>7165</v>
-      </c>
-    </row>
-    <row r="1754" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1754" s="1" t="s">
-        <v>7227</v>
-      </c>
-      <c r="B1754" s="2" t="s">
-        <v>94</v>
+        <v>6844</v>
       </c>
     </row>
     <row r="1755" spans="1:2" x14ac:dyDescent="0.3">
@@ -56336,7 +56339,7 @@
         <v>7228</v>
       </c>
       <c r="B1755" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="1756" spans="1:2" x14ac:dyDescent="0.3">
@@ -56344,7 +56347,7 @@
         <v>7229</v>
       </c>
       <c r="B1756" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="1757" spans="1:2" x14ac:dyDescent="0.3">
@@ -56352,7 +56355,7 @@
         <v>7230</v>
       </c>
       <c r="B1757" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1758" spans="1:2" x14ac:dyDescent="0.3">
@@ -56360,7 +56363,7 @@
         <v>7231</v>
       </c>
       <c r="B1758" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="1759" spans="1:2" x14ac:dyDescent="0.3">
@@ -56368,7 +56371,7 @@
         <v>7232</v>
       </c>
       <c r="B1759" s="2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="1760" spans="1:2" x14ac:dyDescent="0.3">
@@ -56376,7 +56379,7 @@
         <v>7233</v>
       </c>
       <c r="B1760" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1761" spans="1:2" x14ac:dyDescent="0.3">
@@ -56384,7 +56387,7 @@
         <v>7234</v>
       </c>
       <c r="B1761" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="1762" spans="1:2" x14ac:dyDescent="0.3">
@@ -56392,7 +56395,7 @@
         <v>7235</v>
       </c>
       <c r="B1762" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1763" spans="1:2" x14ac:dyDescent="0.3">
@@ -56400,7 +56403,7 @@
         <v>7236</v>
       </c>
       <c r="B1763" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1764" spans="1:2" x14ac:dyDescent="0.3">
@@ -56408,7 +56411,7 @@
         <v>7237</v>
       </c>
       <c r="B1764" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="1765" spans="1:2" x14ac:dyDescent="0.3">
@@ -56416,15 +56419,15 @@
         <v>7238</v>
       </c>
       <c r="B1765" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1766" s="1" t="s">
+        <v>7239</v>
+      </c>
+      <c r="B1766" s="2" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="1767" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1767" s="1" t="s">
-        <v>7157</v>
-      </c>
-      <c r="B1767" s="2" t="s">
-        <v>6847</v>
       </c>
     </row>
     <row r="1768" spans="1:2" x14ac:dyDescent="0.3">
@@ -56432,7 +56435,7 @@
         <v>7158</v>
       </c>
       <c r="B1768" s="2" t="s">
-        <v>6842</v>
+        <v>6848</v>
       </c>
     </row>
     <row r="1769" spans="1:2" x14ac:dyDescent="0.3">
@@ -56440,15 +56443,15 @@
         <v>7159</v>
       </c>
       <c r="B1769" s="2" t="s">
-        <v>109</v>
+        <v>6842</v>
       </c>
     </row>
     <row r="1770" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1770" s="1" t="s">
-        <v>7239</v>
+        <v>7160</v>
       </c>
       <c r="B1770" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="1771" spans="1:2" x14ac:dyDescent="0.3">
@@ -56456,7 +56459,7 @@
         <v>7240</v>
       </c>
       <c r="B1771" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1772" spans="1:2" x14ac:dyDescent="0.3">
@@ -56464,7 +56467,7 @@
         <v>7241</v>
       </c>
       <c r="B1772" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="1773" spans="1:2" x14ac:dyDescent="0.3">
@@ -56472,7 +56475,7 @@
         <v>7242</v>
       </c>
       <c r="B1773" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1774" spans="1:2" x14ac:dyDescent="0.3">
@@ -56480,7 +56483,7 @@
         <v>7243</v>
       </c>
       <c r="B1774" s="2" t="s">
-        <v>7183</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1775" spans="1:2" x14ac:dyDescent="0.3">
@@ -56488,7 +56491,7 @@
         <v>7244</v>
       </c>
       <c r="B1775" s="2" t="s">
-        <v>98</v>
+        <v>7184</v>
       </c>
     </row>
     <row r="1776" spans="1:2" x14ac:dyDescent="0.3">
@@ -56496,7 +56499,7 @@
         <v>7245</v>
       </c>
       <c r="B1776" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="1777" spans="1:2" x14ac:dyDescent="0.3">
@@ -56504,7 +56507,7 @@
         <v>7246</v>
       </c>
       <c r="B1777" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1778" spans="1:2" x14ac:dyDescent="0.3">
@@ -56512,7 +56515,7 @@
         <v>7247</v>
       </c>
       <c r="B1778" s="2" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="1779" spans="1:2" x14ac:dyDescent="0.3">
@@ -56520,7 +56523,7 @@
         <v>7248</v>
       </c>
       <c r="B1779" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="1780" spans="1:2" x14ac:dyDescent="0.3">
@@ -56528,31 +56531,31 @@
         <v>7249</v>
       </c>
       <c r="B1780" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1781" s="1" t="s">
+        <v>7250</v>
+      </c>
+      <c r="B1781" s="2" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="1782" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1782" s="1" t="s">
-        <v>6844</v>
-      </c>
-      <c r="B1782" s="2" t="s">
-        <v>6845</v>
       </c>
     </row>
     <row r="1783" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1783" s="1" t="s">
-        <v>7152</v>
+        <v>6845</v>
       </c>
       <c r="B1783" s="2" t="s">
-        <v>6845</v>
+        <v>6846</v>
       </c>
     </row>
     <row r="1784" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1784" s="1" t="s">
-        <v>7163</v>
+        <v>7153</v>
       </c>
       <c r="B1784" s="2" t="s">
-        <v>94</v>
+        <v>6846</v>
       </c>
     </row>
     <row r="1785" spans="1:2" x14ac:dyDescent="0.3">
@@ -56560,15 +56563,15 @@
         <v>7164</v>
       </c>
       <c r="B1785" s="2" t="s">
-        <v>7165</v>
+        <v>94</v>
       </c>
     </row>
     <row r="1786" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1786" s="1" t="s">
+        <v>7165</v>
+      </c>
+      <c r="B1786" s="2" t="s">
         <v>7166</v>
-      </c>
-      <c r="B1786" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="1787" spans="1:2" x14ac:dyDescent="0.3">
@@ -56576,7 +56579,7 @@
         <v>7167</v>
       </c>
       <c r="B1787" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="1788" spans="1:2" x14ac:dyDescent="0.3">
@@ -56584,7 +56587,7 @@
         <v>7168</v>
       </c>
       <c r="B1788" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="1789" spans="1:2" x14ac:dyDescent="0.3">
@@ -56592,7 +56595,7 @@
         <v>7169</v>
       </c>
       <c r="B1789" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1790" spans="1:2" x14ac:dyDescent="0.3">
@@ -56600,7 +56603,7 @@
         <v>7170</v>
       </c>
       <c r="B1790" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="1791" spans="1:2" x14ac:dyDescent="0.3">
@@ -56608,7 +56611,7 @@
         <v>7171</v>
       </c>
       <c r="B1791" s="2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="1792" spans="1:2" x14ac:dyDescent="0.3">
@@ -56616,7 +56619,7 @@
         <v>7172</v>
       </c>
       <c r="B1792" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1793" spans="1:2" x14ac:dyDescent="0.3">
@@ -56624,7 +56627,7 @@
         <v>7173</v>
       </c>
       <c r="B1793" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="1794" spans="1:2" x14ac:dyDescent="0.3">
@@ -56632,7 +56635,7 @@
         <v>7174</v>
       </c>
       <c r="B1794" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1795" spans="1:2" x14ac:dyDescent="0.3">
@@ -56640,7 +56643,7 @@
         <v>7175</v>
       </c>
       <c r="B1795" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1796" spans="1:2" x14ac:dyDescent="0.3">
@@ -56648,7 +56651,7 @@
         <v>7176</v>
       </c>
       <c r="B1796" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="1797" spans="1:2" x14ac:dyDescent="0.3">
@@ -56656,23 +56659,23 @@
         <v>7177</v>
       </c>
       <c r="B1797" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1798" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1798" s="1" t="s">
-        <v>6846</v>
+        <v>7178</v>
       </c>
       <c r="B1798" s="2" t="s">
-        <v>6847</v>
+        <v>124</v>
       </c>
     </row>
     <row r="1799" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1799" s="1" t="s">
+        <v>6847</v>
+      </c>
+      <c r="B1799" s="2" t="s">
         <v>6848</v>
-      </c>
-      <c r="B1799" s="2" t="s">
-        <v>6842</v>
       </c>
     </row>
     <row r="1800" spans="1:2" x14ac:dyDescent="0.3">
@@ -56680,15 +56683,15 @@
         <v>6849</v>
       </c>
       <c r="B1800" s="2" t="s">
-        <v>109</v>
+        <v>6842</v>
       </c>
     </row>
     <row r="1801" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1801" s="1" t="s">
-        <v>7178</v>
+        <v>6850</v>
       </c>
       <c r="B1801" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="1802" spans="1:2" x14ac:dyDescent="0.3">
@@ -56696,7 +56699,7 @@
         <v>7179</v>
       </c>
       <c r="B1802" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1803" spans="1:2" x14ac:dyDescent="0.3">
@@ -56704,7 +56707,7 @@
         <v>7180</v>
       </c>
       <c r="B1803" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="1804" spans="1:2" x14ac:dyDescent="0.3">
@@ -56712,7 +56715,7 @@
         <v>7181</v>
       </c>
       <c r="B1804" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1805" spans="1:2" x14ac:dyDescent="0.3">
@@ -56720,15 +56723,15 @@
         <v>7182</v>
       </c>
       <c r="B1805" s="2" t="s">
-        <v>7183</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1806" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1806" s="1" t="s">
+        <v>7183</v>
+      </c>
+      <c r="B1806" s="2" t="s">
         <v>7184</v>
-      </c>
-      <c r="B1806" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="1807" spans="1:2" x14ac:dyDescent="0.3">
@@ -56736,7 +56739,7 @@
         <v>7185</v>
       </c>
       <c r="B1807" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="1808" spans="1:2" x14ac:dyDescent="0.3">
@@ -56744,7 +56747,7 @@
         <v>7186</v>
       </c>
       <c r="B1808" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1809" spans="1:2" x14ac:dyDescent="0.3">
@@ -56752,7 +56755,7 @@
         <v>7187</v>
       </c>
       <c r="B1809" s="2" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="1810" spans="1:2" x14ac:dyDescent="0.3">
@@ -56760,7 +56763,7 @@
         <v>7188</v>
       </c>
       <c r="B1810" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="1811" spans="1:2" x14ac:dyDescent="0.3">
@@ -56768,15 +56771,15 @@
         <v>7189</v>
       </c>
       <c r="B1811" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="1812" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1812" s="1" t="s">
+        <v>7190</v>
+      </c>
+      <c r="B1812" s="2" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="1813" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1813" s="1" t="s">
-        <v>7075</v>
-      </c>
-      <c r="B1813" s="2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="1814" spans="1:2" x14ac:dyDescent="0.3">
@@ -56784,7 +56787,7 @@
         <v>7076</v>
       </c>
       <c r="B1814" s="2" t="s">
-        <v>7071</v>
+        <v>200</v>
       </c>
     </row>
     <row r="1815" spans="1:2" x14ac:dyDescent="0.3">
@@ -56792,15 +56795,15 @@
         <v>7077</v>
       </c>
       <c r="B1815" s="2" t="s">
-        <v>6850</v>
-      </c>
-    </row>
-    <row r="1817" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1817" s="1" t="s">
+        <v>7072</v>
+      </c>
+    </row>
+    <row r="1816" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1816" s="1" t="s">
         <v>7078</v>
       </c>
-      <c r="B1817" s="2" t="s">
-        <v>200</v>
+      <c r="B1816" s="2" t="s">
+        <v>6851</v>
       </c>
     </row>
     <row r="1818" spans="1:2" x14ac:dyDescent="0.3">
@@ -56808,7 +56811,7 @@
         <v>7079</v>
       </c>
       <c r="B1818" s="2" t="s">
-        <v>7071</v>
+        <v>200</v>
       </c>
     </row>
     <row r="1819" spans="1:2" x14ac:dyDescent="0.3">
@@ -56816,31 +56819,31 @@
         <v>7080</v>
       </c>
       <c r="B1819" s="2" t="s">
+        <v>7072</v>
+      </c>
+    </row>
+    <row r="1820" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1820" s="1" t="s">
         <v>7081</v>
       </c>
-    </row>
-    <row r="1821" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1821" s="1" t="s">
-        <v>7115</v>
-      </c>
-      <c r="B1821" s="2" t="s">
-        <v>6851</v>
+      <c r="B1820" s="2" t="s">
+        <v>7082</v>
       </c>
     </row>
     <row r="1822" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1822" s="1" t="s">
-        <v>7153</v>
+        <v>7116</v>
       </c>
       <c r="B1822" s="2" t="s">
-        <v>7154</v>
+        <v>6852</v>
       </c>
     </row>
     <row r="1823" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1823" s="1" t="s">
+        <v>7154</v>
+      </c>
+      <c r="B1823" s="2" t="s">
         <v>7155</v>
-      </c>
-      <c r="B1823" s="2" t="s">
-        <v>6852</v>
       </c>
     </row>
     <row r="1824" spans="1:2" x14ac:dyDescent="0.3">
@@ -56851,12 +56854,12 @@
         <v>6853</v>
       </c>
     </row>
-    <row r="1826" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1826" s="1" t="s">
+    <row r="1825" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1825" s="1" t="s">
+        <v>7157</v>
+      </c>
+      <c r="B1825" s="2" t="s">
         <v>6854</v>
-      </c>
-      <c r="B1826" s="2" t="s">
-        <v>6835</v>
       </c>
     </row>
     <row r="1827" spans="1:2" x14ac:dyDescent="0.3">
@@ -56864,87 +56867,87 @@
         <v>6855</v>
       </c>
       <c r="B1827" s="2" t="s">
-        <v>6856</v>
+        <v>6835</v>
       </c>
     </row>
     <row r="1828" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1828" s="1" t="s">
+        <v>6856</v>
+      </c>
+      <c r="B1828" s="2" t="s">
         <v>6857</v>
-      </c>
-      <c r="B1828" s="2" t="s">
-        <v>6858</v>
       </c>
     </row>
     <row r="1829" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1829" s="1" t="s">
+        <v>6858</v>
+      </c>
+      <c r="B1829" s="2" t="s">
         <v>6859</v>
-      </c>
-      <c r="B1829" s="2" t="s">
-        <v>6860</v>
       </c>
     </row>
     <row r="1830" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1830" s="1" t="s">
+        <v>6860</v>
+      </c>
+      <c r="B1830" s="2" t="s">
         <v>6861</v>
-      </c>
-      <c r="B1830" s="2" t="s">
-        <v>6862</v>
       </c>
     </row>
     <row r="1831" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1831" s="1" t="s">
-        <v>7160</v>
+        <v>6862</v>
       </c>
       <c r="B1831" s="2" t="s">
-        <v>7161</v>
+        <v>6863</v>
       </c>
     </row>
     <row r="1832" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1832" s="1" t="s">
+        <v>7161</v>
+      </c>
+      <c r="B1832" s="2" t="s">
         <v>7162</v>
       </c>
-      <c r="B1832" s="2" t="s">
+    </row>
+    <row r="1833" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1833" s="1" t="s">
+        <v>7163</v>
+      </c>
+      <c r="B1833" s="2" t="s">
         <v>1665</v>
-      </c>
-    </row>
-    <row r="1834" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1834" s="1" t="s">
-        <v>7118</v>
-      </c>
-      <c r="B1834" s="2" t="s">
-        <v>7119</v>
       </c>
     </row>
     <row r="1835" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1835" s="1" t="s">
+        <v>7119</v>
+      </c>
+      <c r="B1835" s="2" t="s">
         <v>7120</v>
-      </c>
-      <c r="B1835" s="2" t="s">
-        <v>7121</v>
       </c>
     </row>
     <row r="1836" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1836" s="1" t="s">
+        <v>7121</v>
+      </c>
+      <c r="B1836" s="2" t="s">
         <v>7122</v>
-      </c>
-      <c r="B1836" s="2" t="s">
-        <v>7123</v>
       </c>
     </row>
     <row r="1837" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1837" s="1" t="s">
+        <v>7123</v>
+      </c>
+      <c r="B1837" s="2" t="s">
         <v>7124</v>
-      </c>
-      <c r="B1837" s="2" t="s">
-        <v>7125</v>
       </c>
     </row>
     <row r="1838" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1838" s="1" t="s">
+        <v>7125</v>
+      </c>
+      <c r="B1838" s="2" t="s">
         <v>7126</v>
-      </c>
-      <c r="B1838" s="2" t="s">
-        <v>6842</v>
       </c>
     </row>
     <row r="1839" spans="1:2" x14ac:dyDescent="0.3">
@@ -56952,7 +56955,7 @@
         <v>7127</v>
       </c>
       <c r="B1839" s="2" t="s">
-        <v>109</v>
+        <v>6842</v>
       </c>
     </row>
     <row r="1840" spans="1:2" x14ac:dyDescent="0.3">
@@ -56960,7 +56963,7 @@
         <v>7128</v>
       </c>
       <c r="B1840" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="1841" spans="1:2" x14ac:dyDescent="0.3">
@@ -56968,7 +56971,7 @@
         <v>7129</v>
       </c>
       <c r="B1841" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1842" spans="1:2" x14ac:dyDescent="0.3">
@@ -56976,7 +56979,7 @@
         <v>7130</v>
       </c>
       <c r="B1842" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="1843" spans="1:2" x14ac:dyDescent="0.3">
@@ -56984,7 +56987,7 @@
         <v>7131</v>
       </c>
       <c r="B1843" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1844" spans="1:2" x14ac:dyDescent="0.3">
@@ -56992,7 +56995,7 @@
         <v>7132</v>
       </c>
       <c r="B1844" s="2" t="s">
-        <v>6843</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1845" spans="1:2" x14ac:dyDescent="0.3">
@@ -57000,7 +57003,7 @@
         <v>7133</v>
       </c>
       <c r="B1845" s="2" t="s">
-        <v>6921</v>
+        <v>6844</v>
       </c>
     </row>
     <row r="1846" spans="1:2" x14ac:dyDescent="0.3">
@@ -57008,63 +57011,63 @@
         <v>7134</v>
       </c>
       <c r="B1846" s="2" t="s">
-        <v>7135</v>
+        <v>6922</v>
       </c>
     </row>
     <row r="1847" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1847" s="1" t="s">
+        <v>7135</v>
+      </c>
+      <c r="B1847" s="2" t="s">
         <v>7136</v>
-      </c>
-      <c r="B1847" s="2" t="s">
-        <v>7137</v>
       </c>
     </row>
     <row r="1848" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1848" s="1" t="s">
+        <v>7137</v>
+      </c>
+      <c r="B1848" s="2" t="s">
         <v>7138</v>
-      </c>
-      <c r="B1848" s="2" t="s">
-        <v>7139</v>
       </c>
     </row>
     <row r="1849" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1849" s="1" t="s">
+        <v>7139</v>
+      </c>
+      <c r="B1849" s="2" t="s">
         <v>7140</v>
-      </c>
-      <c r="B1849" s="2" t="s">
-        <v>7141</v>
       </c>
     </row>
     <row r="1850" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1850" s="1" t="s">
+        <v>7141</v>
+      </c>
+      <c r="B1850" s="2" t="s">
         <v>7142</v>
-      </c>
-      <c r="B1850" s="2" t="s">
-        <v>7143</v>
       </c>
     </row>
     <row r="1851" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1851" s="1" t="s">
+        <v>7143</v>
+      </c>
+      <c r="B1851" s="2" t="s">
         <v>7144</v>
-      </c>
-      <c r="B1851" s="2" t="s">
-        <v>7145</v>
       </c>
     </row>
     <row r="1852" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1852" s="1" t="s">
+        <v>7145</v>
+      </c>
+      <c r="B1852" s="2" t="s">
         <v>7146</v>
-      </c>
-      <c r="B1852" s="2" t="s">
-        <v>7147</v>
       </c>
     </row>
     <row r="1853" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1853" s="1" t="s">
+        <v>7147</v>
+      </c>
+      <c r="B1853" s="2" t="s">
         <v>7148</v>
-      </c>
-      <c r="B1853" s="2" t="s">
-        <v>6921</v>
       </c>
     </row>
     <row r="1854" spans="1:2" x14ac:dyDescent="0.3">
@@ -57072,7 +57075,7 @@
         <v>7149</v>
       </c>
       <c r="B1854" s="2" t="s">
-        <v>7135</v>
+        <v>6922</v>
       </c>
     </row>
     <row r="1855" spans="1:2" x14ac:dyDescent="0.3">
@@ -57080,7 +57083,7 @@
         <v>7150</v>
       </c>
       <c r="B1855" s="2" t="s">
-        <v>7137</v>
+        <v>7136</v>
       </c>
     </row>
     <row r="1856" spans="1:2" x14ac:dyDescent="0.3">
@@ -57088,31 +57091,31 @@
         <v>7151</v>
       </c>
       <c r="B1856" s="2" t="s">
-        <v>7139</v>
-      </c>
-    </row>
-    <row r="1858" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1858" s="1" t="s">
-        <v>6863</v>
-      </c>
-      <c r="B1858" s="2" t="s">
-        <v>6864</v>
+        <v>7138</v>
+      </c>
+    </row>
+    <row r="1857" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1857" s="1" t="s">
+        <v>7152</v>
+      </c>
+      <c r="B1857" s="2" t="s">
+        <v>7140</v>
       </c>
     </row>
     <row r="1859" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1859" s="1" t="s">
+        <v>6864</v>
+      </c>
+      <c r="B1859" s="2" t="s">
         <v>6865</v>
-      </c>
-      <c r="B1859" s="2" t="s">
-        <v>6866</v>
       </c>
     </row>
     <row r="1860" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1860" s="1" t="s">
+        <v>6866</v>
+      </c>
+      <c r="B1860" s="2" t="s">
         <v>6867</v>
-      </c>
-      <c r="B1860" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="1861" spans="1:2" x14ac:dyDescent="0.3">
@@ -57120,7 +57123,7 @@
         <v>6868</v>
       </c>
       <c r="B1861" s="2" t="s">
-        <v>6847</v>
+        <v>94</v>
       </c>
     </row>
     <row r="1862" spans="1:2" x14ac:dyDescent="0.3">
@@ -57128,7 +57131,7 @@
         <v>6869</v>
       </c>
       <c r="B1862" s="2" t="s">
-        <v>94</v>
+        <v>6848</v>
       </c>
     </row>
     <row r="1863" spans="1:2" x14ac:dyDescent="0.3">
@@ -57136,7 +57139,7 @@
         <v>6870</v>
       </c>
       <c r="B1863" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="1864" spans="1:2" x14ac:dyDescent="0.3">
@@ -57144,7 +57147,7 @@
         <v>6871</v>
       </c>
       <c r="B1864" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="1865" spans="1:2" x14ac:dyDescent="0.3">
@@ -57152,7 +57155,7 @@
         <v>6872</v>
       </c>
       <c r="B1865" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1866" spans="1:2" x14ac:dyDescent="0.3">
@@ -57160,7 +57163,7 @@
         <v>6873</v>
       </c>
       <c r="B1866" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="1867" spans="1:2" x14ac:dyDescent="0.3">
@@ -57168,7 +57171,7 @@
         <v>6874</v>
       </c>
       <c r="B1867" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="1868" spans="1:2" x14ac:dyDescent="0.3">
@@ -57176,7 +57179,7 @@
         <v>6875</v>
       </c>
       <c r="B1868" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1869" spans="1:2" x14ac:dyDescent="0.3">
@@ -57184,7 +57187,7 @@
         <v>6876</v>
       </c>
       <c r="B1869" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="1870" spans="1:2" x14ac:dyDescent="0.3">
@@ -57192,7 +57195,7 @@
         <v>6877</v>
       </c>
       <c r="B1870" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1871" spans="1:2" x14ac:dyDescent="0.3">
@@ -57200,7 +57203,7 @@
         <v>6878</v>
       </c>
       <c r="B1871" s="2" t="s">
-        <v>7052</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1872" spans="1:2" x14ac:dyDescent="0.3">
@@ -57208,7 +57211,7 @@
         <v>6879</v>
       </c>
       <c r="B1872" s="2" t="s">
-        <v>121</v>
+        <v>7053</v>
       </c>
     </row>
     <row r="1873" spans="1:2" x14ac:dyDescent="0.3">
@@ -57216,7 +57219,7 @@
         <v>6880</v>
       </c>
       <c r="B1873" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="1874" spans="1:2" x14ac:dyDescent="0.3">
@@ -57224,7 +57227,7 @@
         <v>6881</v>
       </c>
       <c r="B1874" s="2" t="s">
-        <v>5224</v>
+        <v>124</v>
       </c>
     </row>
     <row r="1875" spans="1:2" x14ac:dyDescent="0.3">
@@ -57232,7 +57235,7 @@
         <v>6882</v>
       </c>
       <c r="B1875" s="2" t="s">
-        <v>126</v>
+        <v>5224</v>
       </c>
     </row>
     <row r="1876" spans="1:2" x14ac:dyDescent="0.3">
@@ -57240,7 +57243,7 @@
         <v>6883</v>
       </c>
       <c r="B1876" s="2" t="s">
-        <v>6847</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1877" spans="1:2" x14ac:dyDescent="0.3">
@@ -57248,7 +57251,7 @@
         <v>6884</v>
       </c>
       <c r="B1877" s="2" t="s">
-        <v>7053</v>
+        <v>6848</v>
       </c>
     </row>
     <row r="1878" spans="1:2" x14ac:dyDescent="0.3">
@@ -57256,7 +57259,7 @@
         <v>6885</v>
       </c>
       <c r="B1878" s="2" t="s">
-        <v>111</v>
+        <v>7054</v>
       </c>
     </row>
     <row r="1879" spans="1:2" x14ac:dyDescent="0.3">
@@ -57264,7 +57267,7 @@
         <v>6886</v>
       </c>
       <c r="B1879" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1880" spans="1:2" x14ac:dyDescent="0.3">
@@ -57272,7 +57275,7 @@
         <v>6887</v>
       </c>
       <c r="B1880" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="1881" spans="1:2" x14ac:dyDescent="0.3">
@@ -57280,7 +57283,7 @@
         <v>6888</v>
       </c>
       <c r="B1881" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1882" spans="1:2" x14ac:dyDescent="0.3">
@@ -57288,7 +57291,7 @@
         <v>6889</v>
       </c>
       <c r="B1882" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1883" spans="1:2" x14ac:dyDescent="0.3">
@@ -57296,7 +57299,7 @@
         <v>6890</v>
       </c>
       <c r="B1883" s="2" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1884" spans="1:2" x14ac:dyDescent="0.3">
@@ -57304,7 +57307,7 @@
         <v>6891</v>
       </c>
       <c r="B1884" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="1885" spans="1:2" x14ac:dyDescent="0.3">
@@ -57312,7 +57315,7 @@
         <v>6892</v>
       </c>
       <c r="B1885" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1886" spans="1:2" x14ac:dyDescent="0.3">
@@ -57320,7 +57323,7 @@
         <v>6893</v>
       </c>
       <c r="B1886" s="2" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="1887" spans="1:2" x14ac:dyDescent="0.3">
@@ -57328,7 +57331,7 @@
         <v>6894</v>
       </c>
       <c r="B1887" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="1888" spans="1:2" x14ac:dyDescent="0.3">
@@ -57336,7 +57339,7 @@
         <v>6895</v>
       </c>
       <c r="B1888" s="2" t="s">
-        <v>5224</v>
+        <v>124</v>
       </c>
     </row>
     <row r="1889" spans="1:2" x14ac:dyDescent="0.3">
@@ -57344,7 +57347,7 @@
         <v>6896</v>
       </c>
       <c r="B1889" s="2" t="s">
-        <v>126</v>
+        <v>5224</v>
       </c>
     </row>
     <row r="1890" spans="1:2" x14ac:dyDescent="0.3">
@@ -57352,7 +57355,7 @@
         <v>6897</v>
       </c>
       <c r="B1890" s="2" t="s">
-        <v>6847</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1891" spans="1:2" x14ac:dyDescent="0.3">
@@ -57360,7 +57363,7 @@
         <v>6898</v>
       </c>
       <c r="B1891" s="2" t="s">
-        <v>7043</v>
+        <v>6848</v>
       </c>
     </row>
     <row r="1892" spans="1:2" x14ac:dyDescent="0.3">
@@ -57368,23 +57371,23 @@
         <v>6899</v>
       </c>
       <c r="B1892" s="2" t="s">
-        <v>7054</v>
+        <v>7044</v>
       </c>
     </row>
     <row r="1893" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1893" s="1" t="s">
-        <v>7038</v>
+        <v>6900</v>
       </c>
       <c r="B1893" s="2" t="s">
-        <v>7039</v>
+        <v>7055</v>
       </c>
     </row>
     <row r="1894" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1894" s="1" t="s">
-        <v>6900</v>
+        <v>7039</v>
       </c>
       <c r="B1894" s="2" t="s">
-        <v>7048</v>
+        <v>7040</v>
       </c>
     </row>
     <row r="1895" spans="1:2" x14ac:dyDescent="0.3">
@@ -57392,87 +57395,87 @@
         <v>6901</v>
       </c>
       <c r="B1895" s="2" t="s">
-        <v>6902</v>
+        <v>7049</v>
       </c>
     </row>
     <row r="1896" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1896" s="1" t="s">
+        <v>6902</v>
+      </c>
+      <c r="B1896" s="2" t="s">
         <v>6903</v>
-      </c>
-      <c r="B1896" s="2" t="s">
-        <v>6904</v>
       </c>
     </row>
     <row r="1897" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1897" s="1" t="s">
-        <v>7034</v>
+        <v>6904</v>
       </c>
       <c r="B1897" s="2" t="s">
-        <v>7035</v>
+        <v>6905</v>
       </c>
     </row>
     <row r="1898" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1898" s="1" t="s">
+        <v>7035</v>
+      </c>
+      <c r="B1898" s="2" t="s">
         <v>7036</v>
-      </c>
-      <c r="B1898" s="2" t="s">
-        <v>7037</v>
       </c>
     </row>
     <row r="1899" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1899" s="1" t="s">
-        <v>6905</v>
+        <v>7037</v>
       </c>
       <c r="B1899" s="2" t="s">
-        <v>6906</v>
+        <v>7038</v>
       </c>
     </row>
     <row r="1900" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1900" s="1" t="s">
+        <v>6906</v>
+      </c>
+      <c r="B1900" s="2" t="s">
         <v>6907</v>
-      </c>
-      <c r="B1900" s="2" t="s">
-        <v>6908</v>
       </c>
     </row>
     <row r="1901" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1901" s="1" t="s">
-        <v>7031</v>
+        <v>6908</v>
       </c>
       <c r="B1901" s="2" t="s">
-        <v>7032</v>
+        <v>6909</v>
       </c>
     </row>
     <row r="1902" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1902" s="1" t="s">
-        <v>6909</v>
+        <v>7032</v>
       </c>
       <c r="B1902" s="2" t="s">
-        <v>6910</v>
+        <v>7033</v>
       </c>
     </row>
     <row r="1903" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1903" s="1" t="s">
+        <v>6910</v>
+      </c>
+      <c r="B1903" s="2" t="s">
         <v>6911</v>
-      </c>
-      <c r="B1903" s="2" t="s">
-        <v>6912</v>
       </c>
     </row>
     <row r="1904" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1904" s="1" t="s">
+        <v>6912</v>
+      </c>
+      <c r="B1904" s="2" t="s">
         <v>6913</v>
-      </c>
-      <c r="B1904" s="2" t="s">
-        <v>6914</v>
       </c>
     </row>
     <row r="1905" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1905" s="1" t="s">
+        <v>6914</v>
+      </c>
+      <c r="B1905" s="2" t="s">
         <v>6915</v>
-      </c>
-      <c r="B1905" s="2" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="1906" spans="1:2" x14ac:dyDescent="0.3">
@@ -57480,31 +57483,31 @@
         <v>6916</v>
       </c>
       <c r="B1906" s="2" t="s">
-        <v>6917</v>
+        <v>311</v>
       </c>
     </row>
     <row r="1907" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1907" s="1" t="s">
+        <v>6917</v>
+      </c>
+      <c r="B1907" s="2" t="s">
         <v>6918</v>
-      </c>
-      <c r="B1907" s="2" t="s">
-        <v>6919</v>
       </c>
     </row>
     <row r="1908" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1908" s="1" t="s">
+        <v>6919</v>
+      </c>
+      <c r="B1908" s="2" t="s">
         <v>6920</v>
-      </c>
-      <c r="B1908" s="2" t="s">
-        <v>6921</v>
       </c>
     </row>
     <row r="1909" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1909" s="1" t="s">
+        <v>6921</v>
+      </c>
+      <c r="B1909" s="2" t="s">
         <v>6922</v>
-      </c>
-      <c r="B1909" s="2" t="s">
-        <v>7047</v>
       </c>
     </row>
     <row r="1910" spans="1:2" x14ac:dyDescent="0.3">
@@ -57512,7 +57515,7 @@
         <v>6923</v>
       </c>
       <c r="B1910" s="2" t="s">
-        <v>7046</v>
+        <v>7048</v>
       </c>
     </row>
     <row r="1911" spans="1:2" x14ac:dyDescent="0.3">
@@ -57520,7 +57523,7 @@
         <v>6924</v>
       </c>
       <c r="B1911" s="2" t="s">
-        <v>7043</v>
+        <v>7047</v>
       </c>
     </row>
     <row r="1912" spans="1:2" x14ac:dyDescent="0.3">
@@ -57528,15 +57531,15 @@
         <v>6925</v>
       </c>
       <c r="B1912" s="2" t="s">
-        <v>6926</v>
+        <v>7044</v>
       </c>
     </row>
     <row r="1913" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1913" s="1" t="s">
+        <v>6926</v>
+      </c>
+      <c r="B1913" s="2" t="s">
         <v>6927</v>
-      </c>
-      <c r="B1913" s="2" t="s">
-        <v>7055</v>
       </c>
     </row>
     <row r="1914" spans="1:2" x14ac:dyDescent="0.3">
@@ -57544,15 +57547,15 @@
         <v>6928</v>
       </c>
       <c r="B1914" s="2" t="s">
-        <v>6929</v>
+        <v>7056</v>
       </c>
     </row>
     <row r="1915" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1915" s="1" t="s">
+        <v>6929</v>
+      </c>
+      <c r="B1915" s="2" t="s">
         <v>6930</v>
-      </c>
-      <c r="B1915" s="2" t="s">
-        <v>7056</v>
       </c>
     </row>
     <row r="1916" spans="1:2" x14ac:dyDescent="0.3">
@@ -57568,119 +57571,119 @@
         <v>6932</v>
       </c>
       <c r="B1917" s="2" t="s">
-        <v>6933</v>
+        <v>7058</v>
       </c>
     </row>
     <row r="1918" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1918" s="1" t="s">
+        <v>6933</v>
+      </c>
+      <c r="B1918" s="2" t="s">
         <v>6934</v>
-      </c>
-      <c r="B1918" s="2" t="s">
-        <v>6935</v>
       </c>
     </row>
     <row r="1919" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1919" s="1" t="s">
+        <v>6935</v>
+      </c>
+      <c r="B1919" s="2" t="s">
         <v>6936</v>
-      </c>
-      <c r="B1919" s="2" t="s">
-        <v>6937</v>
       </c>
     </row>
     <row r="1920" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1920" s="1" t="s">
+        <v>6937</v>
+      </c>
+      <c r="B1920" s="2" t="s">
         <v>6938</v>
-      </c>
-      <c r="B1920" s="2" t="s">
-        <v>6939</v>
       </c>
     </row>
     <row r="1921" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1921" s="1" t="s">
+        <v>6939</v>
+      </c>
+      <c r="B1921" s="2" t="s">
         <v>6940</v>
-      </c>
-      <c r="B1921" s="2" t="s">
-        <v>6941</v>
       </c>
     </row>
     <row r="1922" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1922" s="1" t="s">
+        <v>6941</v>
+      </c>
+      <c r="B1922" s="2" t="s">
         <v>6942</v>
-      </c>
-      <c r="B1922" s="2" t="s">
-        <v>6943</v>
       </c>
     </row>
     <row r="1923" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1923" s="1" t="s">
+        <v>6943</v>
+      </c>
+      <c r="B1923" s="2" t="s">
         <v>6944</v>
-      </c>
-      <c r="B1923" s="2" t="s">
-        <v>6945</v>
       </c>
     </row>
     <row r="1924" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1924" s="1" t="s">
+        <v>6945</v>
+      </c>
+      <c r="B1924" s="2" t="s">
         <v>6946</v>
-      </c>
-      <c r="B1924" s="2" t="s">
-        <v>6947</v>
       </c>
     </row>
     <row r="1925" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1925" s="1" t="s">
+        <v>6947</v>
+      </c>
+      <c r="B1925" s="2" t="s">
         <v>6948</v>
-      </c>
-      <c r="B1925" s="2" t="s">
-        <v>6949</v>
       </c>
     </row>
     <row r="1926" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1926" s="1" t="s">
+        <v>6949</v>
+      </c>
+      <c r="B1926" s="2" t="s">
         <v>6950</v>
-      </c>
-      <c r="B1926" s="2" t="s">
-        <v>6951</v>
       </c>
     </row>
     <row r="1927" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1927" s="1" t="s">
+        <v>6951</v>
+      </c>
+      <c r="B1927" s="2" t="s">
         <v>6952</v>
-      </c>
-      <c r="B1927" s="2" t="s">
-        <v>6953</v>
       </c>
     </row>
     <row r="1928" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1928" s="1" t="s">
+        <v>6953</v>
+      </c>
+      <c r="B1928" s="2" t="s">
         <v>6954</v>
-      </c>
-      <c r="B1928" s="2" t="s">
-        <v>6955</v>
       </c>
     </row>
     <row r="1929" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1929" s="1" t="s">
+        <v>6955</v>
+      </c>
+      <c r="B1929" s="2" t="s">
         <v>6956</v>
-      </c>
-      <c r="B1929" s="2" t="s">
-        <v>6957</v>
       </c>
     </row>
     <row r="1930" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1930" s="1" t="s">
+        <v>6957</v>
+      </c>
+      <c r="B1930" s="2" t="s">
         <v>6958</v>
-      </c>
-      <c r="B1930" s="2" t="s">
-        <v>6959</v>
       </c>
     </row>
     <row r="1931" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1931" s="1" t="s">
+        <v>6959</v>
+      </c>
+      <c r="B1931" s="2" t="s">
         <v>6960</v>
-      </c>
-      <c r="B1931" s="2" t="s">
-        <v>7058</v>
       </c>
     </row>
     <row r="1932" spans="1:2" x14ac:dyDescent="0.3">
@@ -57688,7 +57691,7 @@
         <v>6961</v>
       </c>
       <c r="B1932" s="2" t="s">
-        <v>94</v>
+        <v>7059</v>
       </c>
     </row>
     <row r="1933" spans="1:2" x14ac:dyDescent="0.3">
@@ -57696,7 +57699,7 @@
         <v>6962</v>
       </c>
       <c r="B1933" s="2" t="s">
-        <v>6847</v>
+        <v>94</v>
       </c>
     </row>
     <row r="1934" spans="1:2" x14ac:dyDescent="0.3">
@@ -57704,7 +57707,7 @@
         <v>6963</v>
       </c>
       <c r="B1934" s="2" t="s">
-        <v>7058</v>
+        <v>6848</v>
       </c>
     </row>
     <row r="1935" spans="1:2" x14ac:dyDescent="0.3">
@@ -57712,7 +57715,7 @@
         <v>6964</v>
       </c>
       <c r="B1935" s="2" t="s">
-        <v>98</v>
+        <v>7059</v>
       </c>
     </row>
     <row r="1936" spans="1:2" x14ac:dyDescent="0.3">
@@ -57720,7 +57723,7 @@
         <v>6965</v>
       </c>
       <c r="B1936" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="1937" spans="1:2" x14ac:dyDescent="0.3">
@@ -57728,7 +57731,7 @@
         <v>6966</v>
       </c>
       <c r="B1937" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1938" spans="1:2" x14ac:dyDescent="0.3">
@@ -57736,7 +57739,7 @@
         <v>6967</v>
       </c>
       <c r="B1938" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="1939" spans="1:2" x14ac:dyDescent="0.3">
@@ -57744,7 +57747,7 @@
         <v>6968</v>
       </c>
       <c r="B1939" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="1940" spans="1:2" x14ac:dyDescent="0.3">
@@ -57752,7 +57755,7 @@
         <v>6969</v>
       </c>
       <c r="B1940" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1941" spans="1:2" x14ac:dyDescent="0.3">
@@ -57760,7 +57763,7 @@
         <v>6970</v>
       </c>
       <c r="B1941" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="1942" spans="1:2" x14ac:dyDescent="0.3">
@@ -57768,7 +57771,7 @@
         <v>6971</v>
       </c>
       <c r="B1942" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1943" spans="1:2" x14ac:dyDescent="0.3">
@@ -57776,7 +57779,7 @@
         <v>6972</v>
       </c>
       <c r="B1943" s="2" t="s">
-        <v>7052</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1944" spans="1:2" x14ac:dyDescent="0.3">
@@ -57784,7 +57787,7 @@
         <v>6973</v>
       </c>
       <c r="B1944" s="2" t="s">
-        <v>121</v>
+        <v>7053</v>
       </c>
     </row>
     <row r="1945" spans="1:2" x14ac:dyDescent="0.3">
@@ -57792,7 +57795,7 @@
         <v>6974</v>
       </c>
       <c r="B1945" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="1946" spans="1:2" x14ac:dyDescent="0.3">
@@ -57800,23 +57803,23 @@
         <v>6975</v>
       </c>
       <c r="B1946" s="2" t="s">
-        <v>5224</v>
+        <v>124</v>
       </c>
     </row>
     <row r="1947" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1947" s="1" t="s">
-        <v>7033</v>
+        <v>6976</v>
       </c>
       <c r="B1947" s="2" t="s">
-        <v>126</v>
+        <v>5224</v>
       </c>
     </row>
     <row r="1948" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1948" s="1" t="s">
-        <v>6976</v>
+        <v>7034</v>
       </c>
       <c r="B1948" s="2" t="s">
-        <v>6847</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1949" spans="1:2" x14ac:dyDescent="0.3">
@@ -57824,7 +57827,7 @@
         <v>6977</v>
       </c>
       <c r="B1949" s="2" t="s">
-        <v>7053</v>
+        <v>6848</v>
       </c>
     </row>
     <row r="1950" spans="1:2" x14ac:dyDescent="0.3">
@@ -57832,7 +57835,7 @@
         <v>6978</v>
       </c>
       <c r="B1950" s="2" t="s">
-        <v>111</v>
+        <v>7054</v>
       </c>
     </row>
     <row r="1951" spans="1:2" x14ac:dyDescent="0.3">
@@ -57840,7 +57843,7 @@
         <v>6979</v>
       </c>
       <c r="B1951" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1952" spans="1:2" x14ac:dyDescent="0.3">
@@ -57848,7 +57851,7 @@
         <v>6980</v>
       </c>
       <c r="B1952" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="1953" spans="1:2" x14ac:dyDescent="0.3">
@@ -57856,7 +57859,7 @@
         <v>6981</v>
       </c>
       <c r="B1953" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1954" spans="1:2" x14ac:dyDescent="0.3">
@@ -57864,7 +57867,7 @@
         <v>6982</v>
       </c>
       <c r="B1954" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1955" spans="1:2" x14ac:dyDescent="0.3">
@@ -57872,7 +57875,7 @@
         <v>6983</v>
       </c>
       <c r="B1955" s="2" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1956" spans="1:2" x14ac:dyDescent="0.3">
@@ -57880,7 +57883,7 @@
         <v>6984</v>
       </c>
       <c r="B1956" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="1957" spans="1:2" x14ac:dyDescent="0.3">
@@ -57888,7 +57891,7 @@
         <v>6985</v>
       </c>
       <c r="B1957" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1958" spans="1:2" x14ac:dyDescent="0.3">
@@ -57896,7 +57899,7 @@
         <v>6986</v>
       </c>
       <c r="B1958" s="2" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="1959" spans="1:2" x14ac:dyDescent="0.3">
@@ -57904,7 +57907,7 @@
         <v>6987</v>
       </c>
       <c r="B1959" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="1960" spans="1:2" x14ac:dyDescent="0.3">
@@ -57912,7 +57915,7 @@
         <v>6988</v>
       </c>
       <c r="B1960" s="2" t="s">
-        <v>5224</v>
+        <v>124</v>
       </c>
     </row>
     <row r="1961" spans="1:2" x14ac:dyDescent="0.3">
@@ -57920,7 +57923,7 @@
         <v>6989</v>
       </c>
       <c r="B1961" s="2" t="s">
-        <v>126</v>
+        <v>5224</v>
       </c>
     </row>
     <row r="1962" spans="1:2" x14ac:dyDescent="0.3">
@@ -57928,7 +57931,7 @@
         <v>6990</v>
       </c>
       <c r="B1962" s="2" t="s">
-        <v>6847</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1963" spans="1:2" x14ac:dyDescent="0.3">
@@ -57936,39 +57939,39 @@
         <v>6991</v>
       </c>
       <c r="B1963" s="2" t="s">
-        <v>6992</v>
+        <v>6848</v>
       </c>
     </row>
     <row r="1964" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1964" s="1" t="s">
+        <v>6992</v>
+      </c>
+      <c r="B1964" s="2" t="s">
         <v>6993</v>
-      </c>
-      <c r="B1964" s="2" t="s">
-        <v>6994</v>
       </c>
     </row>
     <row r="1965" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1965" s="1" t="s">
+        <v>6994</v>
+      </c>
+      <c r="B1965" s="2" t="s">
         <v>6995</v>
-      </c>
-      <c r="B1965" s="2" t="s">
-        <v>6996</v>
       </c>
     </row>
     <row r="1966" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1966" s="1" t="s">
+        <v>6996</v>
+      </c>
+      <c r="B1966" s="2" t="s">
         <v>6997</v>
-      </c>
-      <c r="B1966" s="2" t="s">
-        <v>6998</v>
       </c>
     </row>
     <row r="1967" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1967" s="1" t="s">
+        <v>6998</v>
+      </c>
+      <c r="B1967" s="2" t="s">
         <v>6999</v>
-      </c>
-      <c r="B1967" s="2" t="s">
-        <v>6998</v>
       </c>
     </row>
     <row r="1968" spans="1:2" x14ac:dyDescent="0.3">
@@ -57976,7 +57979,7 @@
         <v>7000</v>
       </c>
       <c r="B1968" s="2" t="s">
-        <v>2887</v>
+        <v>6999</v>
       </c>
     </row>
     <row r="1969" spans="1:2" x14ac:dyDescent="0.3">
@@ -57984,15 +57987,15 @@
         <v>7001</v>
       </c>
       <c r="B1969" s="2" t="s">
-        <v>7002</v>
+        <v>2887</v>
       </c>
     </row>
     <row r="1970" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1970" s="1" t="s">
+        <v>7002</v>
+      </c>
+      <c r="B1970" s="2" t="s">
         <v>7003</v>
-      </c>
-      <c r="B1970" s="2" t="s">
-        <v>6926</v>
       </c>
     </row>
     <row r="1971" spans="1:2" x14ac:dyDescent="0.3">
@@ -58000,23 +58003,23 @@
         <v>7004</v>
       </c>
       <c r="B1971" s="2" t="s">
-        <v>7005</v>
+        <v>6927</v>
       </c>
     </row>
     <row r="1972" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1972" s="1" t="s">
+        <v>7005</v>
+      </c>
+      <c r="B1972" s="2" t="s">
         <v>7006</v>
-      </c>
-      <c r="B1972" s="2" t="s">
-        <v>7007</v>
       </c>
     </row>
     <row r="1973" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1973" s="1" t="s">
+        <v>7007</v>
+      </c>
+      <c r="B1973" s="2" t="s">
         <v>7008</v>
-      </c>
-      <c r="B1973" s="2" t="s">
-        <v>7050</v>
       </c>
     </row>
     <row r="1974" spans="1:2" x14ac:dyDescent="0.3">
@@ -58024,7 +58027,7 @@
         <v>7009</v>
       </c>
       <c r="B1974" s="2" t="s">
-        <v>7050</v>
+        <v>7051</v>
       </c>
     </row>
     <row r="1975" spans="1:2" x14ac:dyDescent="0.3">
@@ -58032,23 +58035,23 @@
         <v>7010</v>
       </c>
       <c r="B1975" s="2" t="s">
-        <v>7011</v>
+        <v>7051</v>
       </c>
     </row>
     <row r="1976" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1976" s="1" t="s">
+        <v>7011</v>
+      </c>
+      <c r="B1976" s="2" t="s">
         <v>7012</v>
-      </c>
-      <c r="B1976" s="2" t="s">
-        <v>7013</v>
       </c>
     </row>
     <row r="1977" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1977" s="1" t="s">
+        <v>7013</v>
+      </c>
+      <c r="B1977" s="2" t="s">
         <v>7014</v>
-      </c>
-      <c r="B1977" s="2" t="s">
-        <v>7050</v>
       </c>
     </row>
     <row r="1978" spans="1:2" x14ac:dyDescent="0.3">
@@ -58056,7 +58059,7 @@
         <v>7015</v>
       </c>
       <c r="B1978" s="2" t="s">
-        <v>7050</v>
+        <v>7051</v>
       </c>
     </row>
     <row r="1979" spans="1:2" x14ac:dyDescent="0.3">
@@ -58064,7 +58067,7 @@
         <v>7016</v>
       </c>
       <c r="B1979" s="2" t="s">
-        <v>7011</v>
+        <v>7051</v>
       </c>
     </row>
     <row r="1980" spans="1:2" x14ac:dyDescent="0.3">
@@ -58072,23 +58075,23 @@
         <v>7017</v>
       </c>
       <c r="B1980" s="2" t="s">
-        <v>7018</v>
+        <v>7012</v>
       </c>
     </row>
     <row r="1981" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1981" s="1" t="s">
+        <v>7018</v>
+      </c>
+      <c r="B1981" s="2" t="s">
         <v>7019</v>
-      </c>
-      <c r="B1981" s="2" t="s">
-        <v>7020</v>
       </c>
     </row>
     <row r="1982" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1982" s="1" t="s">
+        <v>7020</v>
+      </c>
+      <c r="B1982" s="2" t="s">
         <v>7021</v>
-      </c>
-      <c r="B1982" s="2" t="s">
-        <v>7049</v>
       </c>
     </row>
     <row r="1983" spans="1:2" x14ac:dyDescent="0.3">
@@ -58096,15 +58099,15 @@
         <v>7022</v>
       </c>
       <c r="B1983" s="2" t="s">
-        <v>7023</v>
+        <v>7050</v>
       </c>
     </row>
     <row r="1984" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1984" s="1" t="s">
+        <v>7023</v>
+      </c>
+      <c r="B1984" s="2" t="s">
         <v>7024</v>
-      </c>
-      <c r="B1984" s="2" t="s">
-        <v>7013</v>
       </c>
     </row>
     <row r="1985" spans="1:2" x14ac:dyDescent="0.3">
@@ -58112,7 +58115,7 @@
         <v>7025</v>
       </c>
       <c r="B1985" s="2" t="s">
-        <v>51</v>
+        <v>7014</v>
       </c>
     </row>
     <row r="1986" spans="1:2" x14ac:dyDescent="0.3">
@@ -58120,7 +58123,7 @@
         <v>7026</v>
       </c>
       <c r="B1986" s="2" t="s">
-        <v>111</v>
+        <v>51</v>
       </c>
     </row>
     <row r="1987" spans="1:2" x14ac:dyDescent="0.3">
@@ -58128,15 +58131,15 @@
         <v>7027</v>
       </c>
       <c r="B1987" s="2" t="s">
-        <v>7028</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1988" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1988" s="1" t="s">
+        <v>7028</v>
+      </c>
+      <c r="B1988" s="2" t="s">
         <v>7029</v>
-      </c>
-      <c r="B1988" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="1989" spans="1:2" x14ac:dyDescent="0.3">
@@ -58144,36 +58147,36 @@
         <v>7030</v>
       </c>
       <c r="B1989" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1990" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1990" s="1" t="s">
-        <v>7040</v>
+        <v>7031</v>
       </c>
       <c r="B1990" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="1991" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1991" s="1" t="s">
         <v>7041</v>
       </c>
-    </row>
-    <row r="1991" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1991" s="16" t="s">
+      <c r="B1991" s="2" t="s">
         <v>7042</v>
       </c>
-      <c r="B1991" s="2" t="s">
+    </row>
+    <row r="1992" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1992" s="16" t="s">
         <v>7043</v>
       </c>
-    </row>
-    <row r="1992" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1992" s="1" t="s">
+      <c r="B1992" s="2" t="s">
         <v>7044</v>
-      </c>
-      <c r="B1992" s="2" t="s">
-        <v>7045</v>
       </c>
     </row>
     <row r="1993" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1993" s="1" t="s">
-        <v>7065</v>
+        <v>7045</v>
       </c>
       <c r="B1993" s="2" t="s">
         <v>7046</v>
@@ -58181,15 +58184,15 @@
     </row>
     <row r="1994" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1994" s="1" t="s">
-        <v>7051</v>
+        <v>7066</v>
       </c>
       <c r="B1994" s="2" t="s">
-        <v>6550</v>
+        <v>7047</v>
       </c>
     </row>
     <row r="1995" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1995" s="1" t="s">
-        <v>7073</v>
+        <v>7052</v>
       </c>
       <c r="B1995" s="2" t="s">
         <v>6550</v>
@@ -58205,36 +58208,44 @@
     </row>
     <row r="1997" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1997" s="1" t="s">
-        <v>7059</v>
+        <v>7075</v>
       </c>
       <c r="B1997" s="2" t="s">
-        <v>7060</v>
+        <v>6550</v>
       </c>
     </row>
     <row r="1998" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1998" s="1" t="s">
+        <v>7060</v>
+      </c>
+      <c r="B1998" s="2" t="s">
         <v>7061</v>
-      </c>
-      <c r="B1998" s="2" t="s">
-        <v>7062</v>
       </c>
     </row>
     <row r="1999" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1999" s="1" t="s">
+        <v>7062</v>
+      </c>
+      <c r="B1999" s="2" t="s">
         <v>7063</v>
-      </c>
-      <c r="B1999" s="2" t="s">
-        <v>7064</v>
       </c>
     </row>
     <row r="2000" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2000" s="1" t="s">
-        <v>7066</v>
+        <v>7064</v>
+      </c>
+      <c r="B2000" s="2" t="s">
+        <v>7065</v>
       </c>
     </row>
     <row r="2001" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2001" s="1" t="s">
         <v>7067</v>
+      </c>
+    </row>
+    <row r="2002" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2002" s="1" t="s">
+        <v>7068</v>
       </c>
     </row>
   </sheetData>
@@ -58251,7 +58262,7 @@
       <formula>AND($B2 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A1629 A1992 A1995:A1997 A2000:A2001 A1686:A1688 A1690:A1990 A2004:A1048576">
+  <conditionalFormatting sqref="A2:A1629 A1993 A1996:A1998 A2001:A2002 A1686:A1688 A1690:A1991 A2005:A1048576">
     <cfRule type="expression" dxfId="11" priority="44">
       <formula>AND( $A2 = "", OR( $B2 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
@@ -58266,19 +58277,19 @@
       <formula>AND( $A1630 = "", OR( $B1630 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1994">
+  <conditionalFormatting sqref="A1995">
     <cfRule type="expression" dxfId="8" priority="1">
-      <formula>AND( $A1994 = "", OR( $B1994 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
+      <formula>AND( $A1995 = "", OR( $B1995 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1993">
+  <conditionalFormatting sqref="A1994">
     <cfRule type="expression" dxfId="7" priority="48">
-      <formula>AND( $A1993 = "", OR( $B2002 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
+      <formula>AND( $A1994 = "", OR( $B2003 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1999">
+  <conditionalFormatting sqref="A2000">
     <cfRule type="expression" dxfId="6" priority="51">
-      <formula>AND( $A1999 = "", OR( $B2003 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
+      <formula>AND( $A2000 = "", OR( $B2004 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Moved sijoituslupa's strings to i18n excel.
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11850" uniqueCount="7251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11888" uniqueCount="7285">
   <si>
     <t>fi</t>
   </si>
@@ -21820,6 +21820,108 @@
   </si>
   <si>
     <t>yleiset-alueet-maksaja.yritys.vastuuhenkilo.yhteystiedot.email</t>
+  </si>
+  <si>
+    <t>sijoituslupa-sijoituksen-tarkoitus._group_label</t>
+  </si>
+  <si>
+    <t>Sijoituksen tarkoitus</t>
+  </si>
+  <si>
+    <t>sijoituslupa-sijoituksen-tarkoitus.sijoituksen-tarkoitus.sahko</t>
+  </si>
+  <si>
+    <t>sijoituslupa-sijoituksen-tarkoitus.sijoituksen-tarkoitus.tele</t>
+  </si>
+  <si>
+    <t>Tele</t>
+  </si>
+  <si>
+    <t>sijoituslupa-sijoituksen-tarkoitus.sijoituksen-tarkoitus.kaivo-(tele/sahko)</t>
+  </si>
+  <si>
+    <t>Kaivo (tele/sähkö)</t>
+  </si>
+  <si>
+    <t>sijoituslupa-sijoituksen-tarkoitus.sijoituksen-tarkoitus.jakokaappi-(tele/sahko)</t>
+  </si>
+  <si>
+    <t>Jakokaappi (tele/sähkö)</t>
+  </si>
+  <si>
+    <t>sijoituslupa-sijoituksen-tarkoitus.sijoituksen-tarkoitus.kaukolampo</t>
+  </si>
+  <si>
+    <t>Kaukolämpö</t>
+  </si>
+  <si>
+    <t>sijoituslupa-sijoituksen-tarkoitus.sijoituksen-tarkoitus.kaivo-(kaukolampo)</t>
+  </si>
+  <si>
+    <t>Kaivo (kaukolämpö)</t>
+  </si>
+  <si>
+    <t>sijoituslupa-sijoituksen-tarkoitus.sijoituksen-tarkoitus.liikennevalo</t>
+  </si>
+  <si>
+    <t>Liikennevalo</t>
+  </si>
+  <si>
+    <t>sijoituslupa-sijoituksen-tarkoitus.sijoituksen-tarkoitus.katuvalo</t>
+  </si>
+  <si>
+    <t>Katuvalo</t>
+  </si>
+  <si>
+    <t>sijoituslupa-sijoituksen-tarkoitus.sijoituksen-tarkoitus.jate--tai-sadevesi</t>
+  </si>
+  <si>
+    <t>Jäte- tai sadevesi</t>
+  </si>
+  <si>
+    <t>sijoituslupa-sijoituksen-tarkoitus.sijoituksen-tarkoitus.kaivo-(vesi,-jate--tai-sadevesi)</t>
+  </si>
+  <si>
+    <t>Kaivo (vesi, jäte- tai sadevesi)</t>
+  </si>
+  <si>
+    <t>sijoituslupa-sijoituksen-tarkoitus.sijoituksen-tarkoitus.vesijohto</t>
+  </si>
+  <si>
+    <t>sijoituslupa-sijoituksen-tarkoitus.sijoituksen-tarkoitus.muu</t>
+  </si>
+  <si>
+    <t>sijoituslupa-sijoituksen-tarkoitus.sijoituksen-tarkoitus._group_label</t>
+  </si>
+  <si>
+    <t>sijoituslupa-sijoituksen-tarkoitus.muu-sijoituksen-tarkoitus</t>
+  </si>
+  <si>
+    <t>Muu sijoituksen tarkoitus, ellei mikään edellisistä</t>
+  </si>
+  <si>
+    <t>sijoituslupa-sijoituksen-tarkoitus.lisatietoja-sijoituskohteesta</t>
+  </si>
+  <si>
+    <t>Lisätietoja kohteesta</t>
+  </si>
+  <si>
+    <t>attachmentType.yleiset-alueet.rakennuspiirros</t>
+  </si>
+  <si>
+    <t>Rakennuspiirros</t>
+  </si>
+  <si>
+    <t>attachmentType.yleiset-alueet.suunnitelmakartta</t>
+  </si>
+  <si>
+    <t>Suunnitelmakartta</t>
+  </si>
+  <si>
+    <t>attachmentType.yleiset-alueet.muu</t>
+  </si>
+  <si>
+    <t>muu</t>
   </si>
 </sst>
 </file>
@@ -22336,7 +22438,17 @@
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -37452,10 +37564,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2002"/>
+  <dimension ref="A1:D2023"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1732" workbookViewId="0">
-      <selection activeCell="A1753" sqref="A1753"/>
+    <sheetView tabSelected="1" topLeftCell="A1823" workbookViewId="0">
+      <selection activeCell="A1844" sqref="A1844"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -56552,258 +56664,258 @@
     </row>
     <row r="1784" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1784" s="1" t="s">
-        <v>7153</v>
+        <v>7164</v>
       </c>
       <c r="B1784" s="2" t="s">
-        <v>6846</v>
+        <v>94</v>
       </c>
     </row>
     <row r="1785" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1785" s="1" t="s">
-        <v>7164</v>
+        <v>7165</v>
       </c>
       <c r="B1785" s="2" t="s">
-        <v>94</v>
+        <v>7166</v>
       </c>
     </row>
     <row r="1786" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1786" s="1" t="s">
-        <v>7165</v>
+        <v>7167</v>
       </c>
       <c r="B1786" s="2" t="s">
-        <v>7166</v>
+        <v>94</v>
       </c>
     </row>
     <row r="1787" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1787" s="1" t="s">
-        <v>7167</v>
+        <v>7168</v>
       </c>
       <c r="B1787" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="1788" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1788" s="1" t="s">
-        <v>7168</v>
+        <v>7169</v>
       </c>
       <c r="B1788" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1789" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1789" s="1" t="s">
-        <v>7169</v>
+        <v>7170</v>
       </c>
       <c r="B1789" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="1790" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1790" s="1" t="s">
-        <v>7170</v>
+        <v>7171</v>
       </c>
       <c r="B1790" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="1791" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1791" s="1" t="s">
-        <v>7171</v>
+        <v>7172</v>
       </c>
       <c r="B1791" s="2" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1792" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1792" s="1" t="s">
-        <v>7172</v>
+        <v>7173</v>
       </c>
       <c r="B1792" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="1793" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1793" s="1" t="s">
-        <v>7173</v>
+        <v>7174</v>
       </c>
       <c r="B1793" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1794" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1794" s="1" t="s">
-        <v>7174</v>
+        <v>7175</v>
       </c>
       <c r="B1794" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1795" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1795" s="1" t="s">
-        <v>7175</v>
+        <v>7176</v>
       </c>
       <c r="B1795" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="1796" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1796" s="1" t="s">
-        <v>7176</v>
+        <v>7177</v>
       </c>
       <c r="B1796" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1797" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1797" s="1" t="s">
-        <v>7177</v>
+        <v>7178</v>
       </c>
       <c r="B1797" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="1798" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1798" s="1" t="s">
-        <v>7178</v>
+        <v>6847</v>
       </c>
       <c r="B1798" s="2" t="s">
-        <v>124</v>
+        <v>6848</v>
       </c>
     </row>
     <row r="1799" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1799" s="1" t="s">
-        <v>6847</v>
+        <v>6849</v>
       </c>
       <c r="B1799" s="2" t="s">
-        <v>6848</v>
+        <v>6842</v>
       </c>
     </row>
     <row r="1800" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1800" s="1" t="s">
-        <v>6849</v>
+        <v>6850</v>
       </c>
       <c r="B1800" s="2" t="s">
-        <v>6842</v>
+        <v>109</v>
       </c>
     </row>
     <row r="1801" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1801" s="1" t="s">
-        <v>6850</v>
+        <v>7179</v>
       </c>
       <c r="B1801" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1802" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1802" s="1" t="s">
-        <v>7179</v>
+        <v>7180</v>
       </c>
       <c r="B1802" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="1803" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1803" s="1" t="s">
-        <v>7180</v>
+        <v>7181</v>
       </c>
       <c r="B1803" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1804" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1804" s="1" t="s">
-        <v>7181</v>
+        <v>7182</v>
       </c>
       <c r="B1804" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1805" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1805" s="1" t="s">
-        <v>7182</v>
+        <v>7183</v>
       </c>
       <c r="B1805" s="2" t="s">
-        <v>117</v>
+        <v>7184</v>
       </c>
     </row>
     <row r="1806" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1806" s="1" t="s">
-        <v>7183</v>
+        <v>7185</v>
       </c>
       <c r="B1806" s="2" t="s">
-        <v>7184</v>
+        <v>98</v>
       </c>
     </row>
     <row r="1807" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1807" s="1" t="s">
-        <v>7185</v>
+        <v>7186</v>
       </c>
       <c r="B1807" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1808" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1808" s="1" t="s">
-        <v>7186</v>
+        <v>7187</v>
       </c>
       <c r="B1808" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="1809" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1809" s="1" t="s">
-        <v>7187</v>
+        <v>7188</v>
       </c>
       <c r="B1809" s="2" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
     </row>
     <row r="1810" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1810" s="1" t="s">
-        <v>7188</v>
+        <v>7189</v>
       </c>
       <c r="B1810" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1811" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1811" s="1" t="s">
-        <v>7189</v>
+        <v>7190</v>
       </c>
       <c r="B1811" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="1812" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1812" s="1" t="s">
-        <v>7190</v>
-      </c>
-      <c r="B1812" s="2" t="s">
         <v>124</v>
+      </c>
+    </row>
+    <row r="1813" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1813" s="1" t="s">
+        <v>7076</v>
+      </c>
+      <c r="B1813" s="2" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="1814" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1814" s="1" t="s">
-        <v>7076</v>
+        <v>7077</v>
       </c>
       <c r="B1814" s="2" t="s">
-        <v>200</v>
+        <v>7072</v>
       </c>
     </row>
     <row r="1815" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1815" s="1" t="s">
-        <v>7077</v>
+        <v>7078</v>
       </c>
       <c r="B1815" s="2" t="s">
-        <v>7072</v>
-      </c>
-    </row>
-    <row r="1816" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1816" s="1" t="s">
-        <v>7078</v>
-      </c>
-      <c r="B1816" s="2" t="s">
         <v>6851</v>
+      </c>
+    </row>
+    <row r="1817" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1817" s="1" t="s">
+        <v>7153</v>
+      </c>
+      <c r="B1817" s="2" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="1818" spans="1:2" x14ac:dyDescent="0.3">
@@ -56832,1419 +56944,1571 @@
     </row>
     <row r="1822" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1822" s="1" t="s">
-        <v>7116</v>
+        <v>7251</v>
       </c>
       <c r="B1822" s="2" t="s">
-        <v>6852</v>
+        <v>7252</v>
       </c>
     </row>
     <row r="1823" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1823" s="1" t="s">
-        <v>7154</v>
+        <v>7253</v>
       </c>
       <c r="B1823" s="2" t="s">
-        <v>7155</v>
+        <v>566</v>
       </c>
     </row>
     <row r="1824" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1824" s="1" t="s">
-        <v>7156</v>
+        <v>7254</v>
       </c>
       <c r="B1824" s="2" t="s">
-        <v>6853</v>
+        <v>7255</v>
       </c>
     </row>
     <row r="1825" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1825" s="1" t="s">
-        <v>7157</v>
+        <v>7256</v>
       </c>
       <c r="B1825" s="2" t="s">
-        <v>6854</v>
+        <v>7257</v>
+      </c>
+    </row>
+    <row r="1826" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1826" s="1" t="s">
+        <v>7258</v>
+      </c>
+      <c r="B1826" s="2" t="s">
+        <v>7259</v>
       </c>
     </row>
     <row r="1827" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1827" s="1" t="s">
-        <v>6855</v>
+        <v>7260</v>
       </c>
       <c r="B1827" s="2" t="s">
-        <v>6835</v>
+        <v>7261</v>
       </c>
     </row>
     <row r="1828" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1828" s="1" t="s">
-        <v>6856</v>
+        <v>7262</v>
       </c>
       <c r="B1828" s="2" t="s">
-        <v>6857</v>
+        <v>7263</v>
       </c>
     </row>
     <row r="1829" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1829" s="1" t="s">
-        <v>6858</v>
+        <v>7264</v>
       </c>
       <c r="B1829" s="2" t="s">
-        <v>6859</v>
+        <v>7265</v>
       </c>
     </row>
     <row r="1830" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1830" s="1" t="s">
-        <v>6860</v>
+        <v>7266</v>
       </c>
       <c r="B1830" s="2" t="s">
-        <v>6861</v>
+        <v>7267</v>
       </c>
     </row>
     <row r="1831" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1831" s="1" t="s">
-        <v>6862</v>
+        <v>7268</v>
       </c>
       <c r="B1831" s="2" t="s">
-        <v>6863</v>
+        <v>7269</v>
       </c>
     </row>
     <row r="1832" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1832" s="1" t="s">
-        <v>7161</v>
+        <v>7270</v>
       </c>
       <c r="B1832" s="2" t="s">
-        <v>7162</v>
+        <v>7271</v>
       </c>
     </row>
     <row r="1833" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1833" s="1" t="s">
-        <v>7163</v>
+        <v>7272</v>
       </c>
       <c r="B1833" s="2" t="s">
-        <v>1665</v>
-      </c>
-    </row>
-    <row r="1835" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1835" s="1" t="s">
-        <v>7119</v>
-      </c>
-      <c r="B1835" s="2" t="s">
-        <v>7120</v>
+        <v>596</v>
+      </c>
+    </row>
+    <row r="1834" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1834" s="1" t="s">
+        <v>7273</v>
+      </c>
+      <c r="B1834" s="2" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="1836" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1836" s="1" t="s">
-        <v>7121</v>
+        <v>7274</v>
       </c>
       <c r="B1836" s="2" t="s">
-        <v>7122</v>
+        <v>7252</v>
       </c>
     </row>
     <row r="1837" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1837" s="1" t="s">
-        <v>7123</v>
+        <v>7275</v>
       </c>
       <c r="B1837" s="2" t="s">
-        <v>7124</v>
+        <v>7276</v>
       </c>
     </row>
     <row r="1838" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1838" s="1" t="s">
-        <v>7125</v>
+        <v>7277</v>
       </c>
       <c r="B1838" s="2" t="s">
-        <v>7126</v>
-      </c>
-    </row>
-    <row r="1839" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1839" s="1" t="s">
-        <v>7127</v>
-      </c>
-      <c r="B1839" s="2" t="s">
-        <v>6842</v>
+        <v>7278</v>
       </c>
     </row>
     <row r="1840" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1840" s="1" t="s">
-        <v>7128</v>
+        <v>7116</v>
       </c>
       <c r="B1840" s="2" t="s">
-        <v>109</v>
+        <v>6852</v>
       </c>
     </row>
     <row r="1841" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1841" s="1" t="s">
-        <v>7129</v>
+        <v>7154</v>
       </c>
       <c r="B1841" s="2" t="s">
-        <v>111</v>
+        <v>7155</v>
       </c>
     </row>
     <row r="1842" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1842" s="1" t="s">
-        <v>7130</v>
+        <v>7156</v>
       </c>
       <c r="B1842" s="2" t="s">
-        <v>113</v>
+        <v>6853</v>
       </c>
     </row>
     <row r="1843" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1843" s="1" t="s">
-        <v>7131</v>
+        <v>7157</v>
       </c>
       <c r="B1843" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="1844" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1844" s="1" t="s">
-        <v>7132</v>
-      </c>
-      <c r="B1844" s="2" t="s">
-        <v>117</v>
+        <v>6854</v>
       </c>
     </row>
     <row r="1845" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1845" s="1" t="s">
-        <v>7133</v>
+        <v>6855</v>
       </c>
       <c r="B1845" s="2" t="s">
-        <v>6844</v>
+        <v>6835</v>
       </c>
     </row>
     <row r="1846" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1846" s="1" t="s">
-        <v>7134</v>
+        <v>6856</v>
       </c>
       <c r="B1846" s="2" t="s">
-        <v>6922</v>
+        <v>6857</v>
       </c>
     </row>
     <row r="1847" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1847" s="1" t="s">
-        <v>7135</v>
+        <v>6858</v>
       </c>
       <c r="B1847" s="2" t="s">
-        <v>7136</v>
+        <v>6859</v>
       </c>
     </row>
     <row r="1848" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1848" s="1" t="s">
-        <v>7137</v>
+        <v>6860</v>
       </c>
       <c r="B1848" s="2" t="s">
-        <v>7138</v>
+        <v>6861</v>
       </c>
     </row>
     <row r="1849" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1849" s="1" t="s">
-        <v>7139</v>
+        <v>6862</v>
       </c>
       <c r="B1849" s="2" t="s">
-        <v>7140</v>
+        <v>6863</v>
       </c>
     </row>
     <row r="1850" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1850" s="1" t="s">
-        <v>7141</v>
+        <v>7161</v>
       </c>
       <c r="B1850" s="2" t="s">
-        <v>7142</v>
+        <v>7162</v>
       </c>
     </row>
     <row r="1851" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1851" s="1" t="s">
-        <v>7143</v>
+        <v>7163</v>
       </c>
       <c r="B1851" s="2" t="s">
-        <v>7144</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="1852" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1852" s="1" t="s">
-        <v>7145</v>
+        <v>7279</v>
       </c>
       <c r="B1852" s="2" t="s">
-        <v>7146</v>
+        <v>7280</v>
       </c>
     </row>
     <row r="1853" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1853" s="1" t="s">
-        <v>7147</v>
+        <v>7281</v>
       </c>
       <c r="B1853" s="2" t="s">
-        <v>7148</v>
+        <v>7282</v>
       </c>
     </row>
     <row r="1854" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1854" s="1" t="s">
-        <v>7149</v>
+        <v>7283</v>
       </c>
       <c r="B1854" s="2" t="s">
-        <v>6922</v>
-      </c>
-    </row>
-    <row r="1855" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1855" s="1" t="s">
-        <v>7150</v>
-      </c>
-      <c r="B1855" s="2" t="s">
-        <v>7136</v>
+        <v>7284</v>
       </c>
     </row>
     <row r="1856" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1856" s="1" t="s">
-        <v>7151</v>
+        <v>7119</v>
       </c>
       <c r="B1856" s="2" t="s">
-        <v>7138</v>
+        <v>7120</v>
       </c>
     </row>
     <row r="1857" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1857" s="1" t="s">
-        <v>7152</v>
+        <v>7121</v>
       </c>
       <c r="B1857" s="2" t="s">
-        <v>7140</v>
+        <v>7122</v>
+      </c>
+    </row>
+    <row r="1858" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1858" s="1" t="s">
+        <v>7123</v>
+      </c>
+      <c r="B1858" s="2" t="s">
+        <v>7124</v>
       </c>
     </row>
     <row r="1859" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1859" s="1" t="s">
-        <v>6864</v>
+        <v>7125</v>
       </c>
       <c r="B1859" s="2" t="s">
-        <v>6865</v>
+        <v>7126</v>
       </c>
     </row>
     <row r="1860" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1860" s="1" t="s">
-        <v>6866</v>
+        <v>7127</v>
       </c>
       <c r="B1860" s="2" t="s">
-        <v>6867</v>
+        <v>6842</v>
       </c>
     </row>
     <row r="1861" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1861" s="1" t="s">
-        <v>6868</v>
+        <v>7128</v>
       </c>
       <c r="B1861" s="2" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
     </row>
     <row r="1862" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1862" s="1" t="s">
-        <v>6869</v>
+        <v>7129</v>
       </c>
       <c r="B1862" s="2" t="s">
-        <v>6848</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1863" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1863" s="1" t="s">
-        <v>6870</v>
+        <v>7130</v>
       </c>
       <c r="B1863" s="2" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
     </row>
     <row r="1864" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1864" s="1" t="s">
-        <v>6871</v>
+        <v>7131</v>
       </c>
       <c r="B1864" s="2" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1865" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1865" s="1" t="s">
-        <v>6872</v>
+        <v>7132</v>
       </c>
       <c r="B1865" s="2" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1866" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1866" s="1" t="s">
-        <v>6873</v>
+        <v>7133</v>
       </c>
       <c r="B1866" s="2" t="s">
-        <v>102</v>
+        <v>6844</v>
       </c>
     </row>
     <row r="1867" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1867" s="1" t="s">
-        <v>6874</v>
+        <v>7134</v>
       </c>
       <c r="B1867" s="2" t="s">
-        <v>104</v>
+        <v>6922</v>
       </c>
     </row>
     <row r="1868" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1868" s="1" t="s">
-        <v>6875</v>
+        <v>7135</v>
       </c>
       <c r="B1868" s="2" t="s">
-        <v>111</v>
+        <v>7136</v>
       </c>
     </row>
     <row r="1869" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1869" s="1" t="s">
-        <v>6876</v>
+        <v>7137</v>
       </c>
       <c r="B1869" s="2" t="s">
-        <v>113</v>
+        <v>7138</v>
       </c>
     </row>
     <row r="1870" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1870" s="1" t="s">
-        <v>6877</v>
+        <v>7139</v>
       </c>
       <c r="B1870" s="2" t="s">
-        <v>115</v>
+        <v>7140</v>
       </c>
     </row>
     <row r="1871" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1871" s="1" t="s">
-        <v>6878</v>
+        <v>7141</v>
       </c>
       <c r="B1871" s="2" t="s">
-        <v>117</v>
+        <v>7142</v>
       </c>
     </row>
     <row r="1872" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1872" s="1" t="s">
-        <v>6879</v>
+        <v>7143</v>
       </c>
       <c r="B1872" s="2" t="s">
-        <v>7053</v>
+        <v>7144</v>
       </c>
     </row>
     <row r="1873" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1873" s="1" t="s">
-        <v>6880</v>
+        <v>7145</v>
       </c>
       <c r="B1873" s="2" t="s">
-        <v>121</v>
+        <v>7146</v>
       </c>
     </row>
     <row r="1874" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1874" s="1" t="s">
-        <v>6881</v>
+        <v>7147</v>
       </c>
       <c r="B1874" s="2" t="s">
-        <v>124</v>
+        <v>7148</v>
       </c>
     </row>
     <row r="1875" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1875" s="1" t="s">
-        <v>6882</v>
+        <v>7149</v>
       </c>
       <c r="B1875" s="2" t="s">
-        <v>5224</v>
+        <v>6922</v>
       </c>
     </row>
     <row r="1876" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1876" s="1" t="s">
-        <v>6883</v>
+        <v>7150</v>
       </c>
       <c r="B1876" s="2" t="s">
-        <v>126</v>
+        <v>7136</v>
       </c>
     </row>
     <row r="1877" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1877" s="1" t="s">
-        <v>6884</v>
+        <v>7151</v>
       </c>
       <c r="B1877" s="2" t="s">
-        <v>6848</v>
+        <v>7138</v>
       </c>
     </row>
     <row r="1878" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1878" s="1" t="s">
-        <v>6885</v>
+        <v>7152</v>
       </c>
       <c r="B1878" s="2" t="s">
-        <v>7054</v>
-      </c>
-    </row>
-    <row r="1879" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1879" s="1" t="s">
-        <v>6886</v>
-      </c>
-      <c r="B1879" s="2" t="s">
-        <v>111</v>
+        <v>7140</v>
       </c>
     </row>
     <row r="1880" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1880" s="1" t="s">
-        <v>6887</v>
+        <v>6864</v>
       </c>
       <c r="B1880" s="2" t="s">
-        <v>113</v>
+        <v>6865</v>
       </c>
     </row>
     <row r="1881" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1881" s="1" t="s">
-        <v>6888</v>
+        <v>6866</v>
       </c>
       <c r="B1881" s="2" t="s">
-        <v>115</v>
+        <v>6867</v>
       </c>
     </row>
     <row r="1882" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1882" s="1" t="s">
-        <v>6889</v>
+        <v>6868</v>
       </c>
       <c r="B1882" s="2" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="1883" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1883" s="1" t="s">
-        <v>6890</v>
+        <v>6869</v>
       </c>
       <c r="B1883" s="2" t="s">
-        <v>119</v>
+        <v>6848</v>
       </c>
     </row>
     <row r="1884" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1884" s="1" t="s">
-        <v>6891</v>
+        <v>6870</v>
       </c>
       <c r="B1884" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="1885" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1885" s="1" t="s">
-        <v>6892</v>
+        <v>6871</v>
       </c>
       <c r="B1885" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="1886" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1886" s="1" t="s">
-        <v>6893</v>
+        <v>6872</v>
       </c>
       <c r="B1886" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1887" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1887" s="1" t="s">
-        <v>6894</v>
+        <v>6873</v>
       </c>
       <c r="B1887" s="2" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
     </row>
     <row r="1888" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1888" s="1" t="s">
-        <v>6895</v>
+        <v>6874</v>
       </c>
       <c r="B1888" s="2" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
     </row>
     <row r="1889" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1889" s="1" t="s">
-        <v>6896</v>
+        <v>6875</v>
       </c>
       <c r="B1889" s="2" t="s">
-        <v>5224</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1890" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1890" s="1" t="s">
-        <v>6897</v>
+        <v>6876</v>
       </c>
       <c r="B1890" s="2" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="1891" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1891" s="1" t="s">
-        <v>6898</v>
+        <v>6877</v>
       </c>
       <c r="B1891" s="2" t="s">
-        <v>6848</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1892" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1892" s="1" t="s">
-        <v>6899</v>
+        <v>6878</v>
       </c>
       <c r="B1892" s="2" t="s">
-        <v>7044</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1893" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1893" s="1" t="s">
-        <v>6900</v>
+        <v>6879</v>
       </c>
       <c r="B1893" s="2" t="s">
-        <v>7055</v>
+        <v>7053</v>
       </c>
     </row>
     <row r="1894" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1894" s="1" t="s">
-        <v>7039</v>
+        <v>6880</v>
       </c>
       <c r="B1894" s="2" t="s">
-        <v>7040</v>
+        <v>121</v>
       </c>
     </row>
     <row r="1895" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1895" s="1" t="s">
-        <v>6901</v>
+        <v>6881</v>
       </c>
       <c r="B1895" s="2" t="s">
-        <v>7049</v>
+        <v>124</v>
       </c>
     </row>
     <row r="1896" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1896" s="1" t="s">
-        <v>6902</v>
+        <v>6882</v>
       </c>
       <c r="B1896" s="2" t="s">
-        <v>6903</v>
+        <v>5224</v>
       </c>
     </row>
     <row r="1897" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1897" s="1" t="s">
-        <v>6904</v>
+        <v>6883</v>
       </c>
       <c r="B1897" s="2" t="s">
-        <v>6905</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1898" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1898" s="1" t="s">
-        <v>7035</v>
+        <v>6884</v>
       </c>
       <c r="B1898" s="2" t="s">
-        <v>7036</v>
+        <v>6848</v>
       </c>
     </row>
     <row r="1899" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1899" s="1" t="s">
-        <v>7037</v>
+        <v>6885</v>
       </c>
       <c r="B1899" s="2" t="s">
-        <v>7038</v>
+        <v>7054</v>
       </c>
     </row>
     <row r="1900" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1900" s="1" t="s">
-        <v>6906</v>
+        <v>6886</v>
       </c>
       <c r="B1900" s="2" t="s">
-        <v>6907</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1901" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1901" s="1" t="s">
-        <v>6908</v>
+        <v>6887</v>
       </c>
       <c r="B1901" s="2" t="s">
-        <v>6909</v>
+        <v>113</v>
       </c>
     </row>
     <row r="1902" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1902" s="1" t="s">
-        <v>7032</v>
+        <v>6888</v>
       </c>
       <c r="B1902" s="2" t="s">
-        <v>7033</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1903" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1903" s="1" t="s">
-        <v>6910</v>
+        <v>6889</v>
       </c>
       <c r="B1903" s="2" t="s">
-        <v>6911</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1904" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1904" s="1" t="s">
-        <v>6912</v>
+        <v>6890</v>
       </c>
       <c r="B1904" s="2" t="s">
-        <v>6913</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1905" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1905" s="1" t="s">
-        <v>6914</v>
+        <v>6891</v>
       </c>
       <c r="B1905" s="2" t="s">
-        <v>6915</v>
+        <v>98</v>
       </c>
     </row>
     <row r="1906" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1906" s="1" t="s">
-        <v>6916</v>
+        <v>6892</v>
       </c>
       <c r="B1906" s="2" t="s">
-        <v>311</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1907" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1907" s="1" t="s">
-        <v>6917</v>
+        <v>6893</v>
       </c>
       <c r="B1907" s="2" t="s">
-        <v>6918</v>
+        <v>104</v>
       </c>
     </row>
     <row r="1908" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1908" s="1" t="s">
-        <v>6919</v>
+        <v>6894</v>
       </c>
       <c r="B1908" s="2" t="s">
-        <v>6920</v>
+        <v>121</v>
       </c>
     </row>
     <row r="1909" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1909" s="1" t="s">
-        <v>6921</v>
+        <v>6895</v>
       </c>
       <c r="B1909" s="2" t="s">
-        <v>6922</v>
+        <v>124</v>
       </c>
     </row>
     <row r="1910" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1910" s="1" t="s">
-        <v>6923</v>
+        <v>6896</v>
       </c>
       <c r="B1910" s="2" t="s">
-        <v>7048</v>
+        <v>5224</v>
       </c>
     </row>
     <row r="1911" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1911" s="1" t="s">
-        <v>6924</v>
+        <v>6897</v>
       </c>
       <c r="B1911" s="2" t="s">
-        <v>7047</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1912" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1912" s="1" t="s">
-        <v>6925</v>
+        <v>6898</v>
       </c>
       <c r="B1912" s="2" t="s">
-        <v>7044</v>
+        <v>6848</v>
       </c>
     </row>
     <row r="1913" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1913" s="1" t="s">
-        <v>6926</v>
+        <v>6899</v>
       </c>
       <c r="B1913" s="2" t="s">
-        <v>6927</v>
+        <v>7044</v>
       </c>
     </row>
     <row r="1914" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1914" s="1" t="s">
-        <v>6928</v>
+        <v>6900</v>
       </c>
       <c r="B1914" s="2" t="s">
-        <v>7056</v>
+        <v>7055</v>
       </c>
     </row>
     <row r="1915" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1915" s="1" t="s">
-        <v>6929</v>
+        <v>7039</v>
       </c>
       <c r="B1915" s="2" t="s">
-        <v>6930</v>
+        <v>7040</v>
       </c>
     </row>
     <row r="1916" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1916" s="1" t="s">
-        <v>6931</v>
+        <v>6901</v>
       </c>
       <c r="B1916" s="2" t="s">
-        <v>7057</v>
+        <v>7049</v>
       </c>
     </row>
     <row r="1917" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1917" s="1" t="s">
-        <v>6932</v>
+        <v>6902</v>
       </c>
       <c r="B1917" s="2" t="s">
-        <v>7058</v>
+        <v>6903</v>
       </c>
     </row>
     <row r="1918" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1918" s="1" t="s">
-        <v>6933</v>
+        <v>6904</v>
       </c>
       <c r="B1918" s="2" t="s">
-        <v>6934</v>
+        <v>6905</v>
       </c>
     </row>
     <row r="1919" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1919" s="1" t="s">
-        <v>6935</v>
+        <v>7035</v>
       </c>
       <c r="B1919" s="2" t="s">
-        <v>6936</v>
+        <v>7036</v>
       </c>
     </row>
     <row r="1920" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1920" s="1" t="s">
-        <v>6937</v>
+        <v>7037</v>
       </c>
       <c r="B1920" s="2" t="s">
-        <v>6938</v>
+        <v>7038</v>
       </c>
     </row>
     <row r="1921" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1921" s="1" t="s">
-        <v>6939</v>
+        <v>6906</v>
       </c>
       <c r="B1921" s="2" t="s">
-        <v>6940</v>
+        <v>6907</v>
       </c>
     </row>
     <row r="1922" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1922" s="1" t="s">
-        <v>6941</v>
+        <v>6908</v>
       </c>
       <c r="B1922" s="2" t="s">
-        <v>6942</v>
+        <v>6909</v>
       </c>
     </row>
     <row r="1923" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1923" s="1" t="s">
-        <v>6943</v>
+        <v>7032</v>
       </c>
       <c r="B1923" s="2" t="s">
-        <v>6944</v>
+        <v>7033</v>
       </c>
     </row>
     <row r="1924" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1924" s="1" t="s">
-        <v>6945</v>
+        <v>6910</v>
       </c>
       <c r="B1924" s="2" t="s">
-        <v>6946</v>
+        <v>6911</v>
       </c>
     </row>
     <row r="1925" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1925" s="1" t="s">
-        <v>6947</v>
+        <v>6912</v>
       </c>
       <c r="B1925" s="2" t="s">
-        <v>6948</v>
+        <v>6913</v>
       </c>
     </row>
     <row r="1926" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1926" s="1" t="s">
-        <v>6949</v>
+        <v>6914</v>
       </c>
       <c r="B1926" s="2" t="s">
-        <v>6950</v>
+        <v>6915</v>
       </c>
     </row>
     <row r="1927" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1927" s="1" t="s">
-        <v>6951</v>
+        <v>6916</v>
       </c>
       <c r="B1927" s="2" t="s">
-        <v>6952</v>
+        <v>311</v>
       </c>
     </row>
     <row r="1928" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1928" s="1" t="s">
-        <v>6953</v>
+        <v>6917</v>
       </c>
       <c r="B1928" s="2" t="s">
-        <v>6954</v>
+        <v>6918</v>
       </c>
     </row>
     <row r="1929" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1929" s="1" t="s">
-        <v>6955</v>
+        <v>6919</v>
       </c>
       <c r="B1929" s="2" t="s">
-        <v>6956</v>
+        <v>6920</v>
       </c>
     </row>
     <row r="1930" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1930" s="1" t="s">
-        <v>6957</v>
+        <v>6921</v>
       </c>
       <c r="B1930" s="2" t="s">
-        <v>6958</v>
+        <v>6922</v>
       </c>
     </row>
     <row r="1931" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1931" s="1" t="s">
-        <v>6959</v>
+        <v>6923</v>
       </c>
       <c r="B1931" s="2" t="s">
-        <v>6960</v>
+        <v>7048</v>
       </c>
     </row>
     <row r="1932" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1932" s="1" t="s">
-        <v>6961</v>
+        <v>6924</v>
       </c>
       <c r="B1932" s="2" t="s">
-        <v>7059</v>
+        <v>7047</v>
       </c>
     </row>
     <row r="1933" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1933" s="1" t="s">
-        <v>6962</v>
+        <v>6925</v>
       </c>
       <c r="B1933" s="2" t="s">
-        <v>94</v>
+        <v>7044</v>
       </c>
     </row>
     <row r="1934" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1934" s="1" t="s">
-        <v>6963</v>
+        <v>6926</v>
       </c>
       <c r="B1934" s="2" t="s">
-        <v>6848</v>
+        <v>6927</v>
       </c>
     </row>
     <row r="1935" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1935" s="1" t="s">
-        <v>6964</v>
+        <v>6928</v>
       </c>
       <c r="B1935" s="2" t="s">
-        <v>7059</v>
+        <v>7056</v>
       </c>
     </row>
     <row r="1936" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1936" s="1" t="s">
-        <v>6965</v>
+        <v>6929</v>
       </c>
       <c r="B1936" s="2" t="s">
-        <v>98</v>
+        <v>6930</v>
       </c>
     </row>
     <row r="1937" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1937" s="1" t="s">
-        <v>6966</v>
+        <v>6931</v>
       </c>
       <c r="B1937" s="2" t="s">
-        <v>100</v>
+        <v>7057</v>
       </c>
     </row>
     <row r="1938" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1938" s="1" t="s">
-        <v>6967</v>
+        <v>6932</v>
       </c>
       <c r="B1938" s="2" t="s">
-        <v>102</v>
+        <v>7058</v>
       </c>
     </row>
     <row r="1939" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1939" s="1" t="s">
-        <v>6968</v>
+        <v>6933</v>
       </c>
       <c r="B1939" s="2" t="s">
-        <v>104</v>
+        <v>6934</v>
       </c>
     </row>
     <row r="1940" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1940" s="1" t="s">
-        <v>6969</v>
+        <v>6935</v>
       </c>
       <c r="B1940" s="2" t="s">
-        <v>111</v>
+        <v>6936</v>
       </c>
     </row>
     <row r="1941" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1941" s="1" t="s">
-        <v>6970</v>
+        <v>6937</v>
       </c>
       <c r="B1941" s="2" t="s">
-        <v>113</v>
+        <v>6938</v>
       </c>
     </row>
     <row r="1942" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1942" s="1" t="s">
-        <v>6971</v>
+        <v>6939</v>
       </c>
       <c r="B1942" s="2" t="s">
-        <v>115</v>
+        <v>6940</v>
       </c>
     </row>
     <row r="1943" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1943" s="1" t="s">
-        <v>6972</v>
+        <v>6941</v>
       </c>
       <c r="B1943" s="2" t="s">
-        <v>117</v>
+        <v>6942</v>
       </c>
     </row>
     <row r="1944" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1944" s="1" t="s">
-        <v>6973</v>
+        <v>6943</v>
       </c>
       <c r="B1944" s="2" t="s">
-        <v>7053</v>
+        <v>6944</v>
       </c>
     </row>
     <row r="1945" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1945" s="1" t="s">
-        <v>6974</v>
+        <v>6945</v>
       </c>
       <c r="B1945" s="2" t="s">
-        <v>121</v>
+        <v>6946</v>
       </c>
     </row>
     <row r="1946" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1946" s="1" t="s">
-        <v>6975</v>
+        <v>6947</v>
       </c>
       <c r="B1946" s="2" t="s">
-        <v>124</v>
+        <v>6948</v>
       </c>
     </row>
     <row r="1947" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1947" s="1" t="s">
-        <v>6976</v>
+        <v>6949</v>
       </c>
       <c r="B1947" s="2" t="s">
-        <v>5224</v>
+        <v>6950</v>
       </c>
     </row>
     <row r="1948" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1948" s="1" t="s">
-        <v>7034</v>
+        <v>6951</v>
       </c>
       <c r="B1948" s="2" t="s">
-        <v>126</v>
+        <v>6952</v>
       </c>
     </row>
     <row r="1949" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1949" s="1" t="s">
-        <v>6977</v>
+        <v>6953</v>
       </c>
       <c r="B1949" s="2" t="s">
-        <v>6848</v>
+        <v>6954</v>
       </c>
     </row>
     <row r="1950" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1950" s="1" t="s">
-        <v>6978</v>
+        <v>6955</v>
       </c>
       <c r="B1950" s="2" t="s">
-        <v>7054</v>
+        <v>6956</v>
       </c>
     </row>
     <row r="1951" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1951" s="1" t="s">
-        <v>6979</v>
+        <v>6957</v>
       </c>
       <c r="B1951" s="2" t="s">
-        <v>111</v>
+        <v>6958</v>
       </c>
     </row>
     <row r="1952" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1952" s="1" t="s">
-        <v>6980</v>
+        <v>6959</v>
       </c>
       <c r="B1952" s="2" t="s">
-        <v>113</v>
+        <v>6960</v>
       </c>
     </row>
     <row r="1953" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1953" s="1" t="s">
-        <v>6981</v>
+        <v>6961</v>
       </c>
       <c r="B1953" s="2" t="s">
-        <v>115</v>
+        <v>7059</v>
       </c>
     </row>
     <row r="1954" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1954" s="1" t="s">
-        <v>6982</v>
+        <v>6962</v>
       </c>
       <c r="B1954" s="2" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="1955" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1955" s="1" t="s">
-        <v>6983</v>
+        <v>6963</v>
       </c>
       <c r="B1955" s="2" t="s">
-        <v>119</v>
+        <v>6848</v>
       </c>
     </row>
     <row r="1956" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1956" s="1" t="s">
-        <v>6984</v>
+        <v>6964</v>
       </c>
       <c r="B1956" s="2" t="s">
-        <v>98</v>
+        <v>7059</v>
       </c>
     </row>
     <row r="1957" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1957" s="1" t="s">
-        <v>6985</v>
+        <v>6965</v>
       </c>
       <c r="B1957" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="1958" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1958" s="1" t="s">
-        <v>6986</v>
+        <v>6966</v>
       </c>
       <c r="B1958" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1959" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1959" s="1" t="s">
-        <v>6987</v>
+        <v>6967</v>
       </c>
       <c r="B1959" s="2" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
     </row>
     <row r="1960" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1960" s="1" t="s">
-        <v>6988</v>
+        <v>6968</v>
       </c>
       <c r="B1960" s="2" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
     </row>
     <row r="1961" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1961" s="1" t="s">
-        <v>6989</v>
+        <v>6969</v>
       </c>
       <c r="B1961" s="2" t="s">
-        <v>5224</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1962" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1962" s="1" t="s">
-        <v>6990</v>
+        <v>6970</v>
       </c>
       <c r="B1962" s="2" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="1963" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1963" s="1" t="s">
-        <v>6991</v>
+        <v>6971</v>
       </c>
       <c r="B1963" s="2" t="s">
-        <v>6848</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1964" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1964" s="1" t="s">
-        <v>6992</v>
+        <v>6972</v>
       </c>
       <c r="B1964" s="2" t="s">
-        <v>6993</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1965" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1965" s="1" t="s">
-        <v>6994</v>
+        <v>6973</v>
       </c>
       <c r="B1965" s="2" t="s">
-        <v>6995</v>
+        <v>7053</v>
       </c>
     </row>
     <row r="1966" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1966" s="1" t="s">
-        <v>6996</v>
+        <v>6974</v>
       </c>
       <c r="B1966" s="2" t="s">
-        <v>6997</v>
+        <v>121</v>
       </c>
     </row>
     <row r="1967" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1967" s="1" t="s">
-        <v>6998</v>
+        <v>6975</v>
       </c>
       <c r="B1967" s="2" t="s">
-        <v>6999</v>
+        <v>124</v>
       </c>
     </row>
     <row r="1968" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1968" s="1" t="s">
-        <v>7000</v>
+        <v>6976</v>
       </c>
       <c r="B1968" s="2" t="s">
-        <v>6999</v>
+        <v>5224</v>
       </c>
     </row>
     <row r="1969" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1969" s="1" t="s">
-        <v>7001</v>
+        <v>7034</v>
       </c>
       <c r="B1969" s="2" t="s">
-        <v>2887</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1970" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1970" s="1" t="s">
-        <v>7002</v>
+        <v>6977</v>
       </c>
       <c r="B1970" s="2" t="s">
-        <v>7003</v>
+        <v>6848</v>
       </c>
     </row>
     <row r="1971" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1971" s="1" t="s">
-        <v>7004</v>
+        <v>6978</v>
       </c>
       <c r="B1971" s="2" t="s">
-        <v>6927</v>
+        <v>7054</v>
       </c>
     </row>
     <row r="1972" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1972" s="1" t="s">
-        <v>7005</v>
+        <v>6979</v>
       </c>
       <c r="B1972" s="2" t="s">
-        <v>7006</v>
+        <v>111</v>
       </c>
     </row>
     <row r="1973" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1973" s="1" t="s">
-        <v>7007</v>
+        <v>6980</v>
       </c>
       <c r="B1973" s="2" t="s">
-        <v>7008</v>
+        <v>113</v>
       </c>
     </row>
     <row r="1974" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1974" s="1" t="s">
-        <v>7009</v>
+        <v>6981</v>
       </c>
       <c r="B1974" s="2" t="s">
-        <v>7051</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1975" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1975" s="1" t="s">
-        <v>7010</v>
+        <v>6982</v>
       </c>
       <c r="B1975" s="2" t="s">
-        <v>7051</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1976" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1976" s="1" t="s">
-        <v>7011</v>
+        <v>6983</v>
       </c>
       <c r="B1976" s="2" t="s">
-        <v>7012</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1977" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1977" s="1" t="s">
-        <v>7013</v>
+        <v>6984</v>
       </c>
       <c r="B1977" s="2" t="s">
-        <v>7014</v>
+        <v>98</v>
       </c>
     </row>
     <row r="1978" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1978" s="1" t="s">
-        <v>7015</v>
+        <v>6985</v>
       </c>
       <c r="B1978" s="2" t="s">
-        <v>7051</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1979" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1979" s="1" t="s">
-        <v>7016</v>
+        <v>6986</v>
       </c>
       <c r="B1979" s="2" t="s">
-        <v>7051</v>
+        <v>104</v>
       </c>
     </row>
     <row r="1980" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1980" s="1" t="s">
-        <v>7017</v>
+        <v>6987</v>
       </c>
       <c r="B1980" s="2" t="s">
-        <v>7012</v>
+        <v>121</v>
       </c>
     </row>
     <row r="1981" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1981" s="1" t="s">
-        <v>7018</v>
+        <v>6988</v>
       </c>
       <c r="B1981" s="2" t="s">
-        <v>7019</v>
+        <v>124</v>
       </c>
     </row>
     <row r="1982" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1982" s="1" t="s">
-        <v>7020</v>
+        <v>6989</v>
       </c>
       <c r="B1982" s="2" t="s">
-        <v>7021</v>
+        <v>5224</v>
       </c>
     </row>
     <row r="1983" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1983" s="1" t="s">
-        <v>7022</v>
+        <v>6990</v>
       </c>
       <c r="B1983" s="2" t="s">
-        <v>7050</v>
+        <v>126</v>
       </c>
     </row>
     <row r="1984" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1984" s="1" t="s">
-        <v>7023</v>
+        <v>6991</v>
       </c>
       <c r="B1984" s="2" t="s">
-        <v>7024</v>
+        <v>6848</v>
       </c>
     </row>
     <row r="1985" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1985" s="1" t="s">
-        <v>7025</v>
+        <v>6992</v>
       </c>
       <c r="B1985" s="2" t="s">
-        <v>7014</v>
+        <v>6993</v>
       </c>
     </row>
     <row r="1986" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1986" s="1" t="s">
-        <v>7026</v>
+        <v>6994</v>
       </c>
       <c r="B1986" s="2" t="s">
-        <v>51</v>
+        <v>6995</v>
       </c>
     </row>
     <row r="1987" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1987" s="1" t="s">
-        <v>7027</v>
+        <v>6996</v>
       </c>
       <c r="B1987" s="2" t="s">
-        <v>111</v>
+        <v>6997</v>
       </c>
     </row>
     <row r="1988" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1988" s="1" t="s">
-        <v>7028</v>
+        <v>6998</v>
       </c>
       <c r="B1988" s="2" t="s">
-        <v>7029</v>
+        <v>6999</v>
       </c>
     </row>
     <row r="1989" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1989" s="1" t="s">
-        <v>7030</v>
+        <v>7000</v>
       </c>
       <c r="B1989" s="2" t="s">
-        <v>115</v>
+        <v>6999</v>
       </c>
     </row>
     <row r="1990" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1990" s="1" t="s">
-        <v>7031</v>
+        <v>7001</v>
       </c>
       <c r="B1990" s="2" t="s">
-        <v>117</v>
+        <v>2887</v>
       </c>
     </row>
     <row r="1991" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1991" s="1" t="s">
-        <v>7041</v>
+        <v>7002</v>
       </c>
       <c r="B1991" s="2" t="s">
-        <v>7042</v>
+        <v>7003</v>
       </c>
     </row>
     <row r="1992" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1992" s="16" t="s">
-        <v>7043</v>
+      <c r="A1992" s="1" t="s">
+        <v>7004</v>
       </c>
       <c r="B1992" s="2" t="s">
-        <v>7044</v>
+        <v>6927</v>
       </c>
     </row>
     <row r="1993" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1993" s="1" t="s">
-        <v>7045</v>
+        <v>7005</v>
       </c>
       <c r="B1993" s="2" t="s">
-        <v>7046</v>
+        <v>7006</v>
       </c>
     </row>
     <row r="1994" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1994" s="1" t="s">
-        <v>7066</v>
+        <v>7007</v>
       </c>
       <c r="B1994" s="2" t="s">
-        <v>7047</v>
+        <v>7008</v>
       </c>
     </row>
     <row r="1995" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1995" s="1" t="s">
-        <v>7052</v>
+        <v>7009</v>
       </c>
       <c r="B1995" s="2" t="s">
-        <v>6550</v>
+        <v>7051</v>
       </c>
     </row>
     <row r="1996" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1996" s="1" t="s">
-        <v>7074</v>
+        <v>7010</v>
       </c>
       <c r="B1996" s="2" t="s">
-        <v>6550</v>
+        <v>7051</v>
       </c>
     </row>
     <row r="1997" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1997" s="1" t="s">
-        <v>7075</v>
+        <v>7011</v>
       </c>
       <c r="B1997" s="2" t="s">
-        <v>6550</v>
+        <v>7012</v>
       </c>
     </row>
     <row r="1998" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1998" s="1" t="s">
-        <v>7060</v>
+        <v>7013</v>
       </c>
       <c r="B1998" s="2" t="s">
-        <v>7061</v>
+        <v>7014</v>
       </c>
     </row>
     <row r="1999" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1999" s="1" t="s">
-        <v>7062</v>
+        <v>7015</v>
       </c>
       <c r="B1999" s="2" t="s">
-        <v>7063</v>
+        <v>7051</v>
       </c>
     </row>
     <row r="2000" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2000" s="1" t="s">
+        <v>7016</v>
+      </c>
+      <c r="B2000" s="2" t="s">
+        <v>7051</v>
+      </c>
+    </row>
+    <row r="2001" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2001" s="1" t="s">
+        <v>7017</v>
+      </c>
+      <c r="B2001" s="2" t="s">
+        <v>7012</v>
+      </c>
+    </row>
+    <row r="2002" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2002" s="1" t="s">
+        <v>7018</v>
+      </c>
+      <c r="B2002" s="2" t="s">
+        <v>7019</v>
+      </c>
+    </row>
+    <row r="2003" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2003" s="1" t="s">
+        <v>7020</v>
+      </c>
+      <c r="B2003" s="2" t="s">
+        <v>7021</v>
+      </c>
+    </row>
+    <row r="2004" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2004" s="1" t="s">
+        <v>7022</v>
+      </c>
+      <c r="B2004" s="2" t="s">
+        <v>7050</v>
+      </c>
+    </row>
+    <row r="2005" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2005" s="1" t="s">
+        <v>7023</v>
+      </c>
+      <c r="B2005" s="2" t="s">
+        <v>7024</v>
+      </c>
+    </row>
+    <row r="2006" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2006" s="1" t="s">
+        <v>7025</v>
+      </c>
+      <c r="B2006" s="2" t="s">
+        <v>7014</v>
+      </c>
+    </row>
+    <row r="2007" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2007" s="1" t="s">
+        <v>7026</v>
+      </c>
+      <c r="B2007" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2008" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2008" s="1" t="s">
+        <v>7027</v>
+      </c>
+      <c r="B2008" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2009" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2009" s="1" t="s">
+        <v>7028</v>
+      </c>
+      <c r="B2009" s="2" t="s">
+        <v>7029</v>
+      </c>
+    </row>
+    <row r="2010" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2010" s="1" t="s">
+        <v>7030</v>
+      </c>
+      <c r="B2010" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2011" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2011" s="1" t="s">
+        <v>7031</v>
+      </c>
+      <c r="B2011" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2012" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2012" s="1" t="s">
+        <v>7041</v>
+      </c>
+      <c r="B2012" s="2" t="s">
+        <v>7042</v>
+      </c>
+    </row>
+    <row r="2013" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2013" s="16" t="s">
+        <v>7043</v>
+      </c>
+      <c r="B2013" s="2" t="s">
+        <v>7044</v>
+      </c>
+    </row>
+    <row r="2014" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2014" s="1" t="s">
+        <v>7045</v>
+      </c>
+      <c r="B2014" s="2" t="s">
+        <v>7046</v>
+      </c>
+    </row>
+    <row r="2015" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2015" s="1" t="s">
+        <v>7066</v>
+      </c>
+      <c r="B2015" s="2" t="s">
+        <v>7047</v>
+      </c>
+    </row>
+    <row r="2016" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2016" s="1" t="s">
+        <v>7052</v>
+      </c>
+      <c r="B2016" s="2" t="s">
+        <v>6550</v>
+      </c>
+    </row>
+    <row r="2017" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2017" s="1" t="s">
+        <v>7074</v>
+      </c>
+      <c r="B2017" s="2" t="s">
+        <v>6550</v>
+      </c>
+    </row>
+    <row r="2018" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2018" s="1" t="s">
+        <v>7075</v>
+      </c>
+      <c r="B2018" s="2" t="s">
+        <v>6550</v>
+      </c>
+    </row>
+    <row r="2019" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2019" s="1" t="s">
+        <v>7060</v>
+      </c>
+      <c r="B2019" s="2" t="s">
+        <v>7061</v>
+      </c>
+    </row>
+    <row r="2020" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2020" s="1" t="s">
+        <v>7062</v>
+      </c>
+      <c r="B2020" s="2" t="s">
+        <v>7063</v>
+      </c>
+    </row>
+    <row r="2021" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2021" s="1" t="s">
         <v>7064</v>
       </c>
-      <c r="B2000" s="2" t="s">
+      <c r="B2021" s="2" t="s">
         <v>7065</v>
       </c>
     </row>
-    <row r="2001" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2001" s="1" t="s">
+    <row r="2022" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2022" s="1" t="s">
         <v>7067</v>
       </c>
     </row>
-    <row r="2002" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2002" s="1" t="s">
+    <row r="2023" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2023" s="1" t="s">
         <v>7068</v>
       </c>
     </row>
@@ -58262,7 +58526,7 @@
       <formula>AND($B2 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A1629 A1993 A1996:A1998 A2001:A2002 A1686:A1688 A1690:A1991 A2005:A1048576">
+  <conditionalFormatting sqref="A2:A1629 A2014 A2017:A2019 A2022:A2023 A1686:A1688 A1690:A2012 A2026:A1048576">
     <cfRule type="expression" dxfId="11" priority="44">
       <formula>AND( $A2 = "", OR( $B2 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
@@ -58277,19 +58541,19 @@
       <formula>AND( $A1630 = "", OR( $B1630 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1995">
+  <conditionalFormatting sqref="A2016">
     <cfRule type="expression" dxfId="8" priority="1">
-      <formula>AND( $A1995 = "", OR( $B1995 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
+      <formula>AND( $A2016 = "", OR( $B2016 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1994">
+  <conditionalFormatting sqref="A2015">
     <cfRule type="expression" dxfId="7" priority="48">
-      <formula>AND( $A1994 = "", OR( $B2003 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
+      <formula>AND( $A2015 = "", OR( $B2024 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2000">
+  <conditionalFormatting sqref="A2021">
     <cfRule type="expression" dxfId="6" priority="51">
-      <formula>AND( $A2000 = "", OR( $B2004 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
+      <formula>AND( $A2021 = "", OR( $B2025 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
svenska translation for neighbours and help texts
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12420" uniqueCount="7480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12444" uniqueCount="7497">
   <si>
     <t>fi</t>
   </si>
@@ -22507,6 +22507,57 @@
   </si>
   <si>
     <t>Kirjoita lausunto. Jos lausunto on liitteenä, niin lisää maininta tähän.</t>
+  </si>
+  <si>
+    <t>Affärsekonomiskt byggande anges som byggare när största delen av byggarbetet utförs av utomstående byggare, t.ex. arbetslag, timmermansgrupp eller entreprenör. Annat slags byggande antecknas som byggare i de fall när största delen av byggarbetet utförs på egen hand.</t>
+  </si>
+  <si>
+    <t>Med gas avses också flytgas i fall byggnaden för detta ändamål är försedd med varaktigt nät.</t>
+  </si>
+  <si>
+    <t>Byggnadens huvudsakliga användningssyfte anges enligt det syfte för vilket största delen av byggnadens våningsyta används. Som bostadsbyggnad anses dock sådana byggnader av vilkas våningsyta minst hälften är bostadslägenhetsyta. Också vid tillbyggnad anges hela byggnadens användningssyfte, inte bara den tillbyggda delens.</t>
+  </si>
+  <si>
+    <t>Byggnadens volym är det utrymme som begränsas av ytterväggarnas utsidor, undersidan av bottenbjälklaget (byggnadsutrymmets understa bjälklag jämte värmeisolering) och översidan av vindbjälklaget (den byggnadsdel som upptill begränsar det översta varma utrymmet i byggnaden och till vilken hör värmeisolering jämte skydd).</t>
+  </si>
+  <si>
+    <t>Till våningsytan räknas våningarnas ytor beräknade enligt ytterväggarnas utsidor och sådan yta i källar- eller vindsvåning där lokaler avsedda för byggnadens huvudsakliga ändamål placeras eller med tanke på dessa lokalers läge, förbindelser, storlek, ljus och andra  egenskaper kunde placeras (115 § 3 mom. markanvändnings- och bygglagen). Närmare anvisningar om hur våningsytan beräknas finns i Finlands standardiseringsförbunds standard (SFS 5139).</t>
+  </si>
+  <si>
+    <t>I byggnadens hela areal medräknas samtliga våningars, källares och värmeisolerade vindars areal sammanlagt i yttre mått. Balkonger, skjul samt utrymmen lägre än 160 cm medräknas inte.</t>
+  </si>
+  <si>
+    <t>I våningsantalet medräknas alla de huvudsakligen ovan jord belägna våningarna i vilka det finns bostads- eller arbetsrum eller mot byggnadens huvudsakliga användningssyfte svarande utrymmen. Våningsantalet anges som helt tal. Om antalet våningar varierar i olika delar av byggnaden, anges det våningsantal som finns i största delen av byggnaden.</t>
+  </si>
+  <si>
+    <t>medräknas inte.</t>
+  </si>
+  <si>
+    <t>belägna våningar</t>
+  </si>
+  <si>
+    <t>Källarens areal är källarvåningens sammanlagda areal. Källarvåningens areal är det område som begränsas av utsidorna av väggarna kring källarvåningen. Utrymmen, lägre än 160 cm, medräknas inte. Som källarvåning räknas alla helt eller i huvudsak under markytan belägna våningar.</t>
+  </si>
+  <si>
+    <t>Som betong betraktas också tillverkningar av siporex, lättgrus, slagg och gasbetong o.d. tillverkningar av lättbetong.</t>
+  </si>
+  <si>
+    <t>I en elementbyggnad är mer än hälften av volymen av de bärande konstruktionerna såsom pelare, balkar, mellanbjälklag och väggar fabrikstillverkade. I en byggnad som uppförs på platsen är högst ventilations- och rökkanalerna, trapploppen, balkongerna och badrummen fabrikstillverkade.</t>
+  </si>
+  <si>
+    <t>Enbart det huvudsakliga uppvärmningssättet anmäls. Vid vattencentraluppvärmning uppvärms byggnaden med hjälp av cirkulerande vatten. Vid luftcentraluppvärmning uppvärms byggnaden med hjälp av cirkulerande luft. Vid direkt eluppvärmning uppvärms byggnaden med hjälp av ett fast värmeelement o.d. som kopplats direkt till elnätet. Som ugnseldning betraktas också i mur installerade eldrivna värmeberedare, separata fasta oljevärmeapparater samt spisar som magasinerar värme.</t>
+  </si>
+  <si>
+    <t>Det huvudsakligen använda bränslet anmäls. I fråga om fjärr- eller blockvärme behöver bränslet inte anges. Jordvärme o.d. förutsätter värmepump.</t>
+  </si>
+  <si>
+    <t>Lägenhetsytan är den yta som begränsas dels av väggarna kring lägenheten, dels av de ytor som vetter mot lägenheten på bärande och andra för hela byggnaden nödvändiga byggnadsdelar.</t>
+  </si>
+  <si>
+    <t>I egenskap av grannar har vi ingenting att anmärka på med anledning av byggprojektet</t>
+  </si>
+  <si>
+    <t>Med anledning av byggprojektet framför vi följande anmärkningar:</t>
   </si>
 </sst>
 </file>
@@ -22825,7 +22876,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -22874,6 +22925,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="165">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -23717,16 +23769,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C875"/>
+  <dimension ref="A1:D875"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A872" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B884" sqref="B884"/>
+    <sheetView tabSelected="1" topLeftCell="A835" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B648" sqref="B648"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="100.69921875" style="1" customWidth="1"/>
     <col min="2" max="3" width="50.69921875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="91" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -30262,7 +30315,7 @@
         <v>4989</v>
       </c>
     </row>
-    <row r="641" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="641" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A641" s="1" t="s">
         <v>4748</v>
       </c>
@@ -30270,7 +30323,7 @@
         <v>4624</v>
       </c>
     </row>
-    <row r="642" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="642" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A642" s="1" t="s">
         <v>1275</v>
       </c>
@@ -30281,7 +30334,7 @@
         <v>5184</v>
       </c>
     </row>
-    <row r="643" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="643" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A643" s="1" t="s">
         <v>1280</v>
       </c>
@@ -30292,7 +30345,7 @@
         <v>5185</v>
       </c>
     </row>
-    <row r="644" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="644" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A644" s="1" t="s">
         <v>1272</v>
       </c>
@@ -30303,7 +30356,7 @@
         <v>5186</v>
       </c>
     </row>
-    <row r="645" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="645" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A645" s="1" t="s">
         <v>1761</v>
       </c>
@@ -30314,92 +30367,131 @@
         <v>5187</v>
       </c>
     </row>
-    <row r="646" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="646" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A646" t="s">
         <v>5673</v>
       </c>
       <c r="B646" t="s">
         <v>5670</v>
       </c>
-    </row>
-    <row r="647" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C646" s="5" t="s">
+        <v>7494</v>
+      </c>
+    </row>
+    <row r="647" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A647" t="s">
         <v>5622</v>
       </c>
       <c r="B647" t="s">
         <v>5619</v>
       </c>
-    </row>
-    <row r="648" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C647" s="5" t="s">
+        <v>7482</v>
+      </c>
+    </row>
+    <row r="648" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A648" t="s">
         <v>5662</v>
       </c>
       <c r="B648" t="s">
         <v>5660</v>
       </c>
-    </row>
-    <row r="649" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C648" s="5" t="s">
+        <v>7492</v>
+      </c>
+    </row>
+    <row r="649" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A649" t="s">
         <v>5667</v>
       </c>
       <c r="B649" t="s">
         <v>5665</v>
       </c>
-    </row>
-    <row r="650" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C649" s="5" t="s">
+        <v>7493</v>
+      </c>
+    </row>
+    <row r="650" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A650" t="s">
         <v>5647</v>
       </c>
       <c r="B650" t="s">
         <v>5646</v>
       </c>
-    </row>
-    <row r="651" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C650" s="21" t="s">
+        <v>7489</v>
+      </c>
+    </row>
+    <row r="651" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A651" t="s">
         <v>5631</v>
       </c>
       <c r="B651" t="s">
         <v>5629</v>
       </c>
-    </row>
-    <row r="652" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C651" t="s">
+        <v>7484</v>
+      </c>
+    </row>
+    <row r="652" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A652" t="s">
         <v>5641</v>
       </c>
       <c r="B652" t="s">
         <v>5639</v>
       </c>
-    </row>
-    <row r="653" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C652" t="s">
+        <v>7486</v>
+      </c>
+      <c r="D652" t="s">
+        <v>7487</v>
+      </c>
+    </row>
+    <row r="653" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A653" t="s">
         <v>5636</v>
       </c>
       <c r="B653" t="s">
         <v>5634</v>
       </c>
-    </row>
-    <row r="654" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C653" t="s">
+        <v>7485</v>
+      </c>
+    </row>
+    <row r="654" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A654" t="s">
         <v>5627</v>
       </c>
       <c r="B654" t="s">
         <v>5624</v>
       </c>
-    </row>
-    <row r="655" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C654" t="s">
+        <v>7483</v>
+      </c>
+      <c r="D654" t="s">
+        <v>7488</v>
+      </c>
+    </row>
+    <row r="655" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A655" t="s">
         <v>5657</v>
       </c>
       <c r="B655" t="s">
         <v>5655</v>
       </c>
-    </row>
-    <row r="656" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C655" s="5" t="s">
+        <v>7490</v>
+      </c>
+    </row>
+    <row r="656" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A656" t="s">
         <v>5652</v>
       </c>
       <c r="B656" t="s">
         <v>5650</v>
+      </c>
+      <c r="C656" s="5" t="s">
+        <v>7491</v>
       </c>
     </row>
     <row r="657" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -30409,6 +30501,9 @@
       <c r="B657" t="s">
         <v>5614</v>
       </c>
+      <c r="C657" s="5" t="s">
+        <v>7480</v>
+      </c>
     </row>
     <row r="658" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A658" s="9" t="s">
@@ -31768,7 +31863,9 @@
       <c r="B849" s="2" t="s">
         <v>7187</v>
       </c>
-      <c r="C849"/>
+      <c r="C849" t="s">
+        <v>7496</v>
+      </c>
     </row>
     <row r="850" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A850" s="1" t="s">
@@ -31777,6 +31874,9 @@
       <c r="B850" s="2" t="s">
         <v>7188</v>
       </c>
+      <c r="C850" s="5" t="s">
+        <v>7495</v>
+      </c>
     </row>
     <row r="851" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A851" s="1" t="s">
@@ -31940,7 +32040,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C713 C850:C1048576">
+  <conditionalFormatting sqref="C1:C649 C850:C1048576 C655:C713">
     <cfRule type="expression" dxfId="32" priority="7">
       <formula>AND($B1 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
@@ -38329,8 +38429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2206"/>
   <sheetViews>
-    <sheetView topLeftCell="A1255" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A1283" sqref="A1283"/>
+    <sheetView topLeftCell="A2181" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C2206" sqref="C2206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
@@ -61072,7 +61172,7 @@
         <v>5361</v>
       </c>
     </row>
-    <row r="2194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2194" s="1" t="s">
         <v>5610</v>
       </c>
@@ -61080,7 +61180,7 @@
         <v>7421</v>
       </c>
     </row>
-    <row r="2195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2195" s="1" t="s">
         <v>7434</v>
       </c>
@@ -61088,7 +61188,7 @@
         <v>7435</v>
       </c>
     </row>
-    <row r="2196" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2196" s="1" t="s">
         <v>7422</v>
       </c>
@@ -61096,68 +61196,92 @@
         <v>7423</v>
       </c>
     </row>
-    <row r="2198" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2198" s="1" t="s">
         <v>7424</v>
       </c>
       <c r="B2198" s="2" t="s">
         <v>7425</v>
       </c>
-    </row>
-    <row r="2199" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2198" t="s">
+        <v>7480</v>
+      </c>
+    </row>
+    <row r="2199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2199" s="1" t="s">
         <v>7426</v>
       </c>
       <c r="B2199" s="2" t="s">
         <v>7425</v>
       </c>
-    </row>
-    <row r="2200" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2199" t="s">
+        <v>7480</v>
+      </c>
+    </row>
+    <row r="2200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2200" s="1" t="s">
         <v>7427</v>
       </c>
       <c r="B2200" s="2" t="s">
         <v>7425</v>
       </c>
-    </row>
-    <row r="2201" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2200" t="s">
+        <v>7480</v>
+      </c>
+    </row>
+    <row r="2201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2201" s="1" t="s">
         <v>7428</v>
       </c>
       <c r="B2201" s="2" t="s">
         <v>7425</v>
       </c>
-    </row>
-    <row r="2203" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2201" t="s">
+        <v>7480</v>
+      </c>
+    </row>
+    <row r="2203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2203" s="1" t="s">
         <v>7429</v>
       </c>
       <c r="B2203" s="2" t="s">
         <v>7430</v>
       </c>
-    </row>
-    <row r="2204" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2203" t="s">
+        <v>7481</v>
+      </c>
+    </row>
+    <row r="2204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2204" s="1" t="s">
         <v>7431</v>
       </c>
       <c r="B2204" s="2" t="s">
         <v>7430</v>
       </c>
-    </row>
-    <row r="2205" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2204" t="s">
+        <v>7481</v>
+      </c>
+    </row>
+    <row r="2205" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2205" s="1" t="s">
         <v>7432</v>
       </c>
       <c r="B2205" s="2" t="s">
         <v>7430</v>
       </c>
-    </row>
-    <row r="2206" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2205" t="s">
+        <v>7481</v>
+      </c>
+    </row>
+    <row r="2206" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2206" s="1" t="s">
         <v>7433</v>
       </c>
       <c r="B2206" s="2" t="s">
         <v>7430</v>
+      </c>
+      <c r="C2206" t="s">
+        <v>7481</v>
       </c>
     </row>
   </sheetData>
@@ -61245,7 +61369,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Moved localisations from the txt-file to the excel.
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51195" windowHeight="18240" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51195" windowHeight="18240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12689" uniqueCount="7532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12701" uniqueCount="7543">
   <si>
     <t>fi</t>
   </si>
@@ -22663,6 +22663,39 @@
   </si>
   <si>
     <t>yleiset-alueet-maksaja.yritys.yhteyshenkilo.yhteystiedot.puhelin</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Rakennuslupa</t>
+  </si>
+  <si>
+    <t>YA</t>
+  </si>
+  <si>
+    <t>Yleisten alueiden lupa</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Poikkeamislupa</t>
+  </si>
+  <si>
+    <t>comment-request-label</t>
+  </si>
+  <si>
+    <t>Lähetä ilmoitus viestistä</t>
+  </si>
+  <si>
+    <t>comment-request-prompt</t>
+  </si>
+  <si>
+    <t>Valitse käyttäjä</t>
   </si>
 </sst>
 </file>
@@ -23874,8 +23907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D879"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C161" sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A833" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A848" sqref="A848"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -32372,28 +32405,56 @@
       </c>
     </row>
     <row r="843" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A843"/>
-      <c r="B843"/>
+      <c r="A843" t="s">
+        <v>7532</v>
+      </c>
+      <c r="B843" t="s">
+        <v>7533</v>
+      </c>
       <c r="C843"/>
     </row>
     <row r="844" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A844"/>
-      <c r="B844"/>
+      <c r="A844" t="s">
+        <v>7534</v>
+      </c>
+      <c r="B844" t="s">
+        <v>7535</v>
+      </c>
       <c r="C844"/>
     </row>
+    <row r="845" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A845" s="2" t="s">
+        <v>7536</v>
+      </c>
+      <c r="B845" s="5" t="s">
+        <v>1751</v>
+      </c>
+    </row>
     <row r="846" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A846"/>
-      <c r="B846"/>
+      <c r="A846" t="s">
+        <v>7537</v>
+      </c>
+      <c r="B846" t="s">
+        <v>7538</v>
+      </c>
       <c r="C846"/>
     </row>
     <row r="847" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A847"/>
-      <c r="B847"/>
+      <c r="A847" t="s">
+        <v>7539</v>
+      </c>
+      <c r="B847" t="s">
+        <v>7540</v>
+      </c>
       <c r="C847"/>
     </row>
     <row r="848" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A848"/>
-      <c r="B848"/>
+      <c r="A848" t="s">
+        <v>7541</v>
+      </c>
+      <c r="B848" t="s">
+        <v>7542</v>
+      </c>
       <c r="C848"/>
     </row>
     <row r="849" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -32581,7 +32642,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -38929,8 +38990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2142" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A2159" sqref="A2159"/>
+    <sheetView topLeftCell="A2113" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A2125" sqref="A2125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added localizations to the txt-file
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -46174,8 +46174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2403"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2191" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B2193" sqref="B2193:B2211"/>
+    <sheetView tabSelected="1" topLeftCell="A2206" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A2194" sqref="A2194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
move localisations to excel
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" updateLinks="never" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14580" tabRatio="644"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="22200" tabRatio="644"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="11" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">schemas!$A$1:$C$2698</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13362" uniqueCount="9356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13330" uniqueCount="9336">
   <si>
     <t>fi</t>
   </si>
@@ -28593,91 +28593,31 @@
     <t>Lupapiste-palvelun käyttöongelmat</t>
   </si>
   <si>
-    <t>application.applicationSummary</t>
-  </si>
-  <si>
-    <t>Hakemus</t>
-  </si>
-  <si>
-    <t>application.tabApplicationSummary</t>
-  </si>
-  <si>
-    <t>verdict.lupamaaraukset.missing</t>
-  </si>
-  <si>
-    <t>Päätökseen ei liity lupamääräyksiä</t>
-  </si>
-  <si>
-    <t>verdict.poytakirjat.missing</t>
-  </si>
-  <si>
-    <t>Päätökseen ei liity pöytäkirjoja</t>
-  </si>
-  <si>
-    <t>application.neighbors.hearings</t>
-  </si>
-  <si>
-    <t>Kuulemiset</t>
-  </si>
-  <si>
-    <t>help.R.applicationSummaryDesc</t>
-  </si>
-  <si>
-    <t>Tällä välilehdellä näet hankkeeseesi liittyvät hakemuksen aikaiset tiedot.</t>
-  </si>
-  <si>
-    <t>help.P.applicationSummaryDesc</t>
-  </si>
-  <si>
-    <t>help.YA.applicationSummaryDesc</t>
-  </si>
-  <si>
-    <t>help.YI.applicationSummaryDesc</t>
-  </si>
-  <si>
-    <t>help.YL.applicationSummaryDesc</t>
-  </si>
-  <si>
-    <t>help.MAL.applicationSummaryDesc</t>
-  </si>
-  <si>
-    <t>help.VVVL.applicationSummaryDesc</t>
-  </si>
-  <si>
-    <t>help.KM.applicationSummaryDesc</t>
-  </si>
-  <si>
-    <t>help.R.tasksDesc</t>
-  </si>
-  <si>
-    <t>Tällä välilehdellä näet luvan edellyttämät rakentamisen aikaiset kokoukset, katselmukset ja tarkastukset sekä muut lupavaatimukset.</t>
-  </si>
-  <si>
-    <t>help.P.tasksDesc</t>
-  </si>
-  <si>
-    <t>Tällä välilehdellä näet luvan edellyttämät toiminnan aikaiset kokoukset, katselmukset ja tarkastukset sekä muut lupavaatimukset.</t>
-  </si>
-  <si>
-    <t>help.YA.tasksDesc</t>
-  </si>
-  <si>
-    <t>help.YI.tasksDesc</t>
-  </si>
-  <si>
-    <t>help.YL.tasksDesc</t>
-  </si>
-  <si>
-    <t>help.MAL.tasksDesc</t>
-  </si>
-  <si>
-    <t>help.VVVL.tasksDesc</t>
-  </si>
-  <si>
-    <t>help.KM.tasksDesc</t>
-  </si>
-  <si>
-    <t>Läsnäolijat</t>
+    <t>verdict.signatures</t>
+  </si>
+  <si>
+    <t>Päätös vaatii hakijan allekirjoituksen</t>
+  </si>
+  <si>
+    <t>verdict.signature.description</t>
+  </si>
+  <si>
+    <t>verdict.sign</t>
+  </si>
+  <si>
+    <t>verdict.sign-dialog.header</t>
+  </si>
+  <si>
+    <t>Allekirjoita päätös</t>
+  </si>
+  <si>
+    <t>verdict.sign-dialog.contentDescription</t>
+  </si>
+  <si>
+    <t>Päätöksen allekirjoituksen kuvaus</t>
+  </si>
+  <si>
+    <t>verdict.sign-dialog.signButton</t>
   </si>
 </sst>
 </file>
@@ -28687,7 +28627,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-81D]General"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -28928,7 +28868,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="618">
+  <cellStyleXfs count="620">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -29547,6 +29487,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -29692,7 +29634,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="618">
+  <cellStyles count="620">
     <cellStyle name="Bad" xfId="190" builtinId="27"/>
     <cellStyle name="Excel Built-in Bad" xfId="193"/>
     <cellStyle name="Excel Built-in Normal" xfId="192"/>
@@ -30002,6 +29944,7 @@
     <cellStyle name="Followed Hyperlink" xfId="613" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="615" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="617" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="619" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="191" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -30309,20 +30252,11 @@
     <cellStyle name="Hyperlink" xfId="612" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="614" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="616" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="618" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="187"/>
   </cellStyles>
-  <dxfs count="190">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="189">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -32227,7 +32161,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="schemas"/>
@@ -32561,17 +32495,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1650"/>
+  <dimension ref="A1:C1629"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1608" workbookViewId="0">
-      <selection activeCell="A1651" sqref="A1651"/>
+    <sheetView tabSelected="1" topLeftCell="A1587" workbookViewId="0">
+      <selection activeCell="B1629" sqref="B1629"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="90.375" customWidth="1"/>
-    <col min="3" max="3" width="73.125" customWidth="1"/>
+    <col min="2" max="2" width="90.33203125" customWidth="1"/>
+    <col min="3" max="3" width="73.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -34508,7 +34442,7 @@
         <v>7647</v>
       </c>
     </row>
-    <row r="177" spans="1:3" s="47" customFormat="1" ht="94.5">
+    <row r="177" spans="1:3" s="47" customFormat="1" ht="90">
       <c r="A177" s="9" t="s">
         <v>3525</v>
       </c>
@@ -46085,7 +46019,7 @@
         <v>7194</v>
       </c>
     </row>
-    <row r="1233" spans="1:3" s="47" customFormat="1" ht="173.25">
+    <row r="1233" spans="1:3" s="47" customFormat="1" ht="165">
       <c r="A1233" s="10" t="s">
         <v>5455</v>
       </c>
@@ -50353,184 +50287,52 @@
       </c>
     </row>
     <row r="1624" spans="1:3">
-      <c r="A1624" s="57"/>
-      <c r="B1624" s="57"/>
+      <c r="A1624" s="57" t="s">
+        <v>9327</v>
+      </c>
+      <c r="B1624" s="57" t="s">
+        <v>8290</v>
+      </c>
       <c r="C1624" s="57"/>
+    </row>
+    <row r="1625" spans="1:3">
+      <c r="A1625" t="s">
+        <v>9329</v>
+      </c>
+      <c r="B1625" t="s">
+        <v>9328</v>
+      </c>
     </row>
     <row r="1626" spans="1:3">
       <c r="A1626" t="s">
-        <v>9327</v>
+        <v>9330</v>
       </c>
       <c r="B1626" t="s">
-        <v>9328</v>
+        <v>8298</v>
       </c>
     </row>
     <row r="1627" spans="1:3">
       <c r="A1627" t="s">
-        <v>9329</v>
+        <v>9331</v>
       </c>
       <c r="B1627" t="s">
-        <v>298</v>
+        <v>9332</v>
       </c>
     </row>
     <row r="1628" spans="1:3">
       <c r="A1628" t="s">
-        <v>9330</v>
+        <v>9333</v>
       </c>
       <c r="B1628" t="s">
-        <v>9331</v>
+        <v>9334</v>
       </c>
     </row>
     <row r="1629" spans="1:3">
       <c r="A1629" t="s">
-        <v>9332</v>
+        <v>9335</v>
       </c>
       <c r="B1629" t="s">
-        <v>9333</v>
-      </c>
-    </row>
-    <row r="1630" spans="1:3">
-      <c r="A1630" t="s">
-        <v>9334</v>
-      </c>
-      <c r="B1630" t="s">
-        <v>9335</v>
-      </c>
-    </row>
-    <row r="1632" spans="1:3">
-      <c r="A1632" t="s">
-        <v>9336</v>
-      </c>
-      <c r="B1632" t="s">
-        <v>9337</v>
-      </c>
-    </row>
-    <row r="1633" spans="1:2">
-      <c r="A1633" t="s">
-        <v>9338</v>
-      </c>
-      <c r="B1633" t="s">
-        <v>9337</v>
-      </c>
-    </row>
-    <row r="1634" spans="1:2">
-      <c r="A1634" t="s">
-        <v>9339</v>
-      </c>
-      <c r="B1634" t="s">
-        <v>9337</v>
-      </c>
-    </row>
-    <row r="1635" spans="1:2">
-      <c r="A1635" t="s">
-        <v>9340</v>
-      </c>
-      <c r="B1635" t="s">
-        <v>9337</v>
-      </c>
-    </row>
-    <row r="1636" spans="1:2">
-      <c r="A1636" t="s">
-        <v>9341</v>
-      </c>
-      <c r="B1636" t="s">
-        <v>9337</v>
-      </c>
-    </row>
-    <row r="1637" spans="1:2">
-      <c r="A1637" t="s">
-        <v>9342</v>
-      </c>
-      <c r="B1637" t="s">
-        <v>9337</v>
-      </c>
-    </row>
-    <row r="1638" spans="1:2">
-      <c r="A1638" t="s">
-        <v>9343</v>
-      </c>
-      <c r="B1638" t="s">
-        <v>9337</v>
-      </c>
-    </row>
-    <row r="1639" spans="1:2">
-      <c r="A1639" t="s">
-        <v>9344</v>
-      </c>
-      <c r="B1639" t="s">
-        <v>9337</v>
-      </c>
-    </row>
-    <row r="1641" spans="1:2">
-      <c r="A1641" t="s">
-        <v>9345</v>
-      </c>
-      <c r="B1641" t="s">
-        <v>9346</v>
-      </c>
-    </row>
-    <row r="1642" spans="1:2">
-      <c r="A1642" t="s">
-        <v>9347</v>
-      </c>
-      <c r="B1642" t="s">
-        <v>9348</v>
-      </c>
-    </row>
-    <row r="1643" spans="1:2">
-      <c r="A1643" t="s">
-        <v>9349</v>
-      </c>
-      <c r="B1643" t="s">
-        <v>9348</v>
-      </c>
-    </row>
-    <row r="1644" spans="1:2">
-      <c r="A1644" t="s">
-        <v>9350</v>
-      </c>
-      <c r="B1644" t="s">
-        <v>9348</v>
-      </c>
-    </row>
-    <row r="1645" spans="1:2">
-      <c r="A1645" t="s">
-        <v>9351</v>
-      </c>
-      <c r="B1645" t="s">
-        <v>9348</v>
-      </c>
-    </row>
-    <row r="1646" spans="1:2">
-      <c r="A1646" t="s">
-        <v>9352</v>
-      </c>
-      <c r="B1646" t="s">
-        <v>9348</v>
-      </c>
-    </row>
-    <row r="1647" spans="1:2">
-      <c r="A1647" t="s">
-        <v>9353</v>
-      </c>
-      <c r="B1647" t="s">
-        <v>9348</v>
-      </c>
-    </row>
-    <row r="1648" spans="1:2">
-      <c r="A1648" t="s">
-        <v>9354</v>
-      </c>
-      <c r="B1648" t="s">
-        <v>9348</v>
-      </c>
-    </row>
-    <row r="1650" spans="1:2">
-      <c r="A1650" t="s">
-        <v>6480</v>
-      </c>
-      <c r="B1650" t="s">
-        <v>9355</v>
+        <v>8298</v>
       </c>
     </row>
   </sheetData>
@@ -50538,263 +50340,262 @@
     <sortCondition ref="B2:B1628"/>
   </sortState>
   <conditionalFormatting sqref="C20:C66 C383:C385 C348:C360 C387:C392 C323:C346 C68:C175 C362:C381 C442:C475 C394:C440 C717:C720 C970 C623:C658 C612:C621 C540:C574 C664:C667 C976 C982 C979 C989 C1010:C1013 C1015:C1018 C1020:C1023 C1025:C1028 C1030:C1033 C967 C987 C1006:C1008 C1133 C578:C609 C179:C241 C1261:C1264 C676:C700 C709:C713 C1167:C1255 C477:C538 C252:C321 C3:C12 C1040:C1107">
-    <cfRule type="expression" dxfId="189" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="188" priority="60" stopIfTrue="1">
       <formula>AND($B3 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65:A66 A18:A63 A348:A350 A68:A241 A1074:A1094 A1201:A1255 A1261:A1264 A252:A346 A3:A12 A1099:A1105">
-    <cfRule type="expression" dxfId="188" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="187" priority="61" stopIfTrue="1">
       <formula>AND( $A3 = "", OR( $B3 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C721:C759 C793:C795 C761:C791 C1109:C1127">
-    <cfRule type="expression" dxfId="187" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="186" priority="59" stopIfTrue="1">
       <formula>AND($B721 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C796:C809 C817:C851">
-    <cfRule type="expression" dxfId="186" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="185" priority="58" stopIfTrue="1">
       <formula>AND($B796 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C382">
-    <cfRule type="expression" dxfId="185" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="184" priority="57" stopIfTrue="1">
       <formula>AND($B382 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C716">
-    <cfRule type="expression" dxfId="184" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="183" priority="55" stopIfTrue="1">
       <formula>AND($B716 &lt;&gt; "",#REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A716">
-    <cfRule type="expression" dxfId="183" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="182" priority="56" stopIfTrue="1">
       <formula>AND( $A716 = "", OR( $B716 &lt;&gt; "",#REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C347 C792">
-    <cfRule type="expression" dxfId="182" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="181" priority="53" stopIfTrue="1">
       <formula>AND($B347 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A347 A243:A251 A987 A989 A1151:A1200">
-    <cfRule type="expression" dxfId="181" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="180" priority="54" stopIfTrue="1">
       <formula>AND( $A243 = "", OR( $B243 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C242">
-    <cfRule type="expression" dxfId="180" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="179" priority="51" stopIfTrue="1">
       <formula>AND($B242 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B243:B251">
-    <cfRule type="expression" dxfId="179" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="178" priority="52" stopIfTrue="1">
       <formula>AND($B243 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C968">
-    <cfRule type="expression" dxfId="178" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="177" priority="62" stopIfTrue="1">
       <formula>AND($B967 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C575">
-    <cfRule type="expression" dxfId="177" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="176" priority="63" stopIfTrue="1">
       <formula>AND($C962 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C386 C1005">
-    <cfRule type="expression" dxfId="176" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="175" priority="50" stopIfTrue="1">
       <formula>AND($B386 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C622">
-    <cfRule type="expression" dxfId="175" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="174" priority="64" stopIfTrue="1">
       <formula>AND(#REF! &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C977">
-    <cfRule type="expression" dxfId="174" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="173" priority="65" stopIfTrue="1">
       <formula>AND($B16 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C975">
-    <cfRule type="expression" dxfId="173" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="172" priority="66" stopIfTrue="1">
       <formula>AND($B622 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C971">
-    <cfRule type="expression" dxfId="172" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="171" priority="67" stopIfTrue="1">
       <formula>AND($B67 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="171" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="170" priority="49" stopIfTrue="1">
       <formula>AND($B67 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C972:C973">
-    <cfRule type="expression" dxfId="170" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="169" priority="68" stopIfTrue="1">
       <formula>AND($B13 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C577">
-    <cfRule type="expression" dxfId="169" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="168" priority="69" stopIfTrue="1">
       <formula>AND($C965 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C963">
-    <cfRule type="expression" dxfId="168" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="167" priority="70" stopIfTrue="1">
       <formula>AND($B15 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C980">
-    <cfRule type="expression" dxfId="167" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="166" priority="46" stopIfTrue="1">
       <formula>AND($B979 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C984">
-    <cfRule type="expression" dxfId="166" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="165" priority="47" stopIfTrue="1">
       <formula>AND($B633 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C983">
-    <cfRule type="expression" dxfId="165" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="164" priority="48" stopIfTrue="1">
       <formula>AND($B77 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C974">
-    <cfRule type="expression" dxfId="164" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="163" priority="71" stopIfTrue="1">
       <formula>AND(#REF! &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C988">
-    <cfRule type="expression" dxfId="163" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="162" priority="45" stopIfTrue="1">
       <formula>AND($B639 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C986">
-    <cfRule type="expression" dxfId="162" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="44" stopIfTrue="1">
       <formula>AND($B634 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1106:A1108 A1131">
-    <cfRule type="expression" dxfId="161" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="43" stopIfTrue="1">
       <formula>AND( $A1106 = "", OR( $B1106 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1109:A1126 A1141 A1132 A1134">
-    <cfRule type="expression" dxfId="160" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="41" stopIfTrue="1">
       <formula>AND( $A1109 = "", OR( $B1109 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1 B1147:B1150">
-    <cfRule type="expression" dxfId="159" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="39" stopIfTrue="1">
       <formula>AND($B1 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" dxfId="158" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="40" stopIfTrue="1">
       <formula>AND( $A1 = "", OR( $B1 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C760 C1150">
-    <cfRule type="expression" dxfId="157" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="38" stopIfTrue="1">
       <formula>AND($B760 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1108">
-    <cfRule type="expression" dxfId="156" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="36" stopIfTrue="1">
       <formula>AND($C1108 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C990">
-    <cfRule type="expression" dxfId="155" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="35" stopIfTrue="1">
       <formula>AND($B990 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1132">
-    <cfRule type="expression" dxfId="154" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="34" stopIfTrue="1">
       <formula>AND($B1132 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1146:C1147">
-    <cfRule type="expression" dxfId="153" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="31" stopIfTrue="1">
       <formula>AND($B1146 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1145">
-    <cfRule type="expression" dxfId="152" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="32" stopIfTrue="1">
       <formula>AND($A1144 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1144">
-    <cfRule type="expression" dxfId="151" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="30" stopIfTrue="1">
       <formula>AND($B1144 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1143">
-    <cfRule type="expression" dxfId="150" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="29" stopIfTrue="1">
       <formula>AND($B1143 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1155:B1200">
-    <cfRule type="expression" dxfId="149" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="23" stopIfTrue="1">
       <formula>AND($B1155 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1151:B1154">
-    <cfRule type="expression" dxfId="148" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="22" stopIfTrue="1">
       <formula>AND($B1151 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C576">
-    <cfRule type="expression" dxfId="147" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="21" stopIfTrue="1">
       <formula>AND($C963 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1129:C1130">
-    <cfRule type="expression" dxfId="146" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="42" stopIfTrue="1">
       <formula>AND(#REF! &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1164:C1166">
-    <cfRule type="expression" dxfId="145" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="27" stopIfTrue="1">
       <formula>AND(#REF! &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1163">
-    <cfRule type="expression" dxfId="144" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="28" stopIfTrue="1">
       <formula>AND(#REF! &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1265:C1272">
-    <cfRule type="expression" dxfId="143" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="20" stopIfTrue="1">
       <formula>AND($B1265 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C701:C705">
-    <cfRule type="expression" dxfId="142" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="19" stopIfTrue="1">
       <formula>AND($B701 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C708">
-    <cfRule type="expression" dxfId="141" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="18" stopIfTrue="1">
       <formula>AND($B708 &lt;&gt; "",#REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C668:C672">
-    <cfRule type="expression" dxfId="140" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="17" stopIfTrue="1">
       <formula>AND($B668 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C675">
-    <cfRule type="expression" dxfId="139" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="16" stopIfTrue="1">
       <formula>AND($B675 &lt;&gt; "",#REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="138" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="137" priority="1"/>
+  <conditionalFormatting sqref="A1631:A1048576 A1:A1629">
+    <cfRule type="duplicateValues" dxfId="0" priority="652"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -50802,7 +50603,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="77" stopIfTrue="1" id="{AA618472-CA56-F044-A0E8-2584A93D16EA}">
+          <x14:cfRule type="expression" priority="76" stopIfTrue="1" id="{AA618472-CA56-F044-A0E8-2584A93D16EA}">
             <xm:f>AND('Macintosh HD:Users:tommi:Downloads:[i18n_eetun2.xlsx]schemas'!#REF! &lt;&gt; "", #REF! = "")</xm:f>
             <x14:dxf>
               <font>
@@ -50818,7 +50619,7 @@
           <xm:sqref>C1256:C1257</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="79" stopIfTrue="1" id="{32A07FB6-CEE3-2F4B-8057-FD736BCFC829}">
+          <x14:cfRule type="expression" priority="78" stopIfTrue="1" id="{32A07FB6-CEE3-2F4B-8057-FD736BCFC829}">
             <xm:f>AND('Macintosh HD:Users:tommi:Downloads:[i18n_eetun2.xlsx]schemas'!#REF! &lt;&gt; "", #REF! = "")</xm:f>
             <x14:dxf>
               <font>
@@ -50834,7 +50635,7 @@
           <xm:sqref>C1258:C1260</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="633" stopIfTrue="1" id="{737EF43F-5842-4AB5-98AD-0723CDE44D0D}">
+          <x14:cfRule type="expression" priority="632" stopIfTrue="1" id="{737EF43F-5842-4AB5-98AD-0723CDE44D0D}">
             <xm:f>AND( $A1133 = "", OR( schemas!$A2300 &lt;&gt; "", #REF! &lt;&gt; "" ) )</xm:f>
             <x14:dxf>
               <font>
@@ -50864,14 +50665,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="30.125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15">
       <c r="A1" s="3" t="s">
         <v>1540</v>
       </c>
@@ -54404,17 +54205,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="expression" dxfId="133" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="3" stopIfTrue="1">
       <formula>AND($B2 = "", $C2 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="expression" dxfId="132" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="2" stopIfTrue="1">
       <formula>AND( $C2 = "", $B2 &lt;&gt; "" )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="expression" dxfId="131" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="1" stopIfTrue="1">
       <formula>AND( $A2 = "", OR( $B2 &lt;&gt; "", $C2 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
@@ -54432,15 +54233,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2698"/>
   <sheetViews>
-    <sheetView topLeftCell="A2321" workbookViewId="0">
-      <selection activeCell="A2326" sqref="A2326"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="66.125" customWidth="1"/>
-    <col min="2" max="2" width="68.625" customWidth="1"/>
-    <col min="3" max="3" width="71.375" customWidth="1"/>
+    <col min="1" max="1" width="66.1640625" customWidth="1"/>
+    <col min="2" max="2" width="68.6640625" customWidth="1"/>
+    <col min="3" max="3" width="71.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -56454,7 +56255,7 @@
         <v>8019</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="378">
+    <row r="184" spans="1:3" ht="360">
       <c r="A184" s="2" t="s">
         <v>5146</v>
       </c>
@@ -59761,7 +59562,7 @@
         <v>8241</v>
       </c>
     </row>
-    <row r="485" spans="1:3" ht="252">
+    <row r="485" spans="1:3" ht="240">
       <c r="A485" s="26" t="s">
         <v>7337</v>
       </c>
@@ -77350,7 +77151,7 @@
         <v>1826</v>
       </c>
     </row>
-    <row r="2084" spans="1:3" ht="15.95" customHeight="1">
+    <row r="2084" spans="1:3" ht="16" customHeight="1">
       <c r="A2084" s="2" t="s">
         <v>1831</v>
       </c>
@@ -80912,490 +80713,490 @@
     <sortCondition ref="A2366"/>
   </sortState>
   <conditionalFormatting sqref="B1:B11 B240:B244 B246:B282 B284:B285 B287:B294 B296:B316 B348:B387 B390:B393 B679:B721 B1390:B1392 B1394:B1398 B1137:B1301 B1492:B1507 B1509:B1540 B1544:B1561 B1563:B1571 B1542 B1421:B1490 B1400:B1401 B1403:B1419 B1117:B1135 B832:B988 B1309:B1310 B1318 B1322:B1333 B1303:B1305 B724:B829 B395:B522 B996:B1114 B1648:B1680 B1573:B1634 B1706 B1708:B1710 B1898:B1902 B1914:B1935 B2003:B2004 B1980:B1983 B2012:B2029 B1894 B1886:B1892 B1960:B1962 B1964:B1972 B41:B49 B524:B671 B318:B346 B2140:B2150 B51:B231 B13:B39">
-    <cfRule type="expression" dxfId="130" priority="200" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="200" stopIfTrue="1">
       <formula>AND($B1 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A39 A240:A282 A284:A285 A287:A294 A296:A316 A348:A387 A1394:A1398 A1492:A1507 A1509:A1540 A1421:A1490 A1400:A1419 A679:A988 A390:A522 A1137:A1392 A996:A1135 A1669 A1677:A1678 A1542:A1667 A1671:A1674 A1681:A1706 A1805 A1902 A1898:A1899 A1914:A1935 A1972 A1894 A1886:A1892 A1749:A1754 A1709:A1716 A1756:A1758 A41:A49 A524:A671 A318:A346 A2140:A2150 A51:A231">
-    <cfRule type="expression" dxfId="129" priority="201" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="201" stopIfTrue="1">
       <formula>AND( $A1 = "", OR( $B1 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B238:B239 B234:B235 B245 B388:B389 B394 B1334:B1389 B1136 B1491 B1543 B1562 B1541 B1420 B1115 B2065:B2069 B1717:B1726 B1728:B1736 B1740:B1748">
-    <cfRule type="expression" dxfId="128" priority="198" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="198" stopIfTrue="1">
       <formula>AND($B234 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1670">
-    <cfRule type="expression" dxfId="127" priority="202" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="202" stopIfTrue="1">
       <formula>AND( $A1670 = "", OR( $B1679 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1681:B1705">
-    <cfRule type="expression" dxfId="126" priority="197" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="197" stopIfTrue="1">
       <formula>AND($B1681 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1676">
-    <cfRule type="expression" dxfId="125" priority="203" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="203" stopIfTrue="1">
       <formula>AND( $A1676 = "", OR( $B1681 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1707">
-    <cfRule type="expression" dxfId="124" priority="204" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="204" stopIfTrue="1">
       <formula>AND( $A1707 = "", OR( $B1708 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1756:B1758 B1749:B1754 B1711:B1716">
-    <cfRule type="expression" dxfId="123" priority="195" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="195" stopIfTrue="1">
       <formula>AND($B1711 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1759:B1761">
-    <cfRule type="expression" dxfId="122" priority="191" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="191" stopIfTrue="1">
       <formula>AND($B1759 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1764:A1803 A1759:A1762">
-    <cfRule type="expression" dxfId="121" priority="192" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="192" stopIfTrue="1">
       <formula>AND( $A1759 = "", OR( $B1759 &lt;&gt; "",#REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1759:C1760 C1765:C1766 C1769:C1783">
-    <cfRule type="expression" dxfId="120" priority="190" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="190" stopIfTrue="1">
       <formula>AND($A1759 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1761">
-    <cfRule type="expression" dxfId="119" priority="189" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="189" stopIfTrue="1">
       <formula>AND($A1761 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C562">
-    <cfRule type="expression" dxfId="118" priority="188" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="188" stopIfTrue="1">
       <formula>AND($B562 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C895:C898 C893 C580:C583">
-    <cfRule type="expression" dxfId="117" priority="206" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="206" stopIfTrue="1">
       <formula>AND($C580 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C168 B1762 B1765:B1804">
-    <cfRule type="expression" dxfId="116" priority="187" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="187" stopIfTrue="1">
       <formula>AND($B168 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C578">
-    <cfRule type="expression" dxfId="115" priority="186" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="186" stopIfTrue="1">
       <formula>AND($B578 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C797">
-    <cfRule type="expression" dxfId="114" priority="185" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="185" stopIfTrue="1">
       <formula>AND($B797 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C798 C1806:C1854">
-    <cfRule type="expression" dxfId="113" priority="184" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="184" stopIfTrue="1">
       <formula>AND($B798 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B523">
-    <cfRule type="expression" dxfId="112" priority="182" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="182" stopIfTrue="1">
       <formula>AND($B523 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A232:A239 A286 A388:A389 A523 A1136 A1491 A1541 A1420 A1804 A2587:A2594 A1743:A1745 A2063:A2064 A1880:A1885 A1895:B1897 A1906:A1908 A1936:B1937 A1956 A1946:A1954 A1938:A1942 B2011 A2016 A1988 A1973:A1978 A1980 A2003:A2010 A2042 A2031:A2036 A1893 A2050:A2053 A2055:A2060 A2061:B2062 A2070:A2073 B1955:B1959 A2077:A2081 A1737:A1738 A1723:A1725 A1717:A1721 A1733:A1735 A1727:A1731 A1747:A1748 A2151:A2177">
-    <cfRule type="expression" dxfId="111" priority="183" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="183" stopIfTrue="1">
       <formula>AND( $A232 = "", OR( $B232 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B232:B233 B236:B237 C1543 C1562 C1541 B1402 B1116 B2005:B2010">
-    <cfRule type="expression" dxfId="110" priority="180" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="180" stopIfTrue="1">
       <formula>AND($B232 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1492">
-    <cfRule type="expression" dxfId="109" priority="175" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="175" stopIfTrue="1">
       <formula>AND($A1493 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1493:C1494">
-    <cfRule type="expression" dxfId="108" priority="174" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="174" stopIfTrue="1">
       <formula>AND($A1494 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C518:C527 C529:C540">
-    <cfRule type="expression" dxfId="107" priority="173" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="173" stopIfTrue="1">
       <formula>AND($A519 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C671">
-    <cfRule type="expression" dxfId="106" priority="172" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="172" stopIfTrue="1">
       <formula>AND($A671 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="105" priority="171" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="171" stopIfTrue="1">
       <formula>AND($A6 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="104" priority="170" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="170" stopIfTrue="1">
       <formula>AND($A7 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="103" priority="169" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="169" stopIfTrue="1">
       <formula>AND($A10 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="102" priority="168" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="168" stopIfTrue="1">
       <formula>AND($A9 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="101" priority="167" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="167" stopIfTrue="1">
       <formula>AND($B4 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1764">
-    <cfRule type="expression" dxfId="100" priority="166" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="166" stopIfTrue="1">
       <formula>AND($B1764 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1762">
-    <cfRule type="expression" dxfId="99" priority="164" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="164" stopIfTrue="1">
       <formula>AND($A1762 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1805">
-    <cfRule type="expression" dxfId="98" priority="162" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="162" stopIfTrue="1">
       <formula>AND($B1805 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1880:C1884 C1861:C1877">
-    <cfRule type="expression" dxfId="97" priority="160" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="160" stopIfTrue="1">
       <formula>AND($B1861 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1885">
-    <cfRule type="expression" dxfId="96" priority="159" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="159" stopIfTrue="1">
       <formula>AND($B1885 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1857 C1907:C1909 C1940:C1944 C2064">
-    <cfRule type="expression" dxfId="95" priority="158" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="158" stopIfTrue="1">
       <formula>AND($B1857 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1855:C1856 C1903 C1910">
-    <cfRule type="expression" dxfId="94" priority="157" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="157" stopIfTrue="1">
       <formula>AND($B1855 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1420 C1402 B830:B831 B1312:B1317 B1306 B1319:B1321 B1302 B1949:B1954 B2031:B2060 B2070:B2073 B2156:B2177">
-    <cfRule type="expression" dxfId="93" priority="156" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="156" stopIfTrue="1">
       <formula>AND($B830 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1572 C1906 C1912:C1913 C1939">
-    <cfRule type="expression" dxfId="92" priority="153" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="153" stopIfTrue="1">
       <formula>AND($B1572 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1893 B2587:B2594 B2153:B2155 B1727 B1737:B1739">
-    <cfRule type="expression" dxfId="91" priority="144" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="144" stopIfTrue="1">
       <formula>AND($B1727 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B286">
-    <cfRule type="expression" dxfId="90" priority="142" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="142" stopIfTrue="1">
       <formula>AND($B286 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2595">
-    <cfRule type="expression" dxfId="89" priority="135" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="135" stopIfTrue="1">
       <formula>AND( $A2595 = "", OR( $B2595 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2595">
-    <cfRule type="expression" dxfId="88" priority="134" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="134" stopIfTrue="1">
       <formula>AND($B2595 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2597:C2598">
-    <cfRule type="expression" dxfId="87" priority="133" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="133" stopIfTrue="1">
       <formula>AND($B2597 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2599:A2600">
-    <cfRule type="expression" dxfId="86" priority="132" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="132" stopIfTrue="1">
       <formula>AND( $A2599 = "", OR( $B2599 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2599:C2600">
-    <cfRule type="expression" dxfId="85" priority="131" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="131" stopIfTrue="1">
       <formula>AND($B2599 &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1878:C1879">
-    <cfRule type="expression" dxfId="84" priority="207" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="207" stopIfTrue="1">
       <formula>AND(#REF! &lt;&gt; "", #REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1904">
-    <cfRule type="expression" dxfId="83" priority="154" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="154" stopIfTrue="1">
       <formula>AND(#REF! &lt;&gt; "",#REF! = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1307">
-    <cfRule type="expression" dxfId="82" priority="130" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="130" stopIfTrue="1">
       <formula>AND($B1307 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1308">
-    <cfRule type="expression" dxfId="81" priority="129" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="129" stopIfTrue="1">
       <formula>AND($B1308 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1311">
-    <cfRule type="expression" dxfId="80" priority="128" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="128" stopIfTrue="1">
       <formula>AND($B1311 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2643:B2651">
-    <cfRule type="expression" dxfId="79" priority="104" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="104" stopIfTrue="1">
       <formula>AND($B2643 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2643:A2651">
-    <cfRule type="expression" dxfId="78" priority="105" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="105" stopIfTrue="1">
       <formula>AND( $A2643 = "", OR( $B2643 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2652">
-    <cfRule type="expression" dxfId="77" priority="103" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="103" stopIfTrue="1">
       <formula>AND( $A2652 = "", OR( $B2652 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2652">
-    <cfRule type="expression" dxfId="76" priority="102" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="102" stopIfTrue="1">
       <formula>AND($B2652 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2656:A2657">
-    <cfRule type="expression" dxfId="75" priority="101" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="101" stopIfTrue="1">
       <formula>AND( $A2656 = "", OR( $B2656 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2677:B2698">
-    <cfRule type="expression" dxfId="74" priority="99" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="99" stopIfTrue="1">
       <formula>AND($B2677 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2677:A2698">
-    <cfRule type="expression" dxfId="73" priority="100" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="100" stopIfTrue="1">
       <formula>AND( $A2677 = "", OR( $B2677 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1708">
-    <cfRule type="expression" dxfId="72" priority="644" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="644" stopIfTrue="1">
       <formula>AND( $A1708 = "", OR( #REF! &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="expression" dxfId="71" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="72" stopIfTrue="1">
       <formula>AND($B50 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50">
-    <cfRule type="expression" dxfId="70" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="73" stopIfTrue="1">
       <formula>AND( $A50 = "", OR( $B50 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2178:A2179 A2181:A2185 A2187:A2193 A2246 A2227:A2229 A2231:A2239">
-    <cfRule type="expression" dxfId="69" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="60" stopIfTrue="1">
       <formula>AND( $A2178 = "", OR( $B2178 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2178:B2179">
-    <cfRule type="expression" dxfId="68" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="59" stopIfTrue="1">
       <formula>AND($B2178 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2181:B2185 B2187:B2193 B2239 B2246 B2227:B2229 B2231:B2234">
-    <cfRule type="expression" dxfId="67" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="58" stopIfTrue="1">
       <formula>AND($B2181 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2180">
-    <cfRule type="expression" dxfId="66" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="56" stopIfTrue="1">
       <formula>AND($B2180 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2180">
-    <cfRule type="expression" dxfId="65" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="57" stopIfTrue="1">
       <formula>AND( $A2180 = "", OR( $B2180 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2208:B2226">
-    <cfRule type="expression" dxfId="64" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="52" stopIfTrue="1">
       <formula>AND($B2208 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2194:A2198">
-    <cfRule type="expression" dxfId="63" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="55" stopIfTrue="1">
       <formula>AND( $A2194 = "", OR( $B2194 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2194:B2198">
-    <cfRule type="expression" dxfId="62" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="54" stopIfTrue="1">
       <formula>AND($B2194 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2208:A2226">
-    <cfRule type="expression" dxfId="61" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="53" stopIfTrue="1">
       <formula>AND( $A2208 = "", OR( $B2208 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2200:A2206">
-    <cfRule type="expression" dxfId="60" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="51" stopIfTrue="1">
       <formula>AND( $A2200 = "", OR( $B2200 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2200:B2206">
-    <cfRule type="expression" dxfId="59" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="50" stopIfTrue="1">
       <formula>AND($B2200 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2263">
-    <cfRule type="expression" dxfId="58" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="49" stopIfTrue="1">
       <formula>AND( $A2263 = "", OR( $B2263 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2263">
-    <cfRule type="expression" dxfId="57" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="48" stopIfTrue="1">
       <formula>AND($B2263 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2264:A2274">
-    <cfRule type="expression" dxfId="56" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="47" stopIfTrue="1">
       <formula>AND( $A2264 = "", OR( $B2264 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2264:B2274">
-    <cfRule type="expression" dxfId="55" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="46" stopIfTrue="1">
       <formula>AND($B2264 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2186">
-    <cfRule type="expression" dxfId="54" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="61" stopIfTrue="1">
       <formula>AND($B2186 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2186">
-    <cfRule type="expression" dxfId="53" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="62" stopIfTrue="1">
       <formula>AND( $A2186 = "", OR( $B2186 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2240:A2245">
-    <cfRule type="expression" dxfId="52" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="45" stopIfTrue="1">
       <formula>AND( $A2240 = "", OR( $B2240 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2245">
-    <cfRule type="expression" dxfId="51" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="44" stopIfTrue="1">
       <formula>AND($B2245 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2240">
-    <cfRule type="expression" dxfId="50" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="43" stopIfTrue="1">
       <formula>AND($B2240 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2230">
-    <cfRule type="expression" dxfId="49" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="42" stopIfTrue="1">
       <formula>AND( $A2230 = "", OR( $B2230 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2230">
-    <cfRule type="expression" dxfId="48" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="41" stopIfTrue="1">
       <formula>AND($B2230 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2199">
-    <cfRule type="expression" dxfId="47" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="63" stopIfTrue="1">
       <formula>AND(#REF! = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2199">
-    <cfRule type="expression" dxfId="46" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="64" stopIfTrue="1">
       <formula>AND( #REF! = "", OR( #REF! &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2207">
-    <cfRule type="expression" dxfId="45" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="65" stopIfTrue="1">
       <formula>AND(#REF! = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2207">
-    <cfRule type="expression" dxfId="44" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="66" stopIfTrue="1">
       <formula>AND( #REF! = "", OR( #REF! &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2248:B2256">
-    <cfRule type="expression" dxfId="43" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="67" stopIfTrue="1">
       <formula>AND(#REF! = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2248:A2257">
-    <cfRule type="expression" dxfId="42" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="68" stopIfTrue="1">
       <formula>AND( #REF! = "", OR( #REF! &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2257">
-    <cfRule type="expression" dxfId="41" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="69" stopIfTrue="1">
       <formula>AND(#REF! = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2258:A2262">
-    <cfRule type="expression" dxfId="40" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="70" stopIfTrue="1">
       <formula>AND( #REF! = "", OR( #REF! &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2258:B2262">
-    <cfRule type="expression" dxfId="39" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="71" stopIfTrue="1">
       <formula>AND(#REF! = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C528">
-    <cfRule type="expression" dxfId="38" priority="651" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="651" stopIfTrue="1">
       <formula>AND($A529 = "",#REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2361:A1048576 A1:A2274">
-    <cfRule type="duplicateValues" dxfId="37" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2275:A2300">
-    <cfRule type="duplicateValues" dxfId="36" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2301:A2318">
-    <cfRule type="duplicateValues" dxfId="35" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2361:A1048576 A1:A2318">
-    <cfRule type="duplicateValues" dxfId="34" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2319:A2352">
-    <cfRule type="duplicateValues" dxfId="33" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2353:A2360">
-    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -81723,11 +81524,11 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="68.625" customWidth="1"/>
+    <col min="1" max="1" width="68.6640625" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="38.625" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -82194,7 +81995,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1">
-    <cfRule type="expression" dxfId="11" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="2" stopIfTrue="1">
       <formula>AND($B1 &lt;&gt; "", $C1 = "")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -82216,14 +82017,14 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="100.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="63.125" customWidth="1"/>
+    <col min="1" max="1" width="100.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="63.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15">
       <c r="A1" s="3" t="s">
         <v>1540</v>
       </c>
@@ -82709,12 +82510,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B20:B1048576 B2:B18">
-    <cfRule type="expression" dxfId="10" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="42" stopIfTrue="1">
       <formula>AND($B2 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="expression" dxfId="9" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="45" stopIfTrue="1">
       <formula>AND( $A2 = "", OR( $B2 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
@@ -82736,13 +82537,13 @@
       <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="100.625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="50.625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="100.6640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="50.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15">
       <c r="A1" s="3" t="s">
         <v>1540</v>
       </c>
@@ -82753,217 +82554,217 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75">
+    <row r="2" spans="1:3" ht="15">
       <c r="A2" s="18"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:3" ht="15">
       <c r="A3" s="18"/>
     </row>
-    <row r="4" spans="1:3" ht="15.75">
+    <row r="4" spans="1:3" ht="15">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:3" ht="15">
       <c r="A5" s="9"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:3" ht="15">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:3" ht="15">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:3" ht="15">
       <c r="A8" s="19"/>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:3" ht="15">
       <c r="A9" s="21"/>
     </row>
-    <row r="10" spans="1:3" ht="15.75">
+    <row r="10" spans="1:3" ht="15">
       <c r="A10" s="21"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75">
+    <row r="11" spans="1:3" ht="15">
       <c r="A11" s="21"/>
     </row>
-    <row r="12" spans="1:3" ht="15.75">
+    <row r="12" spans="1:3" ht="15">
       <c r="A12" s="21"/>
     </row>
-    <row r="13" spans="1:3" ht="15.75">
+    <row r="13" spans="1:3" ht="15">
       <c r="A13" s="20"/>
     </row>
-    <row r="14" spans="1:3" ht="15.75">
+    <row r="14" spans="1:3" ht="15">
       <c r="A14" s="21"/>
     </row>
-    <row r="15" spans="1:3" ht="15.75">
+    <row r="15" spans="1:3" ht="15">
       <c r="A15" s="21"/>
     </row>
-    <row r="16" spans="1:3" ht="15.75">
+    <row r="16" spans="1:3" ht="15">
       <c r="A16" s="19"/>
     </row>
-    <row r="17" spans="1:1" ht="15.75">
+    <row r="17" spans="1:1" ht="15">
       <c r="A17" s="19"/>
     </row>
-    <row r="18" spans="1:1" ht="15.75">
+    <row r="18" spans="1:1" ht="15">
       <c r="A18" s="19"/>
     </row>
-    <row r="19" spans="1:1" ht="15.75">
+    <row r="19" spans="1:1" ht="15">
       <c r="A19" s="19"/>
     </row>
-    <row r="20" spans="1:1" ht="15.75">
+    <row r="20" spans="1:1" ht="15">
       <c r="A20" s="19"/>
     </row>
-    <row r="21" spans="1:1" ht="15.75">
+    <row r="21" spans="1:1" ht="15">
       <c r="A21" s="19"/>
     </row>
-    <row r="22" spans="1:1" ht="15.75">
+    <row r="22" spans="1:1" ht="15">
       <c r="A22" s="19"/>
     </row>
-    <row r="23" spans="1:1" ht="15.75">
+    <row r="23" spans="1:1" ht="15">
       <c r="A23" s="19"/>
     </row>
-    <row r="24" spans="1:1" ht="15.75">
+    <row r="24" spans="1:1" ht="15">
       <c r="A24" s="19"/>
     </row>
-    <row r="25" spans="1:1" ht="15.75">
+    <row r="25" spans="1:1" ht="15">
       <c r="A25" s="19"/>
     </row>
-    <row r="26" spans="1:1" ht="15.75">
+    <row r="26" spans="1:1" ht="15">
       <c r="A26" s="19"/>
     </row>
-    <row r="27" spans="1:1" ht="15.75">
+    <row r="27" spans="1:1" ht="15">
       <c r="A27" s="19"/>
     </row>
-    <row r="28" spans="1:1" ht="15.75">
+    <row r="28" spans="1:1" ht="15">
       <c r="A28" s="19"/>
     </row>
-    <row r="29" spans="1:1" ht="15.75">
+    <row r="29" spans="1:1" ht="15">
       <c r="A29" s="19"/>
     </row>
-    <row r="30" spans="1:1" ht="15.75">
+    <row r="30" spans="1:1" ht="15">
       <c r="A30" s="19"/>
     </row>
-    <row r="31" spans="1:1" ht="15.75">
+    <row r="31" spans="1:1" ht="15">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:1" ht="15.75">
+    <row r="32" spans="1:1" ht="15">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:1" ht="15.75">
+    <row r="33" spans="1:1" ht="15">
       <c r="A33" s="18"/>
     </row>
-    <row r="34" spans="1:1" ht="15.75">
+    <row r="34" spans="1:1" ht="15">
       <c r="A34" s="18"/>
     </row>
-    <row r="35" spans="1:1" ht="15.75">
+    <row r="35" spans="1:1" ht="15">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:1" ht="15.75">
+    <row r="36" spans="1:1" ht="15">
       <c r="A36" s="9"/>
     </row>
-    <row r="37" spans="1:1" ht="15.75">
+    <row r="37" spans="1:1" ht="15">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:1" ht="15.75">
+    <row r="38" spans="1:1" ht="15">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:1" ht="15.75">
+    <row r="39" spans="1:1" ht="15">
       <c r="A39" s="19"/>
     </row>
-    <row r="40" spans="1:1" ht="15.75">
+    <row r="40" spans="1:1" ht="15">
       <c r="A40" s="21"/>
     </row>
-    <row r="41" spans="1:1" ht="15.75">
+    <row r="41" spans="1:1" ht="15">
       <c r="A41" s="21"/>
     </row>
-    <row r="42" spans="1:1" ht="15.75">
+    <row r="42" spans="1:1" ht="15">
       <c r="A42" s="21"/>
     </row>
-    <row r="43" spans="1:1" ht="15.75">
+    <row r="43" spans="1:1" ht="15">
       <c r="A43" s="21"/>
     </row>
-    <row r="44" spans="1:1" ht="15.75">
+    <row r="44" spans="1:1" ht="15">
       <c r="A44" s="20"/>
     </row>
-    <row r="45" spans="1:1" ht="15.75">
+    <row r="45" spans="1:1" ht="15">
       <c r="A45" s="21"/>
     </row>
-    <row r="46" spans="1:1" ht="15.75">
+    <row r="46" spans="1:1" ht="15">
       <c r="A46" s="21"/>
     </row>
-    <row r="47" spans="1:1" ht="15.75">
+    <row r="47" spans="1:1" ht="15">
       <c r="A47" s="19"/>
     </row>
-    <row r="48" spans="1:1" ht="15.75">
+    <row r="48" spans="1:1" ht="15">
       <c r="A48" s="19"/>
     </row>
-    <row r="49" spans="1:1" ht="15.75">
+    <row r="49" spans="1:1" ht="15">
       <c r="A49" s="19"/>
     </row>
-    <row r="50" spans="1:1" ht="15.75">
+    <row r="50" spans="1:1" ht="15">
       <c r="A50" s="19"/>
     </row>
-    <row r="51" spans="1:1" ht="15.75">
+    <row r="51" spans="1:1" ht="15">
       <c r="A51" s="19"/>
     </row>
-    <row r="52" spans="1:1" ht="15.75">
+    <row r="52" spans="1:1" ht="15">
       <c r="A52" s="19"/>
     </row>
-    <row r="53" spans="1:1" ht="15.75">
+    <row r="53" spans="1:1" ht="15">
       <c r="A53" s="19"/>
     </row>
-    <row r="54" spans="1:1" ht="15.75">
+    <row r="54" spans="1:1" ht="15">
       <c r="A54" s="19"/>
     </row>
-    <row r="55" spans="1:1" ht="15.75">
+    <row r="55" spans="1:1" ht="15">
       <c r="A55" s="19"/>
     </row>
-    <row r="56" spans="1:1" ht="15.75">
+    <row r="56" spans="1:1" ht="15">
       <c r="A56" s="19"/>
     </row>
-    <row r="57" spans="1:1" ht="15.75">
+    <row r="57" spans="1:1" ht="15">
       <c r="A57" s="19"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B27:B1048576">
-    <cfRule type="expression" dxfId="8" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
       <formula>AND($B27 = "", $C27 &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
       <formula>AND( $C2 = "", $B2 &lt;&gt; "" )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:A1048576">
-    <cfRule type="expression" dxfId="6" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
       <formula>AND( $A58 = "", OR( $B58 &lt;&gt; "", $C58 &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:A32 A44">
-    <cfRule type="expression" dxfId="5" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
       <formula>AND( $A31 = "", OR( $B31 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:A38">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>AND( $A33 = "", OR( $B33 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>AND($B2 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>AND( $A13 = "", OR( $B13 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A7">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>AND( $A2 = "", OR( $B2 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B26">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>AND($B3 = "", #REF! &lt;&gt; "")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -82985,11 +82786,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="96.125" customWidth="1"/>
-    <col min="2" max="2" width="27.625" customWidth="1"/>
-    <col min="3" max="3" width="28.125" customWidth="1"/>
+    <col min="1" max="1" width="96.1640625" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
add missing translations to excel
</commit_message>
<xml_diff>
--- a/resources/i18n.xlsx
+++ b/resources/i18n.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" updateLinks="never" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33800" windowHeight="20320" tabRatio="644"/>
+    <workbookView xWindow="1600" yWindow="4860" windowWidth="33800" windowHeight="20320" tabRatio="644"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13390" uniqueCount="9382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13402" uniqueCount="9391">
   <si>
     <t>fi</t>
   </si>
@@ -28756,6 +28756,33 @@
   </si>
   <si>
     <t>Du kan befullmäktiga företaget som är med i Lupapiste att hantera ansökan för din del. Befullmäktigande av företag är för nuvarande i begränsad pilotbruk.</t>
+  </si>
+  <si>
+    <t>verdict.signatures</t>
+  </si>
+  <si>
+    <t>verdict.signature.description</t>
+  </si>
+  <si>
+    <t>Päätös vaatii hakijan allekirjoituksen</t>
+  </si>
+  <si>
+    <t>verdict.sign</t>
+  </si>
+  <si>
+    <t>verdict.sign-dialog.header</t>
+  </si>
+  <si>
+    <t>Allekirjoita päätös</t>
+  </si>
+  <si>
+    <t>verdict.sign-dialog.contentDescription</t>
+  </si>
+  <si>
+    <t>Päätöksen allekirjoituksen kuvaus</t>
+  </si>
+  <si>
+    <t>verdict.sign-dialog.signButton</t>
   </si>
 </sst>
 </file>
@@ -30391,37 +30418,7 @@
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="187"/>
   </cellStyles>
-  <dxfs count="194">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="191">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -32680,10 +32677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1648"/>
+  <dimension ref="A1:C1656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1600" workbookViewId="0">
-      <selection activeCell="C1642" sqref="C1642"/>
+    <sheetView tabSelected="1" topLeftCell="A1626" workbookViewId="0">
+      <selection activeCell="A1649" sqref="A1649:XFD1656"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -33936,7 +33933,7 @@
         <v>3756</v>
       </c>
     </row>
-    <row r="114" spans="1:3" s="47" customFormat="1">
+    <row r="114" spans="1:3" s="47" customFormat="1" ht="90">
       <c r="A114" s="9" t="s">
         <v>3525</v>
       </c>
@@ -34607,7 +34604,7 @@
         <v>3775</v>
       </c>
     </row>
-    <row r="175" spans="1:3" s="47" customFormat="1" ht="90">
+    <row r="175" spans="1:3" s="47" customFormat="1">
       <c r="A175" s="9" t="s">
         <v>2066</v>
       </c>
@@ -35586,7 +35583,7 @@
         <v>3808</v>
       </c>
     </row>
-    <row r="264" spans="1:3" s="47" customFormat="1">
+    <row r="264" spans="1:3" s="47" customFormat="1" ht="165">
       <c r="A264" s="10" t="s">
         <v>5455</v>
       </c>
@@ -45935,7 +45932,7 @@
         <v>8513</v>
       </c>
     </row>
-    <row r="1205" spans="1:3" s="47" customFormat="1" ht="165">
+    <row r="1205" spans="1:3" s="47" customFormat="1">
       <c r="A1205" s="53" t="s">
         <v>8442</v>
       </c>
@@ -50708,6 +50705,56 @@
       </c>
       <c r="B1648" s="56" t="s">
         <v>9353</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:2" s="56" customFormat="1"/>
+    <row r="1650" spans="1:2" s="56" customFormat="1">
+      <c r="A1650" s="56" t="s">
+        <v>9382</v>
+      </c>
+      <c r="B1650" s="56" t="s">
+        <v>8290</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:2" s="56" customFormat="1">
+      <c r="A1651" s="56" t="s">
+        <v>9383</v>
+      </c>
+      <c r="B1651" s="56" t="s">
+        <v>9384</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:2" s="56" customFormat="1">
+      <c r="A1652" s="56" t="s">
+        <v>9385</v>
+      </c>
+      <c r="B1652" s="56" t="s">
+        <v>8298</v>
+      </c>
+    </row>
+    <row r="1653" spans="1:2" s="56" customFormat="1"/>
+    <row r="1654" spans="1:2" s="56" customFormat="1">
+      <c r="A1654" s="56" t="s">
+        <v>9386</v>
+      </c>
+      <c r="B1654" s="56" t="s">
+        <v>9387</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:2" s="56" customFormat="1">
+      <c r="A1655" s="56" t="s">
+        <v>9388</v>
+      </c>
+      <c r="B1655" s="56" t="s">
+        <v>9389</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:2" s="56" customFormat="1">
+      <c r="A1656" s="56" t="s">
+        <v>9390</v>
+      </c>
+      <c r="B1656" s="56" t="s">
+        <v>8298</v>
       </c>
     </row>
   </sheetData>
@@ -50964,15 +51011,15 @@
     <cfRule type="duplicateValues" dxfId="140" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1593">
-    <cfRule type="expression" dxfId="136" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="3" stopIfTrue="1">
       <formula>AND( $A1593 = "", OR( $B1593 &lt;&gt; "", #REF! &lt;&gt; "" ) )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1593">
-    <cfRule type="duplicateValues" dxfId="135" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="138" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1595:A1623">
-    <cfRule type="duplicateValues" dxfId="134" priority="659"/>
+    <cfRule type="duplicateValues" dxfId="137" priority="659"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>